<commit_message>
Increased size of text on print order list
</commit_message>
<xml_diff>
--- a/Stores IT System v0.xlsx
+++ b/Stores IT System v0.xlsx
@@ -6360,7 +6360,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0000"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -6444,6 +6444,13 @@
     </font>
     <font>
       <sz val="26"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -6862,24 +6869,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -6893,12 +6882,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -6919,12 +6902,6 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -6941,6 +6918,36 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -7199,98 +7206,6 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>127000</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>66675</xdr:colOff>
-      <xdr:row>54</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="2770" name="Main Screen"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="127000" y="127000"/>
-          <a:ext cx="13017500" cy="10160000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:gradFill flip="none" rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:srgbClr val="154E54"/>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:srgbClr val="154E54"/>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="1"/>
-          <a:tileRect/>
-        </a:gradFill>
-        <a:ln w="0" cap="flat" cmpd="sng" algn="ctr">
-          <a:noFill/>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst>
-          <a:outerShdw blurRad="63500" dist="37357" dir="2700000" rotWithShape="0">
-            <a:prstClr val="black">
-              <a:alpha val="40000"/>
-            </a:prstClr>
-          </a:outerShdw>
-        </a:effectLst>
-        <a:extLst>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:prstDash val="solid"/>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="en-GB" sz="1100" b="0">
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:latin typeface=""/>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>26</xdr:col>
@@ -8509,6 +8424,152 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
+      <xdr:colOff>127000</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="Main Screen"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="127000" y="127000"/>
+          <a:ext cx="13017500" cy="10160000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="154E54"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:srgbClr val="154E54"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln w="0" cap="flat" cmpd="sng" algn="ctr">
+          <a:noFill/>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="63500" dist="37357" dir="2700000" rotWithShape="0">
+            <a:prstClr val="black">
+              <a:alpha val="40000"/>
+            </a:prstClr>
+          </a:outerShdw>
+        </a:effectLst>
+        <a:extLst>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-GB" sz="1100" b="0">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:latin typeface=""/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>127000</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="Rectangle 13" hidden="1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="127000" cy="127000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
@@ -8521,7 +8582,7 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2772" name="MenuBar"/>
+        <xdr:cNvPr id="15" name="MenuBar"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -8602,60 +8663,6 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>127000</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="2771" name="Rectangle 2770" hidden="1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="127000" cy="127000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="en-GB" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:from>
@@ -8667,7 +8674,7 @@
     </xdr:to>
     <xdr:sp macro="'ModUIMenu.ProcessBtnPress(1)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2773" name="MenuItem - My Station"/>
+        <xdr:cNvPr id="16" name="MenuItem - My Station"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -8756,7 +8763,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="246" name="Icon - My Station"/>
+        <xdr:cNvPr id="210" name="Icon - My Station"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -8805,7 +8812,7 @@
     </xdr:to>
     <xdr:sp macro="'ModUIMenu.ProcessBtnPress(2)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2774" name="MenuItem - Stores"/>
+        <xdr:cNvPr id="17" name="MenuItem - Stores"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -8894,7 +8901,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="248" name="Icon - Stores"/>
+        <xdr:cNvPr id="212" name="Icon - Stores"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -8943,7 +8950,7 @@
     </xdr:to>
     <xdr:sp macro="'ModUIMenu.ProcessBtnPress(3)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2775" name="MenuItem - Reports"/>
+        <xdr:cNvPr id="18" name="MenuItem - Reports"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -9032,7 +9039,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="250" name="Icon - Reports"/>
+        <xdr:cNvPr id="214" name="Icon - Reports"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -9081,7 +9088,7 @@
     </xdr:to>
     <xdr:sp macro="'ModUIMenu.ProcessBtnPress(4)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2776" name="MenuItem - My Profile"/>
+        <xdr:cNvPr id="19" name="MenuItem - My Profile"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -9170,7 +9177,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="252" name="Icon - My Profile"/>
+        <xdr:cNvPr id="216" name="Icon - My Profile"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -9219,7 +9226,7 @@
     </xdr:to>
     <xdr:sp macro="'ModUIMenu.ProcessBtnPress(5)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2777" name="MenuItem - Support"/>
+        <xdr:cNvPr id="20" name="MenuItem - Support"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -9308,7 +9315,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="254" name="Icon - Support"/>
+        <xdr:cNvPr id="218" name="Icon - Support"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -9362,7 +9369,7 @@
     </xdr:to>
     <xdr:sp macro="'ModUIStoresScreen.ProcessBtnPress(8)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3274" name="BtnUserMangt"/>
+        <xdr:cNvPr id="23" name="BtnUserMangt"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -9457,7 +9464,7 @@
     </xdr:to>
     <xdr:sp macro="'ModUIStoresScreen.ProcessBtnPress(9)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3275" name="BtnOrderSwitch"/>
+        <xdr:cNvPr id="24" name="BtnOrderSwitch"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -9552,7 +9559,7 @@
     </xdr:to>
     <xdr:sp macro="'ModUIStoresScreen.ProcessBtnPress(10)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3276" name="BtnRemoteOrder"/>
+        <xdr:cNvPr id="25" name="BtnRemoteOrder"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -9642,18 +9649,18 @@
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>1085850</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3273" name="Stores Frame 1"/>
+        <xdr:cNvPr id="22" name="Stores Frame 1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2222500" y="254000"/>
-          <a:ext cx="8255000" cy="7874000"/>
+          <a:ext cx="8255000" cy="7620000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9739,7 +9746,7 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3272" name="Stores 1 Header"/>
+        <xdr:cNvPr id="21" name="Stores 1 Header"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -9828,7 +9835,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="817" name="Stores Frame 1 Icon"/>
+        <xdr:cNvPr id="224" name="Stores Frame 1 Icon"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -9871,7 +9878,7 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3277" name="TextBox 3276"/>
+        <xdr:cNvPr id="26" name="TextBox 25"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -9956,7 +9963,7 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3278" name="TextBox 3277"/>
+        <xdr:cNvPr id="27" name="TextBox 26"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -10041,7 +10048,7 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3279" name="TextBox 3278"/>
+        <xdr:cNvPr id="28" name="TextBox 27"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -10126,7 +10133,7 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3280" name="TextBox 3279"/>
+        <xdr:cNvPr id="29" name="TextBox 28"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -10211,7 +10218,7 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3281" name="TextBox 3280"/>
+        <xdr:cNvPr id="30" name="TextBox 29"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -10296,7 +10303,7 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3282" name="TextBox 3281"/>
+        <xdr:cNvPr id="31" name="TextBox 30"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -10381,7 +10388,7 @@
     </xdr:to>
     <xdr:sp macro="'ModUIStoresScreen.OpenOrder(4)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3283" name="TextBox 3282"/>
+        <xdr:cNvPr id="225" name="TextBox 224"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -10466,7 +10473,7 @@
     </xdr:to>
     <xdr:sp macro="'ModUIStoresScreen.OpenOrder(4)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3284" name="TextBox 3283"/>
+        <xdr:cNvPr id="226" name="TextBox 225"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -10551,7 +10558,7 @@
     </xdr:to>
     <xdr:sp macro="'ModUIStoresScreen.OpenOrder(4)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3285" name="TextBox 3284"/>
+        <xdr:cNvPr id="227" name="TextBox 226"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -10636,7 +10643,7 @@
     </xdr:to>
     <xdr:sp macro="'ModUIStoresScreen.OpenOrder(4)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3286" name="TextBox 3285"/>
+        <xdr:cNvPr id="228" name="TextBox 227"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -10721,7 +10728,7 @@
     </xdr:to>
     <xdr:sp macro="'ModUIStoresScreen.OpenOrder(4)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3287" name="TextBox 3286"/>
+        <xdr:cNvPr id="229" name="TextBox 228"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -10803,7 +10810,7 @@
     </xdr:to>
     <xdr:sp macro="'ModUIStoresScreen.OpenOrder(4)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3288" name="TextBox 3287"/>
+        <xdr:cNvPr id="230" name="TextBox 229"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -10888,7 +10895,7 @@
     </xdr:to>
     <xdr:sp macro="'ModUIStoresScreen.OpenOrder(5)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3289" name="TextBox 3288"/>
+        <xdr:cNvPr id="231" name="TextBox 230"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -10973,7 +10980,7 @@
     </xdr:to>
     <xdr:sp macro="'ModUIStoresScreen.OpenOrder(5)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3290" name="TextBox 3289"/>
+        <xdr:cNvPr id="232" name="TextBox 231"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -11058,7 +11065,7 @@
     </xdr:to>
     <xdr:sp macro="'ModUIStoresScreen.OpenOrder(5)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3291" name="TextBox 3290"/>
+        <xdr:cNvPr id="233" name="TextBox 232"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -11143,7 +11150,7 @@
     </xdr:to>
     <xdr:sp macro="'ModUIStoresScreen.OpenOrder(5)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3292" name="TextBox 3291"/>
+        <xdr:cNvPr id="234" name="TextBox 233"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -11228,7 +11235,7 @@
     </xdr:to>
     <xdr:sp macro="'ModUIStoresScreen.OpenOrder(5)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3293" name="TextBox 3292"/>
+        <xdr:cNvPr id="235" name="TextBox 234"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -11310,7 +11317,7 @@
     </xdr:to>
     <xdr:sp macro="'ModUIStoresScreen.OpenOrder(5)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3294" name="TextBox 3293"/>
+        <xdr:cNvPr id="236" name="TextBox 235"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -11395,7 +11402,7 @@
     </xdr:to>
     <xdr:sp macro="'ModUIStoresScreen.OpenOrder(6)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3295" name="TextBox 3294"/>
+        <xdr:cNvPr id="237" name="TextBox 236"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -11480,7 +11487,7 @@
     </xdr:to>
     <xdr:sp macro="'ModUIStoresScreen.OpenOrder(6)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="800" name="TextBox 799"/>
+        <xdr:cNvPr id="238" name="TextBox 237"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -11565,7 +11572,7 @@
     </xdr:to>
     <xdr:sp macro="'ModUIStoresScreen.OpenOrder(6)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="801" name="TextBox 800"/>
+        <xdr:cNvPr id="239" name="TextBox 238"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -11650,7 +11657,7 @@
     </xdr:to>
     <xdr:sp macro="'ModUIStoresScreen.OpenOrder(6)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="802" name="TextBox 801"/>
+        <xdr:cNvPr id="240" name="TextBox 239"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -11735,7 +11742,7 @@
     </xdr:to>
     <xdr:sp macro="'ModUIStoresScreen.OpenOrder(6)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="803" name="TextBox 802"/>
+        <xdr:cNvPr id="241" name="TextBox 240"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -11791,12 +11798,15 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr algn="ctr"/>
-          <a:endParaRPr lang="en-GB" sz="1000" b="0">
-            <a:solidFill>
-              <a:srgbClr val="154E54"/>
-            </a:solidFill>
-            <a:latin typeface="Eras Medium ITC"/>
-          </a:endParaRPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1000" b="0">
+              <a:solidFill>
+                <a:srgbClr val="154E54"/>
+              </a:solidFill>
+              <a:latin typeface="Eras Medium ITC"/>
+            </a:rPr>
+            <a:t>Julian Turner</a:t>
+          </a:r>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -11817,7 +11827,7 @@
     </xdr:to>
     <xdr:sp macro="'ModUIStoresScreen.OpenOrder(6)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="804" name="TextBox 803"/>
+        <xdr:cNvPr id="242" name="TextBox 241"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -11902,7 +11912,7 @@
     </xdr:to>
     <xdr:sp macro="'ModUIStoresScreen.OpenOrder(7)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="805" name="TextBox 804"/>
+        <xdr:cNvPr id="243" name="TextBox 242"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -11987,7 +11997,7 @@
     </xdr:to>
     <xdr:sp macro="'ModUIStoresScreen.OpenOrder(7)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="806" name="TextBox 805"/>
+        <xdr:cNvPr id="244" name="TextBox 243"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -12072,7 +12082,7 @@
     </xdr:to>
     <xdr:sp macro="'ModUIStoresScreen.OpenOrder(7)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="807" name="TextBox 806"/>
+        <xdr:cNvPr id="245" name="TextBox 244"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -12157,7 +12167,7 @@
     </xdr:to>
     <xdr:sp macro="'ModUIStoresScreen.OpenOrder(7)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="812" name="TextBox 811"/>
+        <xdr:cNvPr id="247" name="TextBox 246"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -12242,7 +12252,7 @@
     </xdr:to>
     <xdr:sp macro="'ModUIStoresScreen.OpenOrder(7)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="813" name="TextBox 812"/>
+        <xdr:cNvPr id="249" name="TextBox 248"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -12324,7 +12334,7 @@
     </xdr:to>
     <xdr:sp macro="'ModUIStoresScreen.OpenOrder(7)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="814" name="TextBox 813"/>
+        <xdr:cNvPr id="251" name="TextBox 250"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -12409,7 +12419,7 @@
     </xdr:to>
     <xdr:sp macro="'ModUIStoresScreen.OpenOrder(8)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="815" name="TextBox 814"/>
+        <xdr:cNvPr id="253" name="TextBox 252"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -12494,7 +12504,7 @@
     </xdr:to>
     <xdr:sp macro="'ModUIStoresScreen.OpenOrder(8)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="816" name="TextBox 815"/>
+        <xdr:cNvPr id="255" name="TextBox 254"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -12579,7 +12589,7 @@
     </xdr:to>
     <xdr:sp macro="'ModUIStoresScreen.OpenOrder(8)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="818" name="TextBox 817"/>
+        <xdr:cNvPr id="2752" name="TextBox 2751"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -12664,7 +12674,7 @@
     </xdr:to>
     <xdr:sp macro="'ModUIStoresScreen.OpenOrder(8)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="819" name="TextBox 818"/>
+        <xdr:cNvPr id="2753" name="TextBox 2752"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -12749,7 +12759,7 @@
     </xdr:to>
     <xdr:sp macro="'ModUIStoresScreen.OpenOrder(8)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="820" name="TextBox 819"/>
+        <xdr:cNvPr id="2754" name="TextBox 2753"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -12831,7 +12841,7 @@
     </xdr:to>
     <xdr:sp macro="'ModUIStoresScreen.OpenOrder(8)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="821" name="TextBox 820"/>
+        <xdr:cNvPr id="2755" name="TextBox 2754"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -12916,7 +12926,7 @@
     </xdr:to>
     <xdr:sp macro="'ModUIStoresScreen.OpenOrder(11)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="822" name="TextBox 821"/>
+        <xdr:cNvPr id="2756" name="TextBox 2755"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -13001,7 +13011,7 @@
     </xdr:to>
     <xdr:sp macro="'ModUIStoresScreen.OpenOrder(11)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="823" name="TextBox 822"/>
+        <xdr:cNvPr id="2757" name="TextBox 2756"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -13086,7 +13096,7 @@
     </xdr:to>
     <xdr:sp macro="'ModUIStoresScreen.OpenOrder(11)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="824" name="TextBox 823"/>
+        <xdr:cNvPr id="2758" name="TextBox 2757"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -13171,7 +13181,7 @@
     </xdr:to>
     <xdr:sp macro="'ModUIStoresScreen.OpenOrder(11)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="825" name="TextBox 824"/>
+        <xdr:cNvPr id="2759" name="TextBox 2758"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -13256,7 +13266,7 @@
     </xdr:to>
     <xdr:sp macro="'ModUIStoresScreen.OpenOrder(11)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="826" name="TextBox 825"/>
+        <xdr:cNvPr id="2760" name="TextBox 2759"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -13338,7 +13348,7 @@
     </xdr:to>
     <xdr:sp macro="'ModUIStoresScreen.OpenOrder(11)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="827" name="TextBox 826"/>
+        <xdr:cNvPr id="2761" name="TextBox 2760"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -13423,7 +13433,7 @@
     </xdr:to>
     <xdr:sp macro="'ModUIStoresScreen.OpenOrder(12)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="828" name="TextBox 827"/>
+        <xdr:cNvPr id="2762" name="TextBox 2761"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -13508,7 +13518,7 @@
     </xdr:to>
     <xdr:sp macro="'ModUIStoresScreen.OpenOrder(12)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="829" name="TextBox 828"/>
+        <xdr:cNvPr id="2763" name="TextBox 2762"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -13593,7 +13603,7 @@
     </xdr:to>
     <xdr:sp macro="'ModUIStoresScreen.OpenOrder(12)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="830" name="TextBox 829"/>
+        <xdr:cNvPr id="2764" name="TextBox 2763"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -13678,7 +13688,7 @@
     </xdr:to>
     <xdr:sp macro="'ModUIStoresScreen.OpenOrder(12)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="831" name="TextBox 830"/>
+        <xdr:cNvPr id="2765" name="TextBox 2764"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -13763,7 +13773,7 @@
     </xdr:to>
     <xdr:sp macro="'ModUIStoresScreen.OpenOrder(12)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3296" name="TextBox 3295"/>
+        <xdr:cNvPr id="2766" name="TextBox 2765"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -13845,7 +13855,7 @@
     </xdr:to>
     <xdr:sp macro="'ModUIStoresScreen.OpenOrder(12)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3297" name="TextBox 3296"/>
+        <xdr:cNvPr id="2767" name="TextBox 2766"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -13930,7 +13940,7 @@
     </xdr:to>
     <xdr:sp macro="'ModUIStoresScreen.OpenOrder(15)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3298" name="TextBox 3297"/>
+        <xdr:cNvPr id="2768" name="TextBox 2767"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -14015,7 +14025,7 @@
     </xdr:to>
     <xdr:sp macro="'ModUIStoresScreen.OpenOrder(15)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3299" name="TextBox 3298"/>
+        <xdr:cNvPr id="2769" name="TextBox 2768"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -14100,7 +14110,7 @@
     </xdr:to>
     <xdr:sp macro="'ModUIStoresScreen.OpenOrder(15)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3300" name="TextBox 3299"/>
+        <xdr:cNvPr id="2778" name="TextBox 2777"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -14185,7 +14195,7 @@
     </xdr:to>
     <xdr:sp macro="'ModUIStoresScreen.OpenOrder(15)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3301" name="TextBox 3300"/>
+        <xdr:cNvPr id="2779" name="TextBox 2778"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -14270,7 +14280,7 @@
     </xdr:to>
     <xdr:sp macro="'ModUIStoresScreen.OpenOrder(15)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3302" name="TextBox 3301"/>
+        <xdr:cNvPr id="2780" name="TextBox 2779"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -14352,7 +14362,7 @@
     </xdr:to>
     <xdr:sp macro="'ModUIStoresScreen.OpenOrder(15)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3303" name="TextBox 3302"/>
+        <xdr:cNvPr id="2781" name="TextBox 2780"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -14437,7 +14447,7 @@
     </xdr:to>
     <xdr:sp macro="'ModUIStoresScreen.OpenOrder(16)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3304" name="TextBox 3303"/>
+        <xdr:cNvPr id="2782" name="TextBox 2781"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -14522,7 +14532,7 @@
     </xdr:to>
     <xdr:sp macro="'ModUIStoresScreen.OpenOrder(16)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3305" name="TextBox 3304"/>
+        <xdr:cNvPr id="2783" name="TextBox 2782"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -14607,7 +14617,7 @@
     </xdr:to>
     <xdr:sp macro="'ModUIStoresScreen.OpenOrder(16)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3306" name="TextBox 3305"/>
+        <xdr:cNvPr id="3264" name="TextBox 3263"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -14692,7 +14702,7 @@
     </xdr:to>
     <xdr:sp macro="'ModUIStoresScreen.OpenOrder(16)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3307" name="TextBox 3306"/>
+        <xdr:cNvPr id="3265" name="TextBox 3264"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -14777,7 +14787,7 @@
     </xdr:to>
     <xdr:sp macro="'ModUIStoresScreen.OpenOrder(16)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3308" name="TextBox 3307"/>
+        <xdr:cNvPr id="3266" name="TextBox 3265"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -14859,7 +14869,7 @@
     </xdr:to>
     <xdr:sp macro="'ModUIStoresScreen.OpenOrder(16)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3309" name="TextBox 3308"/>
+        <xdr:cNvPr id="3267" name="TextBox 3266"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -14944,7 +14954,7 @@
     </xdr:to>
     <xdr:sp macro="'ModUIStoresScreen.OpenOrder(18)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3310" name="TextBox 3309"/>
+        <xdr:cNvPr id="3268" name="TextBox 3267"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -15029,7 +15039,7 @@
     </xdr:to>
     <xdr:sp macro="'ModUIStoresScreen.OpenOrder(18)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3311" name="TextBox 3310"/>
+        <xdr:cNvPr id="3269" name="TextBox 3268"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -15114,7 +15124,7 @@
     </xdr:to>
     <xdr:sp macro="'ModUIStoresScreen.OpenOrder(18)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3312" name="TextBox 3311"/>
+        <xdr:cNvPr id="3270" name="TextBox 3269"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -15199,7 +15209,7 @@
     </xdr:to>
     <xdr:sp macro="'ModUIStoresScreen.OpenOrder(18)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3313" name="TextBox 3312"/>
+        <xdr:cNvPr id="3271" name="TextBox 3270"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -15284,7 +15294,7 @@
     </xdr:to>
     <xdr:sp macro="'ModUIStoresScreen.OpenOrder(18)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3314" name="TextBox 3313"/>
+        <xdr:cNvPr id="808" name="TextBox 807"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -15340,12 +15350,15 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr algn="ctr"/>
-          <a:endParaRPr lang="en-GB" sz="1000" b="0">
-            <a:solidFill>
-              <a:srgbClr val="154E54"/>
-            </a:solidFill>
-            <a:latin typeface="Eras Medium ITC"/>
-          </a:endParaRPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1000" b="0">
+              <a:solidFill>
+                <a:srgbClr val="154E54"/>
+              </a:solidFill>
+              <a:latin typeface="Eras Medium ITC"/>
+            </a:rPr>
+            <a:t>Julian Turner</a:t>
+          </a:r>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -15366,7 +15379,7 @@
     </xdr:to>
     <xdr:sp macro="'ModUIStoresScreen.OpenOrder(18)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3315" name="TextBox 3314"/>
+        <xdr:cNvPr id="809" name="TextBox 808"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -15429,7 +15442,7 @@
               </a:solidFill>
               <a:latin typeface="Eras Medium ITC"/>
             </a:rPr>
-            <a:t>Open</a:t>
+            <a:t>Assigned</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -15451,7 +15464,7 @@
     </xdr:to>
     <xdr:sp macro="'ModUIStoresScreen.OpenOrder(19)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3316" name="TextBox 3315"/>
+        <xdr:cNvPr id="810" name="TextBox 809"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -15536,7 +15549,7 @@
     </xdr:to>
     <xdr:sp macro="'ModUIStoresScreen.OpenOrder(19)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3317" name="TextBox 3316"/>
+        <xdr:cNvPr id="811" name="TextBox 810"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -15621,7 +15634,7 @@
     </xdr:to>
     <xdr:sp macro="'ModUIStoresScreen.OpenOrder(19)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3318" name="TextBox 3317"/>
+        <xdr:cNvPr id="192" name="TextBox 191"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -15706,7 +15719,7 @@
     </xdr:to>
     <xdr:sp macro="'ModUIStoresScreen.OpenOrder(19)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3319" name="TextBox 3318"/>
+        <xdr:cNvPr id="193" name="TextBox 192"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -15791,7 +15804,7 @@
     </xdr:to>
     <xdr:sp macro="'ModUIStoresScreen.OpenOrder(19)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3320" name="TextBox 3319"/>
+        <xdr:cNvPr id="194" name="TextBox 193"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -15847,12 +15860,15 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr algn="ctr"/>
-          <a:endParaRPr lang="en-GB" sz="1000" b="0">
-            <a:solidFill>
-              <a:srgbClr val="154E54"/>
-            </a:solidFill>
-            <a:latin typeface="Eras Medium ITC"/>
-          </a:endParaRPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1000" b="0">
+              <a:solidFill>
+                <a:srgbClr val="154E54"/>
+              </a:solidFill>
+              <a:latin typeface="Eras Medium ITC"/>
+            </a:rPr>
+            <a:t>Julian Turner</a:t>
+          </a:r>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -15873,7 +15889,7 @@
     </xdr:to>
     <xdr:sp macro="'ModUIStoresScreen.OpenOrder(19)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3321" name="TextBox 3320"/>
+        <xdr:cNvPr id="195" name="TextBox 194"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -15936,7 +15952,7 @@
               </a:solidFill>
               <a:latin typeface="Eras Medium ITC"/>
             </a:rPr>
-            <a:t>Open</a:t>
+            <a:t>Assigned</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -15958,7 +15974,7 @@
     </xdr:to>
     <xdr:sp macro="'ModUIStoresScreen.OpenOrder(20)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3322" name="TextBox 3321"/>
+        <xdr:cNvPr id="196" name="TextBox 195"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -16043,7 +16059,7 @@
     </xdr:to>
     <xdr:sp macro="'ModUIStoresScreen.OpenOrder(20)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3323" name="TextBox 3322"/>
+        <xdr:cNvPr id="197" name="TextBox 196"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -16128,7 +16144,7 @@
     </xdr:to>
     <xdr:sp macro="'ModUIStoresScreen.OpenOrder(20)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3324" name="TextBox 3323"/>
+        <xdr:cNvPr id="198" name="TextBox 197"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -16213,7 +16229,7 @@
     </xdr:to>
     <xdr:sp macro="'ModUIStoresScreen.OpenOrder(20)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3325" name="TextBox 3324"/>
+        <xdr:cNvPr id="199" name="TextBox 198"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -16298,7 +16314,7 @@
     </xdr:to>
     <xdr:sp macro="'ModUIStoresScreen.OpenOrder(20)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3326" name="TextBox 3325"/>
+        <xdr:cNvPr id="200" name="TextBox 199"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -16354,12 +16370,15 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr algn="ctr"/>
-          <a:endParaRPr lang="en-GB" sz="1000" b="0">
-            <a:solidFill>
-              <a:srgbClr val="154E54"/>
-            </a:solidFill>
-            <a:latin typeface="Eras Medium ITC"/>
-          </a:endParaRPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1000" b="0">
+              <a:solidFill>
+                <a:srgbClr val="154E54"/>
+              </a:solidFill>
+              <a:latin typeface="Eras Medium ITC"/>
+            </a:rPr>
+            <a:t>Julian Turner</a:t>
+          </a:r>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -16380,7 +16399,7 @@
     </xdr:to>
     <xdr:sp macro="'ModUIStoresScreen.OpenOrder(20)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3327" name="TextBox 3326"/>
+        <xdr:cNvPr id="201" name="TextBox 200"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -16443,7 +16462,7 @@
               </a:solidFill>
               <a:latin typeface="Eras Medium ITC"/>
             </a:rPr>
-            <a:t>Open</a:t>
+            <a:t>Assigned</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -16465,7 +16484,7 @@
     </xdr:to>
     <xdr:sp macro="'ModUIStoresScreen.OpenOrder(22)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3328" name="TextBox 3327"/>
+        <xdr:cNvPr id="202" name="TextBox 201"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -16550,7 +16569,7 @@
     </xdr:to>
     <xdr:sp macro="'ModUIStoresScreen.OpenOrder(22)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3329" name="TextBox 3328"/>
+        <xdr:cNvPr id="203" name="TextBox 202"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -16635,7 +16654,7 @@
     </xdr:to>
     <xdr:sp macro="'ModUIStoresScreen.OpenOrder(22)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3330" name="TextBox 3329"/>
+        <xdr:cNvPr id="204" name="TextBox 203"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -16720,7 +16739,7 @@
     </xdr:to>
     <xdr:sp macro="'ModUIStoresScreen.OpenOrder(22)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3331" name="TextBox 3330"/>
+        <xdr:cNvPr id="205" name="TextBox 204"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -16805,7 +16824,7 @@
     </xdr:to>
     <xdr:sp macro="'ModUIStoresScreen.OpenOrder(22)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3332" name="TextBox 3331"/>
+        <xdr:cNvPr id="206" name="TextBox 205"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -16887,7 +16906,7 @@
     </xdr:to>
     <xdr:sp macro="'ModUIStoresScreen.OpenOrder(22)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3333" name="TextBox 3332"/>
+        <xdr:cNvPr id="207" name="TextBox 206"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -16972,7 +16991,7 @@
     </xdr:to>
     <xdr:sp macro="'ModUIStoresScreen.OpenOrder(23)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3334" name="TextBox 3333"/>
+        <xdr:cNvPr id="208" name="TextBox 207"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -17057,7 +17076,7 @@
     </xdr:to>
     <xdr:sp macro="'ModUIStoresScreen.OpenOrder(23)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3335" name="TextBox 3334"/>
+        <xdr:cNvPr id="209" name="TextBox 208"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -17142,7 +17161,7 @@
     </xdr:to>
     <xdr:sp macro="'ModUIStoresScreen.OpenOrder(23)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3336" name="TextBox 3335"/>
+        <xdr:cNvPr id="211" name="TextBox 210"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -17227,7 +17246,7 @@
     </xdr:to>
     <xdr:sp macro="'ModUIStoresScreen.OpenOrder(23)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3337" name="TextBox 3336"/>
+        <xdr:cNvPr id="213" name="TextBox 212"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -17312,7 +17331,7 @@
     </xdr:to>
     <xdr:sp macro="'ModUIStoresScreen.OpenOrder(23)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3338" name="TextBox 3337"/>
+        <xdr:cNvPr id="215" name="TextBox 214"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -17394,7 +17413,7 @@
     </xdr:to>
     <xdr:sp macro="'ModUIStoresScreen.OpenOrder(23)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3339" name="TextBox 3338"/>
+        <xdr:cNvPr id="217" name="TextBox 216"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -17477,9 +17496,9 @@
       <xdr:row>24</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(24)'" textlink="">
+    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(26)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3340" name="TextBox 3339"/>
+        <xdr:cNvPr id="219" name="TextBox 218"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -17542,7 +17561,7 @@
               </a:solidFill>
               <a:latin typeface="Eras Medium ITC"/>
             </a:rPr>
-            <a:t>24</a:t>
+            <a:t>26</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -17562,9 +17581,9 @@
       <xdr:row>24</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(24)'" textlink="">
+    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(26)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3341" name="TextBox 3340"/>
+        <xdr:cNvPr id="220" name="TextBox 219"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -17647,9 +17666,9 @@
       <xdr:row>24</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(24)'" textlink="">
+    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(26)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3342" name="TextBox 3341"/>
+        <xdr:cNvPr id="221" name="TextBox 220"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -17712,7 +17731,7 @@
               </a:solidFill>
               <a:latin typeface="Eras Medium ITC"/>
             </a:rPr>
-            <a:t>Peter Green</a:t>
+            <a:t>Robin Westerdale</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -17732,9 +17751,9 @@
       <xdr:row>24</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(24)'" textlink="">
+    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(26)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3343" name="TextBox 3342"/>
+        <xdr:cNvPr id="222" name="TextBox 221"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -17797,7 +17816,7 @@
               </a:solidFill>
               <a:latin typeface="Eras Medium ITC"/>
             </a:rPr>
-            <a:t>HQ</a:t>
+            <a:t>Bourne</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -17817,9 +17836,9 @@
       <xdr:row>24</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(24)'" textlink="">
+    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(26)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3344" name="TextBox 3343"/>
+        <xdr:cNvPr id="223" name="TextBox 222"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -17899,9 +17918,9 @@
       <xdr:row>24</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(24)'" textlink="">
+    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(26)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3345" name="TextBox 3344"/>
+        <xdr:cNvPr id="3424" name="TextBox 3423"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -17984,9 +18003,9 @@
       <xdr:row>25</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(25)'" textlink="">
+    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(27)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3346" name="TextBox 3345"/>
+        <xdr:cNvPr id="3425" name="TextBox 3424"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -18049,7 +18068,7 @@
               </a:solidFill>
               <a:latin typeface="Eras Medium ITC"/>
             </a:rPr>
-            <a:t>25</a:t>
+            <a:t>27</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -18069,9 +18088,9 @@
       <xdr:row>25</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(25)'" textlink="">
+    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(27)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3347" name="TextBox 3346"/>
+        <xdr:cNvPr id="3426" name="TextBox 3425"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -18134,7 +18153,7 @@
               </a:solidFill>
               <a:latin typeface="Eras Medium ITC"/>
             </a:rPr>
-            <a:t>1</a:t>
+            <a:t>0</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -18154,9 +18173,9 @@
       <xdr:row>25</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(25)'" textlink="">
+    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(27)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3348" name="TextBox 3347"/>
+        <xdr:cNvPr id="3427" name="TextBox 3426"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -18219,7 +18238,7 @@
               </a:solidFill>
               <a:latin typeface="Eras Medium ITC"/>
             </a:rPr>
-            <a:t>Peter Green</a:t>
+            <a:t>Robin Westerdale</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -18239,9 +18258,9 @@
       <xdr:row>25</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(25)'" textlink="">
+    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(27)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3349" name="TextBox 3348"/>
+        <xdr:cNvPr id="3428" name="TextBox 3427"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -18304,7 +18323,7 @@
               </a:solidFill>
               <a:latin typeface="Eras Medium ITC"/>
             </a:rPr>
-            <a:t>HQ</a:t>
+            <a:t>Bourne</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -18324,9 +18343,9 @@
       <xdr:row>25</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(25)'" textlink="">
+    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(27)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3350" name="TextBox 3349"/>
+        <xdr:cNvPr id="3429" name="TextBox 3428"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -18406,9 +18425,9 @@
       <xdr:row>25</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(25)'" textlink="">
+    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(27)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3351" name="TextBox 3350"/>
+        <xdr:cNvPr id="3430" name="TextBox 3429"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -18491,9 +18510,9 @@
       <xdr:row>27</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(26)'" textlink="">
+    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(31)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3352" name="TextBox 3351"/>
+        <xdr:cNvPr id="3431" name="TextBox 3430"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -18556,7 +18575,7 @@
               </a:solidFill>
               <a:latin typeface="Eras Medium ITC"/>
             </a:rPr>
-            <a:t>26</a:t>
+            <a:t>31</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -18576,9 +18595,9 @@
       <xdr:row>27</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(26)'" textlink="">
+    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(31)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3353" name="TextBox 3352"/>
+        <xdr:cNvPr id="3432" name="TextBox 3431"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -18641,7 +18660,7 @@
               </a:solidFill>
               <a:latin typeface="Eras Medium ITC"/>
             </a:rPr>
-            <a:t>0</a:t>
+            <a:t>1</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -18661,9 +18680,9 @@
       <xdr:row>27</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(26)'" textlink="">
+    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(31)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3354" name="TextBox 3353"/>
+        <xdr:cNvPr id="3433" name="TextBox 3432"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -18726,7 +18745,7 @@
               </a:solidFill>
               <a:latin typeface="Eras Medium ITC"/>
             </a:rPr>
-            <a:t>Robin Westerdale</a:t>
+            <a:t>Julian Turner</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -18746,9 +18765,9 @@
       <xdr:row>27</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(26)'" textlink="">
+    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(31)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3355" name="TextBox 3354"/>
+        <xdr:cNvPr id="3434" name="TextBox 3433"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -18811,7 +18830,7 @@
               </a:solidFill>
               <a:latin typeface="Eras Medium ITC"/>
             </a:rPr>
-            <a:t>Bourne</a:t>
+            <a:t>Brant Broughton</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -18831,9 +18850,9 @@
       <xdr:row>27</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(26)'" textlink="">
+    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(31)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3356" name="TextBox 3355"/>
+        <xdr:cNvPr id="3435" name="TextBox 3434"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -18913,9 +18932,9 @@
       <xdr:row>27</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(26)'" textlink="">
+    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(31)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3357" name="TextBox 3356"/>
+        <xdr:cNvPr id="3436" name="TextBox 3435"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -18998,9 +19017,9 @@
       <xdr:row>28</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(27)'" textlink="">
+    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(32)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3358" name="TextBox 3357"/>
+        <xdr:cNvPr id="3437" name="TextBox 3436"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -19063,7 +19082,7 @@
               </a:solidFill>
               <a:latin typeface="Eras Medium ITC"/>
             </a:rPr>
-            <a:t>27</a:t>
+            <a:t>32</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -19083,9 +19102,9 @@
       <xdr:row>28</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(27)'" textlink="">
+    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(32)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3359" name="TextBox 3358"/>
+        <xdr:cNvPr id="3438" name="TextBox 3437"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -19148,7 +19167,7 @@
               </a:solidFill>
               <a:latin typeface="Eras Medium ITC"/>
             </a:rPr>
-            <a:t>0</a:t>
+            <a:t>1</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -19168,9 +19187,9 @@
       <xdr:row>28</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(27)'" textlink="">
+    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(32)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3360" name="TextBox 3359"/>
+        <xdr:cNvPr id="3439" name="TextBox 3438"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -19233,7 +19252,7 @@
               </a:solidFill>
               <a:latin typeface="Eras Medium ITC"/>
             </a:rPr>
-            <a:t>Robin Westerdale</a:t>
+            <a:t>David Byrne</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -19253,9 +19272,9 @@
       <xdr:row>28</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(27)'" textlink="">
+    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(32)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3361" name="TextBox 3360"/>
+        <xdr:cNvPr id="3440" name="TextBox 3439"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -19318,7 +19337,7 @@
               </a:solidFill>
               <a:latin typeface="Eras Medium ITC"/>
             </a:rPr>
-            <a:t>Bourne</a:t>
+            <a:t>Lincoln South</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -19338,9 +19357,9 @@
       <xdr:row>28</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(27)'" textlink="">
+    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(32)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3362" name="TextBox 3361"/>
+        <xdr:cNvPr id="3441" name="TextBox 3440"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -19420,9 +19439,9 @@
       <xdr:row>28</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(27)'" textlink="">
+    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(32)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3363" name="TextBox 3362"/>
+        <xdr:cNvPr id="3442" name="TextBox 3441"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -19485,7 +19504,7 @@
               </a:solidFill>
               <a:latin typeface="Eras Medium ITC"/>
             </a:rPr>
-            <a:t>Open</a:t>
+            <a:t>Issued</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -19505,9 +19524,9 @@
       <xdr:row>29</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(31)'" textlink="">
+    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(33)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3364" name="TextBox 3363"/>
+        <xdr:cNvPr id="3443" name="TextBox 3442"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -19570,7 +19589,7 @@
               </a:solidFill>
               <a:latin typeface="Eras Medium ITC"/>
             </a:rPr>
-            <a:t>31</a:t>
+            <a:t>33</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -19590,9 +19609,9 @@
       <xdr:row>29</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(31)'" textlink="">
+    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(33)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3365" name="TextBox 3364"/>
+        <xdr:cNvPr id="3444" name="TextBox 3443"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -19675,9 +19694,9 @@
       <xdr:row>29</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(31)'" textlink="">
+    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(33)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3366" name="TextBox 3365"/>
+        <xdr:cNvPr id="3445" name="TextBox 3444"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -19760,9 +19779,9 @@
       <xdr:row>29</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(31)'" textlink="">
+    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(33)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3367" name="TextBox 3366"/>
+        <xdr:cNvPr id="3446" name="TextBox 3445"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -19845,9 +19864,9 @@
       <xdr:row>29</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(31)'" textlink="">
+    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(33)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3368" name="TextBox 3367"/>
+        <xdr:cNvPr id="3447" name="TextBox 3446"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -19927,9 +19946,9 @@
       <xdr:row>29</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(31)'" textlink="">
+    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(33)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3369" name="TextBox 3368"/>
+        <xdr:cNvPr id="3448" name="TextBox 3447"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -20012,9 +20031,9 @@
       <xdr:row>31</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(32)'" textlink="">
+    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(34)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3370" name="TextBox 3369"/>
+        <xdr:cNvPr id="3449" name="TextBox 3448"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -20077,7 +20096,7 @@
               </a:solidFill>
               <a:latin typeface="Eras Medium ITC"/>
             </a:rPr>
-            <a:t>32</a:t>
+            <a:t>34</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -20097,9 +20116,9 @@
       <xdr:row>31</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(32)'" textlink="">
+    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(34)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3371" name="TextBox 3370"/>
+        <xdr:cNvPr id="3450" name="TextBox 3449"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -20182,9 +20201,9 @@
       <xdr:row>31</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(32)'" textlink="">
+    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(34)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3372" name="TextBox 3371"/>
+        <xdr:cNvPr id="3451" name="TextBox 3450"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -20247,7 +20266,7 @@
               </a:solidFill>
               <a:latin typeface="Eras Medium ITC"/>
             </a:rPr>
-            <a:t>David Byrne</a:t>
+            <a:t>Julian Turner</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -20267,9 +20286,9 @@
       <xdr:row>31</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(32)'" textlink="">
+    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(34)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3373" name="TextBox 3372"/>
+        <xdr:cNvPr id="3452" name="TextBox 3451"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -20332,7 +20351,7 @@
               </a:solidFill>
               <a:latin typeface="Eras Medium ITC"/>
             </a:rPr>
-            <a:t>Lincoln South</a:t>
+            <a:t>Brant Broughton</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -20352,9 +20371,9 @@
       <xdr:row>31</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(32)'" textlink="">
+    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(34)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3374" name="TextBox 3373"/>
+        <xdr:cNvPr id="3453" name="TextBox 3452"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -20434,9 +20453,9 @@
       <xdr:row>31</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(32)'" textlink="">
+    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(34)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3375" name="TextBox 3374"/>
+        <xdr:cNvPr id="3454" name="TextBox 3453"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -20519,9 +20538,9 @@
       <xdr:row>32</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(33)'" textlink="">
+    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(35)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3376" name="TextBox 3375"/>
+        <xdr:cNvPr id="3455" name="TextBox 3454"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -20584,7 +20603,7 @@
               </a:solidFill>
               <a:latin typeface="Eras Medium ITC"/>
             </a:rPr>
-            <a:t>33</a:t>
+            <a:t>35</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -20604,9 +20623,9 @@
       <xdr:row>32</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(33)'" textlink="">
+    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(35)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3377" name="TextBox 3376"/>
+        <xdr:cNvPr id="3456" name="TextBox 3455"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -20689,9 +20708,9 @@
       <xdr:row>32</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(33)'" textlink="">
+    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(35)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3378" name="TextBox 3377"/>
+        <xdr:cNvPr id="3457" name="TextBox 3456"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -20774,9 +20793,9 @@
       <xdr:row>32</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(33)'" textlink="">
+    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(35)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3379" name="TextBox 3378"/>
+        <xdr:cNvPr id="3458" name="TextBox 3457"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -20859,9 +20878,9 @@
       <xdr:row>32</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(33)'" textlink="">
+    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(35)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3380" name="TextBox 3379"/>
+        <xdr:cNvPr id="3459" name="TextBox 3458"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -20941,9 +20960,9 @@
       <xdr:row>32</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(33)'" textlink="">
+    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(35)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3381" name="TextBox 3380"/>
+        <xdr:cNvPr id="3460" name="TextBox 3459"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -21026,9 +21045,9 @@
       <xdr:row>33</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(34)'" textlink="">
+    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(36)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3382" name="TextBox 3381"/>
+        <xdr:cNvPr id="3461" name="TextBox 3460"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -21091,7 +21110,7 @@
               </a:solidFill>
               <a:latin typeface="Eras Medium ITC"/>
             </a:rPr>
-            <a:t>34</a:t>
+            <a:t>36</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -21111,9 +21130,9 @@
       <xdr:row>33</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(34)'" textlink="">
+    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(36)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3383" name="TextBox 3382"/>
+        <xdr:cNvPr id="3462" name="TextBox 3461"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -21196,9 +21215,9 @@
       <xdr:row>33</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(34)'" textlink="">
+    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(36)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3384" name="TextBox 3383"/>
+        <xdr:cNvPr id="3463" name="TextBox 3462"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -21281,9 +21300,9 @@
       <xdr:row>33</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(34)'" textlink="">
+    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(36)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3385" name="TextBox 3384"/>
+        <xdr:cNvPr id="3464" name="TextBox 3463"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -21366,9 +21385,9 @@
       <xdr:row>33</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(34)'" textlink="">
+    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(36)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3386" name="TextBox 3385"/>
+        <xdr:cNvPr id="3465" name="TextBox 3464"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -21448,9 +21467,9 @@
       <xdr:row>33</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(34)'" textlink="">
+    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(36)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3387" name="TextBox 3386"/>
+        <xdr:cNvPr id="3466" name="TextBox 3465"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -21533,9 +21552,9 @@
       <xdr:row>35</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(35)'" textlink="">
+    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(37)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3388" name="TextBox 3387"/>
+        <xdr:cNvPr id="3467" name="TextBox 3466"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -21598,7 +21617,7 @@
               </a:solidFill>
               <a:latin typeface="Eras Medium ITC"/>
             </a:rPr>
-            <a:t>35</a:t>
+            <a:t>37</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -21618,9 +21637,9 @@
       <xdr:row>35</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(35)'" textlink="">
+    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(37)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3389" name="TextBox 3388"/>
+        <xdr:cNvPr id="3468" name="TextBox 3467"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -21703,9 +21722,9 @@
       <xdr:row>35</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(35)'" textlink="">
+    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(37)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3390" name="TextBox 3389"/>
+        <xdr:cNvPr id="3469" name="TextBox 3468"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -21788,9 +21807,9 @@
       <xdr:row>35</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(35)'" textlink="">
+    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(37)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3391" name="TextBox 3390"/>
+        <xdr:cNvPr id="3470" name="TextBox 3469"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -21873,9 +21892,9 @@
       <xdr:row>35</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(35)'" textlink="">
+    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(37)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3392" name="TextBox 3391"/>
+        <xdr:cNvPr id="3471" name="TextBox 3470"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -21955,9 +21974,9 @@
       <xdr:row>35</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(35)'" textlink="">
+    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(37)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3393" name="TextBox 3392"/>
+        <xdr:cNvPr id="3472" name="TextBox 3471"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -22040,9 +22059,9 @@
       <xdr:row>36</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(36)'" textlink="">
+    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(38)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3394" name="TextBox 3393"/>
+        <xdr:cNvPr id="3473" name="TextBox 3472"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -22105,7 +22124,7 @@
               </a:solidFill>
               <a:latin typeface="Eras Medium ITC"/>
             </a:rPr>
-            <a:t>36</a:t>
+            <a:t>38</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -22125,9 +22144,9 @@
       <xdr:row>36</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(36)'" textlink="">
+    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(38)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3395" name="TextBox 3394"/>
+        <xdr:cNvPr id="3474" name="TextBox 3473"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -22210,9 +22229,9 @@
       <xdr:row>36</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(36)'" textlink="">
+    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(38)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3396" name="TextBox 3395"/>
+        <xdr:cNvPr id="3475" name="TextBox 3474"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -22295,9 +22314,9 @@
       <xdr:row>36</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(36)'" textlink="">
+    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(38)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3397" name="TextBox 3396"/>
+        <xdr:cNvPr id="3476" name="TextBox 3475"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -22380,9 +22399,9 @@
       <xdr:row>36</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(36)'" textlink="">
+    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(38)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3398" name="TextBox 3397"/>
+        <xdr:cNvPr id="3477" name="TextBox 3476"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -22462,9 +22481,9 @@
       <xdr:row>36</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(36)'" textlink="">
+    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(38)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3399" name="TextBox 3398"/>
+        <xdr:cNvPr id="3478" name="TextBox 3477"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -22547,9 +22566,9 @@
       <xdr:row>37</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(37)'" textlink="">
+    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(39)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3400" name="TextBox 3399"/>
+        <xdr:cNvPr id="3479" name="TextBox 3478"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -22612,7 +22631,7 @@
               </a:solidFill>
               <a:latin typeface="Eras Medium ITC"/>
             </a:rPr>
-            <a:t>37</a:t>
+            <a:t>39</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -22632,9 +22651,9 @@
       <xdr:row>37</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(37)'" textlink="">
+    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(39)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3401" name="TextBox 3400"/>
+        <xdr:cNvPr id="3480" name="TextBox 3479"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -22717,9 +22736,9 @@
       <xdr:row>37</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(37)'" textlink="">
+    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(39)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3402" name="TextBox 3401"/>
+        <xdr:cNvPr id="3481" name="TextBox 3480"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -22802,9 +22821,9 @@
       <xdr:row>37</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(37)'" textlink="">
+    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(39)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3403" name="TextBox 3402"/>
+        <xdr:cNvPr id="3482" name="TextBox 3481"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -22887,9 +22906,9 @@
       <xdr:row>37</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(37)'" textlink="">
+    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(39)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3404" name="TextBox 3403"/>
+        <xdr:cNvPr id="3483" name="TextBox 3482"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -22969,9 +22988,9 @@
       <xdr:row>37</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(37)'" textlink="">
+    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(39)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3405" name="TextBox 3404"/>
+        <xdr:cNvPr id="3484" name="TextBox 3483"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -23054,9 +23073,9 @@
       <xdr:row>39</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(38)'" textlink="">
+    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(41)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3406" name="TextBox 3405"/>
+        <xdr:cNvPr id="3485" name="TextBox 3484"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -23119,7 +23138,7 @@
               </a:solidFill>
               <a:latin typeface="Eras Medium ITC"/>
             </a:rPr>
-            <a:t>38</a:t>
+            <a:t>41</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -23139,9 +23158,9 @@
       <xdr:row>39</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(38)'" textlink="">
+    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(41)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3407" name="TextBox 3406"/>
+        <xdr:cNvPr id="3486" name="TextBox 3485"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -23224,9 +23243,9 @@
       <xdr:row>39</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(38)'" textlink="">
+    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(41)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3408" name="TextBox 3407"/>
+        <xdr:cNvPr id="3487" name="TextBox 3486"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -23289,7 +23308,7 @@
               </a:solidFill>
               <a:latin typeface="Eras Medium ITC"/>
             </a:rPr>
-            <a:t>Julian Turner</a:t>
+            <a:t>Michael Smith</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -23309,9 +23328,9 @@
       <xdr:row>39</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(38)'" textlink="">
+    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(41)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3409" name="TextBox 3408"/>
+        <xdr:cNvPr id="3488" name="TextBox 3487"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -23374,7 +23393,7 @@
               </a:solidFill>
               <a:latin typeface="Eras Medium ITC"/>
             </a:rPr>
-            <a:t>Brant Broughton</a:t>
+            <a:t>Grantham</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -23394,9 +23413,9 @@
       <xdr:row>39</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(38)'" textlink="">
+    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(41)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3410" name="TextBox 3409"/>
+        <xdr:cNvPr id="3489" name="TextBox 3488"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -23476,9 +23495,9 @@
       <xdr:row>39</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(38)'" textlink="">
+    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(41)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3411" name="TextBox 3410"/>
+        <xdr:cNvPr id="3490" name="TextBox 3489"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -23561,9 +23580,9 @@
       <xdr:row>40</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(39)'" textlink="">
+    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(42)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3412" name="TextBox 3411"/>
+        <xdr:cNvPr id="3491" name="TextBox 3490"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -23626,7 +23645,7 @@
               </a:solidFill>
               <a:latin typeface="Eras Medium ITC"/>
             </a:rPr>
-            <a:t>39</a:t>
+            <a:t>42</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -23646,9 +23665,9 @@
       <xdr:row>40</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(39)'" textlink="">
+    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(42)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3413" name="TextBox 3412"/>
+        <xdr:cNvPr id="3492" name="TextBox 3491"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -23731,9 +23750,9 @@
       <xdr:row>40</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(39)'" textlink="">
+    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(42)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3414" name="TextBox 3413"/>
+        <xdr:cNvPr id="3493" name="TextBox 3492"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -23796,7 +23815,7 @@
               </a:solidFill>
               <a:latin typeface="Eras Medium ITC"/>
             </a:rPr>
-            <a:t>Julian Turner</a:t>
+            <a:t>Michael Smith</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -23816,9 +23835,9 @@
       <xdr:row>40</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(39)'" textlink="">
+    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(42)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3415" name="TextBox 3414"/>
+        <xdr:cNvPr id="3494" name="TextBox 3493"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -23881,7 +23900,7 @@
               </a:solidFill>
               <a:latin typeface="Eras Medium ITC"/>
             </a:rPr>
-            <a:t>Brant Broughton</a:t>
+            <a:t>Grantham</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -23901,9 +23920,9 @@
       <xdr:row>40</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(39)'" textlink="">
+    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(42)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3416" name="TextBox 3415"/>
+        <xdr:cNvPr id="3495" name="TextBox 3494"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -23983,521 +24002,14 @@
       <xdr:row>40</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(39)'" textlink="">
+    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(42)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3417" name="TextBox 3416"/>
+        <xdr:cNvPr id="3496" name="TextBox 3495"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="8509000" y="7493000"/>
-          <a:ext cx="1270000" cy="190500"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:gradFill flip="none" rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:srgbClr val="FFFFFF"/>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:srgbClr val="FFFFFF"/>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="1"/>
-          <a:tileRect/>
-        </a:gradFill>
-        <a:ln w="0" cmpd="sng">
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-        <a:extLst>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1000" b="0">
-              <a:solidFill>
-                <a:srgbClr val="154E54"/>
-              </a:solidFill>
-              <a:latin typeface="Eras Medium ITC"/>
-            </a:rPr>
-            <a:t>Open</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>1320800</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>828675</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(41)'" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="3418" name="TextBox 3417"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2540000" y="7747000"/>
-          <a:ext cx="889000" cy="190500"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:gradFill flip="none" rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:srgbClr val="FFFFFF"/>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:srgbClr val="FFFFFF"/>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="1"/>
-          <a:tileRect/>
-        </a:gradFill>
-        <a:ln w="0" cmpd="sng">
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-        <a:extLst>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1000" b="0">
-              <a:solidFill>
-                <a:srgbClr val="154E54"/>
-              </a:solidFill>
-              <a:latin typeface="Eras Medium ITC"/>
-            </a:rPr>
-            <a:t>41</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>828675</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>327025</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(41)'" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="3419" name="TextBox 3418"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3429000" y="7747000"/>
-          <a:ext cx="1270000" cy="190500"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:gradFill flip="none" rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:srgbClr val="FFFFFF"/>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:srgbClr val="FFFFFF"/>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="1"/>
-          <a:tileRect/>
-        </a:gradFill>
-        <a:ln w="0" cmpd="sng">
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-        <a:extLst>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1000" b="0">
-              <a:solidFill>
-                <a:srgbClr val="154E54"/>
-              </a:solidFill>
-              <a:latin typeface="Eras Medium ITC"/>
-            </a:rPr>
-            <a:t>1</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>327025</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>101600</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(41)'" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="3420" name="TextBox 3419"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4699000" y="7747000"/>
-          <a:ext cx="1270000" cy="190500"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:gradFill flip="none" rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:srgbClr val="FFFFFF"/>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:srgbClr val="FFFFFF"/>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="1"/>
-          <a:tileRect/>
-        </a:gradFill>
-        <a:ln w="0" cmpd="sng">
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-        <a:extLst>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1000" b="0">
-              <a:solidFill>
-                <a:srgbClr val="154E54"/>
-              </a:solidFill>
-              <a:latin typeface="Eras Medium ITC"/>
-            </a:rPr>
-            <a:t>Julian Turner</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>101600</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>1371600</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(41)'" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="3421" name="TextBox 3420"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5969000" y="7747000"/>
-          <a:ext cx="1270000" cy="190500"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:gradFill flip="none" rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:srgbClr val="FFFFFF"/>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:srgbClr val="FFFFFF"/>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="1"/>
-          <a:tileRect/>
-        </a:gradFill>
-        <a:ln w="0" cmpd="sng">
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-        <a:extLst>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1000" b="0">
-              <a:solidFill>
-                <a:srgbClr val="154E54"/>
-              </a:solidFill>
-              <a:latin typeface="Eras Medium ITC"/>
-            </a:rPr>
-            <a:t>Brant Broughton</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>1371600</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>412750</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(41)'" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="3422" name="TextBox 3421"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7239000" y="7747000"/>
-          <a:ext cx="1270000" cy="190500"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:gradFill flip="none" rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:srgbClr val="FFFFFF"/>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:srgbClr val="FFFFFF"/>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="1"/>
-          <a:tileRect/>
-        </a:gradFill>
-        <a:ln w="0" cmpd="sng">
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-        <a:extLst>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:endParaRPr lang="en-GB" sz="1000" b="0">
-            <a:solidFill>
-              <a:srgbClr val="154E54"/>
-            </a:solidFill>
-            <a:latin typeface="Eras Medium ITC"/>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>412750</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>387350</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="'ModUIStoresScreen.OpenOrder(41)'" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="3423" name="TextBox 3422"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="8509000" y="7747000"/>
           <a:ext cx="1270000" cy="190500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -33606,46 +33118,46 @@
       <c r="C16" s="3"/>
     </row>
     <row r="23" spans="12:16" x14ac:dyDescent="0.25">
-      <c r="L23" s="57"/>
-      <c r="M23" s="57"/>
-      <c r="N23" s="57"/>
-      <c r="O23" s="57"/>
-      <c r="P23" s="57"/>
+      <c r="L23" s="47"/>
+      <c r="M23" s="47"/>
+      <c r="N23" s="47"/>
+      <c r="O23" s="47"/>
+      <c r="P23" s="47"/>
     </row>
     <row r="24" spans="12:16" x14ac:dyDescent="0.25">
-      <c r="L24" s="57"/>
-      <c r="M24" s="57"/>
-      <c r="N24" s="57"/>
-      <c r="O24" s="57"/>
-      <c r="P24" s="57"/>
+      <c r="L24" s="47"/>
+      <c r="M24" s="47"/>
+      <c r="N24" s="47"/>
+      <c r="O24" s="47"/>
+      <c r="P24" s="47"/>
     </row>
     <row r="25" spans="12:16" x14ac:dyDescent="0.25">
-      <c r="L25" s="57"/>
-      <c r="M25" s="57"/>
-      <c r="N25" s="57"/>
-      <c r="O25" s="57"/>
-      <c r="P25" s="57"/>
+      <c r="L25" s="47"/>
+      <c r="M25" s="47"/>
+      <c r="N25" s="47"/>
+      <c r="O25" s="47"/>
+      <c r="P25" s="47"/>
     </row>
     <row r="26" spans="12:16" x14ac:dyDescent="0.25">
-      <c r="L26" s="57"/>
-      <c r="M26" s="57"/>
-      <c r="N26" s="57"/>
-      <c r="O26" s="57"/>
-      <c r="P26" s="57"/>
+      <c r="L26" s="47"/>
+      <c r="M26" s="47"/>
+      <c r="N26" s="47"/>
+      <c r="O26" s="47"/>
+      <c r="P26" s="47"/>
     </row>
     <row r="27" spans="12:16" x14ac:dyDescent="0.25">
-      <c r="L27" s="57"/>
-      <c r="M27" s="57"/>
-      <c r="N27" s="57"/>
-      <c r="O27" s="57"/>
-      <c r="P27" s="57"/>
+      <c r="L27" s="47"/>
+      <c r="M27" s="47"/>
+      <c r="N27" s="47"/>
+      <c r="O27" s="47"/>
+      <c r="P27" s="47"/>
     </row>
     <row r="28" spans="12:16" x14ac:dyDescent="0.25">
-      <c r="L28" s="57"/>
-      <c r="M28" s="57"/>
-      <c r="N28" s="57"/>
-      <c r="O28" s="57"/>
-      <c r="P28" s="57"/>
+      <c r="L28" s="47"/>
+      <c r="M28" s="47"/>
+      <c r="N28" s="47"/>
+      <c r="O28" s="47"/>
+      <c r="P28" s="47"/>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
@@ -33993,8 +33505,33 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2052" r:id="rId5" name="CommandButton1">
+        <control shapeId="2049" r:id="rId5" name="BtnDBConnect">
           <controlPr defaultSize="0" autoLine="0" r:id="rId6">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>24</xdr:row>
+                <xdr:rowOff>180975</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>26</xdr:row>
+                <xdr:rowOff>76200</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2049" r:id="rId5" name="BtnDBConnect"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2052" r:id="rId7" name="CommandButton1">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId8">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
@@ -34013,32 +33550,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2052" r:id="rId5" name="CommandButton1"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2049" r:id="rId7" name="BtnDBConnect">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId8">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>24</xdr:row>
-                <xdr:rowOff>180975</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>26</xdr:row>
-                <xdr:rowOff>76200</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2049" r:id="rId7" name="BtnDBConnect"/>
+        <control shapeId="2052" r:id="rId7" name="CommandButton1"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -44776,7 +44288,7 @@
   <dimension ref="B1:I39"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="26.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -44787,419 +44299,419 @@
     <col min="4" max="4" width="8.85546875" style="34" customWidth="1"/>
     <col min="5" max="6" width="20.7109375" style="34" customWidth="1"/>
     <col min="7" max="7" width="21.5703125" style="34" customWidth="1"/>
-    <col min="8" max="8" width="44.42578125" style="56" customWidth="1"/>
-    <col min="9" max="9" width="3.42578125" style="48" customWidth="1"/>
+    <col min="8" max="8" width="44.42578125" style="46" customWidth="1"/>
+    <col min="9" max="9" width="3.42578125" style="40" customWidth="1"/>
     <col min="10" max="16384" width="9.140625" style="34"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="58" t="s">
+      <c r="B1" s="48" t="s">
         <v>2063</v>
       </c>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
-      <c r="F1" s="58"/>
-      <c r="G1" s="58"/>
-      <c r="H1" s="58"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="48"/>
     </row>
     <row r="2" spans="2:9" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="2:9" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="42" t="s">
+      <c r="B3" s="36" t="s">
         <v>2057</v>
       </c>
-      <c r="C3" s="35">
+      <c r="C3" s="52">
         <v>6</v>
       </c>
-      <c r="D3" s="59" t="s">
+      <c r="D3" s="49" t="s">
         <v>2078</v>
       </c>
-      <c r="E3" s="61"/>
-      <c r="F3" s="35" t="s">
+      <c r="E3" s="51"/>
+      <c r="F3" s="52" t="s">
         <v>1482</v>
       </c>
-      <c r="G3" s="41" t="s">
+      <c r="G3" s="35" t="s">
         <v>2058</v>
       </c>
-      <c r="H3" s="36" t="s">
+      <c r="H3" s="53" t="s">
         <v>2067</v>
       </c>
-      <c r="I3" s="49"/>
+      <c r="I3" s="41"/>
     </row>
     <row r="4" spans="2:9" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="2:9" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="59" t="s">
+      <c r="B5" s="49" t="s">
         <v>2059</v>
       </c>
-      <c r="C5" s="60"/>
-      <c r="D5" s="43" t="s">
+      <c r="C5" s="50"/>
+      <c r="D5" s="37" t="s">
         <v>2060</v>
       </c>
-      <c r="E5" s="43" t="s">
+      <c r="E5" s="37" t="s">
         <v>2061</v>
       </c>
-      <c r="F5" s="44" t="s">
+      <c r="F5" s="38" t="s">
         <v>2062</v>
       </c>
-      <c r="G5" s="45" t="s">
+      <c r="G5" s="39" t="s">
         <v>2075</v>
       </c>
-      <c r="H5" s="53" t="s">
+      <c r="H5" s="45" t="s">
         <v>2074</v>
       </c>
-      <c r="I5" s="50" t="b">
+      <c r="I5" s="42" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="37" t="s">
+      <c r="B6" s="54" t="s">
         <v>2076</v>
       </c>
-      <c r="C6" s="38"/>
-      <c r="D6" s="46">
+      <c r="C6" s="55"/>
+      <c r="D6" s="56">
         <v>1</v>
       </c>
-      <c r="E6" s="46"/>
-      <c r="F6" s="46"/>
-      <c r="G6" s="54" t="s">
+      <c r="E6" s="56"/>
+      <c r="F6" s="56"/>
+      <c r="G6" s="57" t="s">
         <v>2077</v>
       </c>
-      <c r="H6" s="54" t="s">
+      <c r="H6" s="57" t="s">
         <v>2067</v>
       </c>
-      <c r="I6" s="51" t="b">
+      <c r="I6" s="43" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="39"/>
-      <c r="C7" s="40"/>
-      <c r="D7" s="47"/>
-      <c r="E7" s="47"/>
-      <c r="F7" s="47"/>
-      <c r="G7" s="55"/>
-      <c r="H7" s="55"/>
-      <c r="I7" s="52"/>
+      <c r="B7" s="58"/>
+      <c r="C7" s="59"/>
+      <c r="D7" s="60"/>
+      <c r="E7" s="60"/>
+      <c r="F7" s="60"/>
+      <c r="G7" s="61"/>
+      <c r="H7" s="61"/>
+      <c r="I7" s="44"/>
     </row>
     <row r="8" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="39"/>
-      <c r="C8" s="40"/>
-      <c r="D8" s="47"/>
-      <c r="E8" s="47"/>
-      <c r="F8" s="47"/>
-      <c r="G8" s="55"/>
-      <c r="H8" s="55"/>
-      <c r="I8" s="52"/>
+      <c r="B8" s="58"/>
+      <c r="C8" s="59"/>
+      <c r="D8" s="60"/>
+      <c r="E8" s="60"/>
+      <c r="F8" s="60"/>
+      <c r="G8" s="61"/>
+      <c r="H8" s="61"/>
+      <c r="I8" s="44"/>
     </row>
     <row r="9" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="39"/>
-      <c r="C9" s="40"/>
-      <c r="D9" s="47"/>
-      <c r="E9" s="47"/>
-      <c r="F9" s="47"/>
-      <c r="G9" s="55"/>
-      <c r="H9" s="55"/>
-      <c r="I9" s="52"/>
+      <c r="B9" s="58"/>
+      <c r="C9" s="59"/>
+      <c r="D9" s="60"/>
+      <c r="E9" s="60"/>
+      <c r="F9" s="60"/>
+      <c r="G9" s="61"/>
+      <c r="H9" s="61"/>
+      <c r="I9" s="44"/>
     </row>
     <row r="10" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="39"/>
-      <c r="C10" s="40"/>
-      <c r="D10" s="47"/>
-      <c r="E10" s="47"/>
-      <c r="F10" s="47"/>
-      <c r="G10" s="55"/>
-      <c r="H10" s="55"/>
-      <c r="I10" s="52"/>
+      <c r="B10" s="58"/>
+      <c r="C10" s="59"/>
+      <c r="D10" s="60"/>
+      <c r="E10" s="60"/>
+      <c r="F10" s="60"/>
+      <c r="G10" s="61"/>
+      <c r="H10" s="61"/>
+      <c r="I10" s="44"/>
     </row>
     <row r="11" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="39"/>
-      <c r="C11" s="40"/>
-      <c r="D11" s="47"/>
-      <c r="E11" s="47"/>
-      <c r="F11" s="47"/>
-      <c r="G11" s="55"/>
-      <c r="H11" s="55"/>
-      <c r="I11" s="52"/>
+      <c r="B11" s="58"/>
+      <c r="C11" s="59"/>
+      <c r="D11" s="60"/>
+      <c r="E11" s="60"/>
+      <c r="F11" s="60"/>
+      <c r="G11" s="61"/>
+      <c r="H11" s="61"/>
+      <c r="I11" s="44"/>
     </row>
     <row r="12" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="39"/>
-      <c r="C12" s="40"/>
-      <c r="D12" s="47"/>
-      <c r="E12" s="47"/>
-      <c r="F12" s="47"/>
-      <c r="G12" s="55"/>
-      <c r="H12" s="55"/>
-      <c r="I12" s="52"/>
+      <c r="B12" s="58"/>
+      <c r="C12" s="59"/>
+      <c r="D12" s="60"/>
+      <c r="E12" s="60"/>
+      <c r="F12" s="60"/>
+      <c r="G12" s="61"/>
+      <c r="H12" s="61"/>
+      <c r="I12" s="44"/>
     </row>
     <row r="13" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="39"/>
-      <c r="C13" s="40"/>
-      <c r="D13" s="47"/>
-      <c r="E13" s="47"/>
-      <c r="F13" s="47"/>
-      <c r="G13" s="55"/>
-      <c r="H13" s="55"/>
-      <c r="I13" s="52"/>
+      <c r="B13" s="58"/>
+      <c r="C13" s="59"/>
+      <c r="D13" s="60"/>
+      <c r="E13" s="60"/>
+      <c r="F13" s="60"/>
+      <c r="G13" s="61"/>
+      <c r="H13" s="61"/>
+      <c r="I13" s="44"/>
     </row>
     <row r="14" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="39"/>
-      <c r="C14" s="40"/>
-      <c r="D14" s="47"/>
-      <c r="E14" s="47"/>
-      <c r="F14" s="47"/>
-      <c r="G14" s="55"/>
-      <c r="H14" s="55"/>
-      <c r="I14" s="52"/>
+      <c r="B14" s="58"/>
+      <c r="C14" s="59"/>
+      <c r="D14" s="60"/>
+      <c r="E14" s="60"/>
+      <c r="F14" s="60"/>
+      <c r="G14" s="61"/>
+      <c r="H14" s="61"/>
+      <c r="I14" s="44"/>
     </row>
     <row r="15" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="39"/>
-      <c r="C15" s="40"/>
-      <c r="D15" s="47"/>
-      <c r="E15" s="47"/>
-      <c r="F15" s="47"/>
-      <c r="G15" s="55"/>
-      <c r="H15" s="55"/>
-      <c r="I15" s="52"/>
+      <c r="B15" s="58"/>
+      <c r="C15" s="59"/>
+      <c r="D15" s="60"/>
+      <c r="E15" s="60"/>
+      <c r="F15" s="60"/>
+      <c r="G15" s="61"/>
+      <c r="H15" s="61"/>
+      <c r="I15" s="44"/>
     </row>
     <row r="16" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="39"/>
-      <c r="C16" s="40"/>
-      <c r="D16" s="47"/>
-      <c r="E16" s="47"/>
-      <c r="F16" s="47"/>
-      <c r="G16" s="55"/>
-      <c r="H16" s="55"/>
-      <c r="I16" s="52"/>
+      <c r="B16" s="58"/>
+      <c r="C16" s="59"/>
+      <c r="D16" s="60"/>
+      <c r="E16" s="60"/>
+      <c r="F16" s="60"/>
+      <c r="G16" s="61"/>
+      <c r="H16" s="61"/>
+      <c r="I16" s="44"/>
     </row>
     <row r="17" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="39"/>
-      <c r="C17" s="40"/>
-      <c r="D17" s="47"/>
-      <c r="E17" s="47"/>
-      <c r="F17" s="47"/>
-      <c r="G17" s="55"/>
-      <c r="H17" s="55"/>
-      <c r="I17" s="52"/>
+      <c r="B17" s="58"/>
+      <c r="C17" s="59"/>
+      <c r="D17" s="60"/>
+      <c r="E17" s="60"/>
+      <c r="F17" s="60"/>
+      <c r="G17" s="61"/>
+      <c r="H17" s="61"/>
+      <c r="I17" s="44"/>
     </row>
     <row r="18" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="39"/>
-      <c r="C18" s="40"/>
-      <c r="D18" s="47"/>
-      <c r="E18" s="47"/>
-      <c r="F18" s="47"/>
-      <c r="G18" s="55"/>
-      <c r="H18" s="55"/>
-      <c r="I18" s="52"/>
+      <c r="B18" s="58"/>
+      <c r="C18" s="59"/>
+      <c r="D18" s="60"/>
+      <c r="E18" s="60"/>
+      <c r="F18" s="60"/>
+      <c r="G18" s="61"/>
+      <c r="H18" s="61"/>
+      <c r="I18" s="44"/>
     </row>
     <row r="19" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="39"/>
-      <c r="C19" s="40"/>
-      <c r="D19" s="47"/>
-      <c r="E19" s="47"/>
-      <c r="F19" s="47"/>
-      <c r="G19" s="55"/>
-      <c r="H19" s="55"/>
-      <c r="I19" s="52"/>
+      <c r="B19" s="58"/>
+      <c r="C19" s="59"/>
+      <c r="D19" s="60"/>
+      <c r="E19" s="60"/>
+      <c r="F19" s="60"/>
+      <c r="G19" s="61"/>
+      <c r="H19" s="61"/>
+      <c r="I19" s="44"/>
     </row>
     <row r="20" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="39"/>
-      <c r="C20" s="40"/>
-      <c r="D20" s="47"/>
-      <c r="E20" s="47"/>
-      <c r="F20" s="47"/>
-      <c r="G20" s="55"/>
-      <c r="H20" s="55"/>
-      <c r="I20" s="52"/>
+      <c r="B20" s="58"/>
+      <c r="C20" s="59"/>
+      <c r="D20" s="60"/>
+      <c r="E20" s="60"/>
+      <c r="F20" s="60"/>
+      <c r="G20" s="61"/>
+      <c r="H20" s="61"/>
+      <c r="I20" s="44"/>
     </row>
     <row r="21" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="39"/>
-      <c r="C21" s="40"/>
-      <c r="D21" s="47"/>
-      <c r="E21" s="47"/>
-      <c r="F21" s="47"/>
-      <c r="G21" s="55"/>
-      <c r="H21" s="55"/>
-      <c r="I21" s="52"/>
+      <c r="B21" s="58"/>
+      <c r="C21" s="59"/>
+      <c r="D21" s="60"/>
+      <c r="E21" s="60"/>
+      <c r="F21" s="60"/>
+      <c r="G21" s="61"/>
+      <c r="H21" s="61"/>
+      <c r="I21" s="44"/>
     </row>
     <row r="22" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="39"/>
-      <c r="C22" s="40"/>
-      <c r="D22" s="47"/>
-      <c r="E22" s="47"/>
-      <c r="F22" s="47"/>
-      <c r="G22" s="55"/>
-      <c r="H22" s="55"/>
-      <c r="I22" s="52"/>
+      <c r="B22" s="58"/>
+      <c r="C22" s="59"/>
+      <c r="D22" s="60"/>
+      <c r="E22" s="60"/>
+      <c r="F22" s="60"/>
+      <c r="G22" s="61"/>
+      <c r="H22" s="61"/>
+      <c r="I22" s="44"/>
     </row>
     <row r="23" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="39"/>
-      <c r="C23" s="40"/>
-      <c r="D23" s="47"/>
-      <c r="E23" s="47"/>
-      <c r="F23" s="47"/>
-      <c r="G23" s="55"/>
-      <c r="H23" s="55"/>
-      <c r="I23" s="52"/>
+      <c r="B23" s="58"/>
+      <c r="C23" s="59"/>
+      <c r="D23" s="60"/>
+      <c r="E23" s="60"/>
+      <c r="F23" s="60"/>
+      <c r="G23" s="61"/>
+      <c r="H23" s="61"/>
+      <c r="I23" s="44"/>
     </row>
     <row r="24" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="39"/>
-      <c r="C24" s="40"/>
-      <c r="D24" s="47"/>
-      <c r="E24" s="47"/>
-      <c r="F24" s="47"/>
-      <c r="G24" s="55"/>
-      <c r="H24" s="55"/>
-      <c r="I24" s="52"/>
+      <c r="B24" s="58"/>
+      <c r="C24" s="59"/>
+      <c r="D24" s="60"/>
+      <c r="E24" s="60"/>
+      <c r="F24" s="60"/>
+      <c r="G24" s="61"/>
+      <c r="H24" s="61"/>
+      <c r="I24" s="44"/>
     </row>
     <row r="25" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="39"/>
-      <c r="C25" s="40"/>
-      <c r="D25" s="47"/>
-      <c r="E25" s="47"/>
-      <c r="F25" s="47"/>
-      <c r="G25" s="55"/>
-      <c r="H25" s="55"/>
-      <c r="I25" s="52"/>
+      <c r="B25" s="58"/>
+      <c r="C25" s="59"/>
+      <c r="D25" s="60"/>
+      <c r="E25" s="60"/>
+      <c r="F25" s="60"/>
+      <c r="G25" s="61"/>
+      <c r="H25" s="61"/>
+      <c r="I25" s="44"/>
     </row>
     <row r="26" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="39"/>
-      <c r="C26" s="40"/>
-      <c r="D26" s="47"/>
-      <c r="E26" s="47"/>
-      <c r="F26" s="47"/>
-      <c r="G26" s="55"/>
-      <c r="H26" s="55"/>
-      <c r="I26" s="52"/>
+      <c r="B26" s="58"/>
+      <c r="C26" s="59"/>
+      <c r="D26" s="60"/>
+      <c r="E26" s="60"/>
+      <c r="F26" s="60"/>
+      <c r="G26" s="61"/>
+      <c r="H26" s="61"/>
+      <c r="I26" s="44"/>
     </row>
     <row r="27" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="39"/>
-      <c r="C27" s="40"/>
-      <c r="D27" s="47"/>
-      <c r="E27" s="47"/>
-      <c r="F27" s="47"/>
-      <c r="G27" s="55"/>
-      <c r="H27" s="55"/>
-      <c r="I27" s="52"/>
+      <c r="B27" s="58"/>
+      <c r="C27" s="59"/>
+      <c r="D27" s="60"/>
+      <c r="E27" s="60"/>
+      <c r="F27" s="60"/>
+      <c r="G27" s="61"/>
+      <c r="H27" s="61"/>
+      <c r="I27" s="44"/>
     </row>
     <row r="28" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="39"/>
-      <c r="C28" s="40"/>
-      <c r="D28" s="47"/>
-      <c r="E28" s="47"/>
-      <c r="F28" s="47"/>
-      <c r="G28" s="55"/>
-      <c r="H28" s="55"/>
-      <c r="I28" s="52"/>
+      <c r="B28" s="58"/>
+      <c r="C28" s="59"/>
+      <c r="D28" s="60"/>
+      <c r="E28" s="60"/>
+      <c r="F28" s="60"/>
+      <c r="G28" s="61"/>
+      <c r="H28" s="61"/>
+      <c r="I28" s="44"/>
     </row>
     <row r="29" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="39"/>
-      <c r="C29" s="40"/>
-      <c r="D29" s="47"/>
-      <c r="E29" s="47"/>
-      <c r="F29" s="47"/>
-      <c r="G29" s="55"/>
-      <c r="H29" s="55"/>
-      <c r="I29" s="52"/>
+      <c r="B29" s="58"/>
+      <c r="C29" s="59"/>
+      <c r="D29" s="60"/>
+      <c r="E29" s="60"/>
+      <c r="F29" s="60"/>
+      <c r="G29" s="61"/>
+      <c r="H29" s="61"/>
+      <c r="I29" s="44"/>
     </row>
     <row r="30" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="39"/>
-      <c r="C30" s="40"/>
-      <c r="D30" s="47"/>
-      <c r="E30" s="47"/>
-      <c r="F30" s="47"/>
-      <c r="G30" s="55"/>
-      <c r="H30" s="55"/>
-      <c r="I30" s="52"/>
+      <c r="B30" s="58"/>
+      <c r="C30" s="59"/>
+      <c r="D30" s="60"/>
+      <c r="E30" s="60"/>
+      <c r="F30" s="60"/>
+      <c r="G30" s="61"/>
+      <c r="H30" s="61"/>
+      <c r="I30" s="44"/>
     </row>
     <row r="31" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="39"/>
-      <c r="C31" s="40"/>
-      <c r="D31" s="47"/>
-      <c r="E31" s="47"/>
-      <c r="F31" s="47"/>
-      <c r="G31" s="55"/>
-      <c r="H31" s="55"/>
-      <c r="I31" s="52"/>
+      <c r="B31" s="58"/>
+      <c r="C31" s="59"/>
+      <c r="D31" s="60"/>
+      <c r="E31" s="60"/>
+      <c r="F31" s="60"/>
+      <c r="G31" s="61"/>
+      <c r="H31" s="61"/>
+      <c r="I31" s="44"/>
     </row>
     <row r="32" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="39"/>
-      <c r="C32" s="40"/>
-      <c r="D32" s="47"/>
-      <c r="E32" s="47"/>
-      <c r="F32" s="47"/>
-      <c r="G32" s="55"/>
-      <c r="H32" s="55"/>
-      <c r="I32" s="52"/>
+      <c r="B32" s="58"/>
+      <c r="C32" s="59"/>
+      <c r="D32" s="60"/>
+      <c r="E32" s="60"/>
+      <c r="F32" s="60"/>
+      <c r="G32" s="61"/>
+      <c r="H32" s="61"/>
+      <c r="I32" s="44"/>
     </row>
     <row r="33" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="39"/>
-      <c r="C33" s="40"/>
-      <c r="D33" s="47"/>
-      <c r="E33" s="47"/>
-      <c r="F33" s="47"/>
-      <c r="G33" s="55"/>
-      <c r="H33" s="55"/>
-      <c r="I33" s="52"/>
+      <c r="B33" s="58"/>
+      <c r="C33" s="59"/>
+      <c r="D33" s="60"/>
+      <c r="E33" s="60"/>
+      <c r="F33" s="60"/>
+      <c r="G33" s="61"/>
+      <c r="H33" s="61"/>
+      <c r="I33" s="44"/>
     </row>
     <row r="34" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="39"/>
-      <c r="C34" s="40"/>
-      <c r="D34" s="47"/>
-      <c r="E34" s="47"/>
-      <c r="F34" s="47"/>
-      <c r="G34" s="55"/>
-      <c r="H34" s="55"/>
-      <c r="I34" s="52"/>
+      <c r="B34" s="58"/>
+      <c r="C34" s="59"/>
+      <c r="D34" s="60"/>
+      <c r="E34" s="60"/>
+      <c r="F34" s="60"/>
+      <c r="G34" s="61"/>
+      <c r="H34" s="61"/>
+      <c r="I34" s="44"/>
     </row>
     <row r="35" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="39"/>
-      <c r="C35" s="40"/>
-      <c r="D35" s="47"/>
-      <c r="E35" s="47"/>
-      <c r="F35" s="47"/>
-      <c r="G35" s="55"/>
-      <c r="H35" s="55"/>
-      <c r="I35" s="52"/>
+      <c r="B35" s="58"/>
+      <c r="C35" s="59"/>
+      <c r="D35" s="60"/>
+      <c r="E35" s="60"/>
+      <c r="F35" s="60"/>
+      <c r="G35" s="61"/>
+      <c r="H35" s="61"/>
+      <c r="I35" s="44"/>
     </row>
     <row r="36" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="39"/>
-      <c r="C36" s="40"/>
-      <c r="D36" s="47"/>
-      <c r="E36" s="47"/>
-      <c r="F36" s="47"/>
-      <c r="G36" s="55"/>
-      <c r="H36" s="55"/>
-      <c r="I36" s="52"/>
+      <c r="B36" s="58"/>
+      <c r="C36" s="59"/>
+      <c r="D36" s="60"/>
+      <c r="E36" s="60"/>
+      <c r="F36" s="60"/>
+      <c r="G36" s="61"/>
+      <c r="H36" s="61"/>
+      <c r="I36" s="44"/>
     </row>
     <row r="37" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="39"/>
-      <c r="C37" s="40"/>
-      <c r="D37" s="47"/>
-      <c r="E37" s="47"/>
-      <c r="F37" s="47"/>
-      <c r="G37" s="55"/>
-      <c r="H37" s="55"/>
-      <c r="I37" s="52"/>
+      <c r="B37" s="58"/>
+      <c r="C37" s="59"/>
+      <c r="D37" s="60"/>
+      <c r="E37" s="60"/>
+      <c r="F37" s="60"/>
+      <c r="G37" s="61"/>
+      <c r="H37" s="61"/>
+      <c r="I37" s="44"/>
     </row>
     <row r="38" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="39"/>
-      <c r="C38" s="40"/>
-      <c r="D38" s="47"/>
-      <c r="E38" s="47"/>
-      <c r="F38" s="47"/>
-      <c r="G38" s="55"/>
-      <c r="H38" s="55"/>
-      <c r="I38" s="52"/>
+      <c r="B38" s="58"/>
+      <c r="C38" s="59"/>
+      <c r="D38" s="60"/>
+      <c r="E38" s="60"/>
+      <c r="F38" s="60"/>
+      <c r="G38" s="61"/>
+      <c r="H38" s="61"/>
+      <c r="I38" s="44"/>
     </row>
     <row r="39" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="39"/>
-      <c r="C39" s="40"/>
-      <c r="D39" s="47"/>
-      <c r="E39" s="47"/>
-      <c r="F39" s="47"/>
-      <c r="G39" s="55"/>
-      <c r="H39" s="55"/>
-      <c r="I39" s="52"/>
+      <c r="B39" s="58"/>
+      <c r="C39" s="59"/>
+      <c r="D39" s="60"/>
+      <c r="E39" s="60"/>
+      <c r="F39" s="60"/>
+      <c r="G39" s="61"/>
+      <c r="H39" s="61"/>
+      <c r="I39" s="44"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -45382,8 +44894,8 @@
       <formula>#REF!=TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="53" fitToHeight="0" orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
+  <pageSetup paperSize="9" scale="56" fitToHeight="0" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
   <legacyDrawing r:id="rId3"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">

</xml_diff>

<commit_message>
Increased text size of Order Form
</commit_message>
<xml_diff>
--- a/Stores IT System v0.xlsx
+++ b/Stores IT System v0.xlsx
@@ -6421,14 +6421,14 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="12"/>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
+      <sz val="14"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -6436,14 +6436,14 @@
     </font>
     <font>
       <b/>
-      <sz val="12"/>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="26"/>
+      <sz val="36"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -6806,7 +6806,7 @@
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -6859,31 +6859,40 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -6895,52 +6904,40 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -25661,46 +25658,46 @@
       <c r="C16" s="3"/>
     </row>
     <row r="23" spans="12:16" x14ac:dyDescent="0.25">
-      <c r="L23" s="57"/>
-      <c r="M23" s="57"/>
-      <c r="N23" s="57"/>
-      <c r="O23" s="57"/>
-      <c r="P23" s="57"/>
+      <c r="L23" s="34"/>
+      <c r="M23" s="34"/>
+      <c r="N23" s="34"/>
+      <c r="O23" s="34"/>
+      <c r="P23" s="34"/>
     </row>
     <row r="24" spans="12:16" x14ac:dyDescent="0.25">
-      <c r="L24" s="57"/>
-      <c r="M24" s="57"/>
-      <c r="N24" s="57"/>
-      <c r="O24" s="57"/>
-      <c r="P24" s="57"/>
+      <c r="L24" s="34"/>
+      <c r="M24" s="34"/>
+      <c r="N24" s="34"/>
+      <c r="O24" s="34"/>
+      <c r="P24" s="34"/>
     </row>
     <row r="25" spans="12:16" x14ac:dyDescent="0.25">
-      <c r="L25" s="57"/>
-      <c r="M25" s="57"/>
-      <c r="N25" s="57"/>
-      <c r="O25" s="57"/>
-      <c r="P25" s="57"/>
+      <c r="L25" s="34"/>
+      <c r="M25" s="34"/>
+      <c r="N25" s="34"/>
+      <c r="O25" s="34"/>
+      <c r="P25" s="34"/>
     </row>
     <row r="26" spans="12:16" x14ac:dyDescent="0.25">
-      <c r="L26" s="57"/>
-      <c r="M26" s="57"/>
-      <c r="N26" s="57"/>
-      <c r="O26" s="57"/>
-      <c r="P26" s="57"/>
+      <c r="L26" s="34"/>
+      <c r="M26" s="34"/>
+      <c r="N26" s="34"/>
+      <c r="O26" s="34"/>
+      <c r="P26" s="34"/>
     </row>
     <row r="27" spans="12:16" x14ac:dyDescent="0.25">
-      <c r="L27" s="57"/>
-      <c r="M27" s="57"/>
-      <c r="N27" s="57"/>
-      <c r="O27" s="57"/>
-      <c r="P27" s="57"/>
+      <c r="L27" s="34"/>
+      <c r="M27" s="34"/>
+      <c r="N27" s="34"/>
+      <c r="O27" s="34"/>
+      <c r="P27" s="34"/>
     </row>
     <row r="28" spans="12:16" x14ac:dyDescent="0.25">
-      <c r="L28" s="57"/>
-      <c r="M28" s="57"/>
-      <c r="N28" s="57"/>
-      <c r="O28" s="57"/>
-      <c r="P28" s="57"/>
+      <c r="L28" s="34"/>
+      <c r="M28" s="34"/>
+      <c r="N28" s="34"/>
+      <c r="O28" s="34"/>
+      <c r="P28" s="34"/>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
@@ -26048,8 +26045,33 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2052" r:id="rId5" name="CommandButton1">
+        <control shapeId="2049" r:id="rId5" name="BtnDBConnect">
           <controlPr defaultSize="0" autoLine="0" r:id="rId6">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>24</xdr:row>
+                <xdr:rowOff>180975</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>26</xdr:row>
+                <xdr:rowOff>76200</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2049" r:id="rId5" name="BtnDBConnect"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2052" r:id="rId7" name="CommandButton1">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId8">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
@@ -26068,32 +26090,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2052" r:id="rId5" name="CommandButton1"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2049" r:id="rId7" name="BtnDBConnect">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId8">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>24</xdr:row>
-                <xdr:rowOff>180975</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>26</xdr:row>
-                <xdr:rowOff>76200</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2049" r:id="rId7" name="BtnDBConnect"/>
+        <control shapeId="2052" r:id="rId7" name="CommandButton1"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -36831,430 +36828,430 @@
   <dimension ref="B1:I39"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="26.25" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="34"/>
-    <col min="2" max="2" width="23.85546875" style="34" customWidth="1"/>
-    <col min="3" max="3" width="23" style="34" customWidth="1"/>
-    <col min="4" max="4" width="8.85546875" style="34" customWidth="1"/>
-    <col min="5" max="6" width="20.7109375" style="34" customWidth="1"/>
-    <col min="7" max="7" width="21.5703125" style="34" customWidth="1"/>
-    <col min="8" max="8" width="44.42578125" style="56" customWidth="1"/>
-    <col min="9" max="9" width="3.42578125" style="48" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="34"/>
+    <col min="1" max="1" width="9.140625" style="36"/>
+    <col min="2" max="2" width="23.85546875" style="36" customWidth="1"/>
+    <col min="3" max="3" width="23" style="36" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" style="36" customWidth="1"/>
+    <col min="5" max="6" width="20.7109375" style="36" customWidth="1"/>
+    <col min="7" max="7" width="21.5703125" style="36" customWidth="1"/>
+    <col min="8" max="8" width="44.42578125" style="37" customWidth="1"/>
+    <col min="9" max="9" width="3.42578125" style="35" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="36"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="58" t="s">
+      <c r="B1" s="60" t="s">
         <v>2063</v>
       </c>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
-      <c r="F1" s="58"/>
-      <c r="G1" s="58"/>
-      <c r="H1" s="58"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="60"/>
+      <c r="H1" s="60"/>
     </row>
     <row r="2" spans="2:9" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="2:9" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="42" t="s">
+      <c r="B3" s="38" t="s">
         <v>2057</v>
       </c>
-      <c r="C3" s="35">
+      <c r="C3" s="39">
         <v>6</v>
       </c>
-      <c r="D3" s="59" t="s">
+      <c r="D3" s="40" t="s">
         <v>2078</v>
       </c>
-      <c r="E3" s="61"/>
-      <c r="F3" s="35" t="s">
+      <c r="E3" s="41"/>
+      <c r="F3" s="39" t="s">
         <v>1482</v>
       </c>
-      <c r="G3" s="41" t="s">
+      <c r="G3" s="42" t="s">
         <v>2058</v>
       </c>
-      <c r="H3" s="36" t="s">
+      <c r="H3" s="43" t="s">
         <v>2067</v>
       </c>
-      <c r="I3" s="49"/>
+      <c r="I3" s="44"/>
     </row>
     <row r="4" spans="2:9" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="2:9" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="59" t="s">
+      <c r="B5" s="40" t="s">
         <v>2059</v>
       </c>
-      <c r="C5" s="60"/>
-      <c r="D5" s="43" t="s">
+      <c r="C5" s="45"/>
+      <c r="D5" s="46" t="s">
         <v>2060</v>
       </c>
-      <c r="E5" s="43" t="s">
+      <c r="E5" s="46" t="s">
         <v>2061</v>
       </c>
-      <c r="F5" s="44" t="s">
+      <c r="F5" s="47" t="s">
         <v>2062</v>
       </c>
-      <c r="G5" s="45" t="s">
+      <c r="G5" s="48" t="s">
         <v>2075</v>
       </c>
-      <c r="H5" s="53" t="s">
+      <c r="H5" s="48" t="s">
         <v>2074</v>
       </c>
-      <c r="I5" s="50" t="b">
+      <c r="I5" s="49" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="37" t="s">
+      <c r="B6" s="50" t="s">
         <v>2076</v>
       </c>
-      <c r="C6" s="38"/>
-      <c r="D6" s="46">
+      <c r="C6" s="51"/>
+      <c r="D6" s="52">
         <v>1</v>
       </c>
-      <c r="E6" s="46"/>
-      <c r="F6" s="46"/>
-      <c r="G6" s="54" t="s">
+      <c r="E6" s="52"/>
+      <c r="F6" s="52"/>
+      <c r="G6" s="53" t="s">
         <v>2077</v>
       </c>
-      <c r="H6" s="54" t="s">
+      <c r="H6" s="53" t="s">
         <v>2067</v>
       </c>
-      <c r="I6" s="51" t="b">
+      <c r="I6" s="54" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="39"/>
-      <c r="C7" s="40"/>
-      <c r="D7" s="47"/>
-      <c r="E7" s="47"/>
-      <c r="F7" s="47"/>
-      <c r="G7" s="55"/>
-      <c r="H7" s="55"/>
-      <c r="I7" s="52"/>
+      <c r="B7" s="55"/>
+      <c r="C7" s="56"/>
+      <c r="D7" s="57"/>
+      <c r="E7" s="57"/>
+      <c r="F7" s="57"/>
+      <c r="G7" s="58"/>
+      <c r="H7" s="58"/>
+      <c r="I7" s="59"/>
     </row>
     <row r="8" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="39"/>
-      <c r="C8" s="40"/>
-      <c r="D8" s="47"/>
-      <c r="E8" s="47"/>
-      <c r="F8" s="47"/>
-      <c r="G8" s="55"/>
-      <c r="H8" s="55"/>
-      <c r="I8" s="52"/>
+      <c r="B8" s="55"/>
+      <c r="C8" s="56"/>
+      <c r="D8" s="57"/>
+      <c r="E8" s="57"/>
+      <c r="F8" s="57"/>
+      <c r="G8" s="58"/>
+      <c r="H8" s="58"/>
+      <c r="I8" s="59"/>
     </row>
     <row r="9" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="39"/>
-      <c r="C9" s="40"/>
-      <c r="D9" s="47"/>
-      <c r="E9" s="47"/>
-      <c r="F9" s="47"/>
-      <c r="G9" s="55"/>
-      <c r="H9" s="55"/>
-      <c r="I9" s="52"/>
+      <c r="B9" s="55"/>
+      <c r="C9" s="56"/>
+      <c r="D9" s="57"/>
+      <c r="E9" s="57"/>
+      <c r="F9" s="57"/>
+      <c r="G9" s="58"/>
+      <c r="H9" s="58"/>
+      <c r="I9" s="59"/>
     </row>
     <row r="10" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="39"/>
-      <c r="C10" s="40"/>
-      <c r="D10" s="47"/>
-      <c r="E10" s="47"/>
-      <c r="F10" s="47"/>
-      <c r="G10" s="55"/>
-      <c r="H10" s="55"/>
-      <c r="I10" s="52"/>
+      <c r="B10" s="55"/>
+      <c r="C10" s="56"/>
+      <c r="D10" s="57"/>
+      <c r="E10" s="57"/>
+      <c r="F10" s="57"/>
+      <c r="G10" s="58"/>
+      <c r="H10" s="58"/>
+      <c r="I10" s="59"/>
     </row>
     <row r="11" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="39"/>
-      <c r="C11" s="40"/>
-      <c r="D11" s="47"/>
-      <c r="E11" s="47"/>
-      <c r="F11" s="47"/>
-      <c r="G11" s="55"/>
-      <c r="H11" s="55"/>
-      <c r="I11" s="52"/>
+      <c r="B11" s="55"/>
+      <c r="C11" s="56"/>
+      <c r="D11" s="57"/>
+      <c r="E11" s="57"/>
+      <c r="F11" s="57"/>
+      <c r="G11" s="58"/>
+      <c r="H11" s="58"/>
+      <c r="I11" s="59"/>
     </row>
     <row r="12" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="39"/>
-      <c r="C12" s="40"/>
-      <c r="D12" s="47"/>
-      <c r="E12" s="47"/>
-      <c r="F12" s="47"/>
-      <c r="G12" s="55"/>
-      <c r="H12" s="55"/>
-      <c r="I12" s="52"/>
+      <c r="B12" s="55"/>
+      <c r="C12" s="56"/>
+      <c r="D12" s="57"/>
+      <c r="E12" s="57"/>
+      <c r="F12" s="57"/>
+      <c r="G12" s="58"/>
+      <c r="H12" s="58"/>
+      <c r="I12" s="59"/>
     </row>
     <row r="13" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="39"/>
-      <c r="C13" s="40"/>
-      <c r="D13" s="47"/>
-      <c r="E13" s="47"/>
-      <c r="F13" s="47"/>
-      <c r="G13" s="55"/>
-      <c r="H13" s="55"/>
-      <c r="I13" s="52"/>
+      <c r="B13" s="55"/>
+      <c r="C13" s="56"/>
+      <c r="D13" s="57"/>
+      <c r="E13" s="57"/>
+      <c r="F13" s="57"/>
+      <c r="G13" s="58"/>
+      <c r="H13" s="58"/>
+      <c r="I13" s="59"/>
     </row>
     <row r="14" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="39"/>
-      <c r="C14" s="40"/>
-      <c r="D14" s="47"/>
-      <c r="E14" s="47"/>
-      <c r="F14" s="47"/>
-      <c r="G14" s="55"/>
-      <c r="H14" s="55"/>
-      <c r="I14" s="52"/>
+      <c r="B14" s="55"/>
+      <c r="C14" s="56"/>
+      <c r="D14" s="57"/>
+      <c r="E14" s="57"/>
+      <c r="F14" s="57"/>
+      <c r="G14" s="58"/>
+      <c r="H14" s="58"/>
+      <c r="I14" s="59"/>
     </row>
     <row r="15" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="39"/>
-      <c r="C15" s="40"/>
-      <c r="D15" s="47"/>
-      <c r="E15" s="47"/>
-      <c r="F15" s="47"/>
-      <c r="G15" s="55"/>
-      <c r="H15" s="55"/>
-      <c r="I15" s="52"/>
+      <c r="B15" s="55"/>
+      <c r="C15" s="56"/>
+      <c r="D15" s="57"/>
+      <c r="E15" s="57"/>
+      <c r="F15" s="57"/>
+      <c r="G15" s="58"/>
+      <c r="H15" s="58"/>
+      <c r="I15" s="59"/>
     </row>
     <row r="16" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="39"/>
-      <c r="C16" s="40"/>
-      <c r="D16" s="47"/>
-      <c r="E16" s="47"/>
-      <c r="F16" s="47"/>
-      <c r="G16" s="55"/>
-      <c r="H16" s="55"/>
-      <c r="I16" s="52"/>
+      <c r="B16" s="55"/>
+      <c r="C16" s="56"/>
+      <c r="D16" s="57"/>
+      <c r="E16" s="57"/>
+      <c r="F16" s="57"/>
+      <c r="G16" s="58"/>
+      <c r="H16" s="58"/>
+      <c r="I16" s="59"/>
     </row>
     <row r="17" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="39"/>
-      <c r="C17" s="40"/>
-      <c r="D17" s="47"/>
-      <c r="E17" s="47"/>
-      <c r="F17" s="47"/>
-      <c r="G17" s="55"/>
-      <c r="H17" s="55"/>
-      <c r="I17" s="52"/>
+      <c r="B17" s="55"/>
+      <c r="C17" s="56"/>
+      <c r="D17" s="57"/>
+      <c r="E17" s="57"/>
+      <c r="F17" s="57"/>
+      <c r="G17" s="58"/>
+      <c r="H17" s="58"/>
+      <c r="I17" s="59"/>
     </row>
     <row r="18" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="39"/>
-      <c r="C18" s="40"/>
-      <c r="D18" s="47"/>
-      <c r="E18" s="47"/>
-      <c r="F18" s="47"/>
-      <c r="G18" s="55"/>
-      <c r="H18" s="55"/>
-      <c r="I18" s="52"/>
+      <c r="B18" s="55"/>
+      <c r="C18" s="56"/>
+      <c r="D18" s="57"/>
+      <c r="E18" s="57"/>
+      <c r="F18" s="57"/>
+      <c r="G18" s="58"/>
+      <c r="H18" s="58"/>
+      <c r="I18" s="59"/>
     </row>
     <row r="19" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="39"/>
-      <c r="C19" s="40"/>
-      <c r="D19" s="47"/>
-      <c r="E19" s="47"/>
-      <c r="F19" s="47"/>
-      <c r="G19" s="55"/>
-      <c r="H19" s="55"/>
-      <c r="I19" s="52"/>
+      <c r="B19" s="55"/>
+      <c r="C19" s="56"/>
+      <c r="D19" s="57"/>
+      <c r="E19" s="57"/>
+      <c r="F19" s="57"/>
+      <c r="G19" s="58"/>
+      <c r="H19" s="58"/>
+      <c r="I19" s="59"/>
     </row>
     <row r="20" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="39"/>
-      <c r="C20" s="40"/>
-      <c r="D20" s="47"/>
-      <c r="E20" s="47"/>
-      <c r="F20" s="47"/>
-      <c r="G20" s="55"/>
-      <c r="H20" s="55"/>
-      <c r="I20" s="52"/>
+      <c r="B20" s="55"/>
+      <c r="C20" s="56"/>
+      <c r="D20" s="57"/>
+      <c r="E20" s="57"/>
+      <c r="F20" s="57"/>
+      <c r="G20" s="58"/>
+      <c r="H20" s="58"/>
+      <c r="I20" s="59"/>
     </row>
     <row r="21" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="39"/>
-      <c r="C21" s="40"/>
-      <c r="D21" s="47"/>
-      <c r="E21" s="47"/>
-      <c r="F21" s="47"/>
-      <c r="G21" s="55"/>
-      <c r="H21" s="55"/>
-      <c r="I21" s="52"/>
+      <c r="B21" s="55"/>
+      <c r="C21" s="56"/>
+      <c r="D21" s="57"/>
+      <c r="E21" s="57"/>
+      <c r="F21" s="57"/>
+      <c r="G21" s="58"/>
+      <c r="H21" s="58"/>
+      <c r="I21" s="59"/>
     </row>
     <row r="22" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="39"/>
-      <c r="C22" s="40"/>
-      <c r="D22" s="47"/>
-      <c r="E22" s="47"/>
-      <c r="F22" s="47"/>
-      <c r="G22" s="55"/>
-      <c r="H22" s="55"/>
-      <c r="I22" s="52"/>
+      <c r="B22" s="55"/>
+      <c r="C22" s="56"/>
+      <c r="D22" s="57"/>
+      <c r="E22" s="57"/>
+      <c r="F22" s="57"/>
+      <c r="G22" s="58"/>
+      <c r="H22" s="58"/>
+      <c r="I22" s="59"/>
     </row>
     <row r="23" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="39"/>
-      <c r="C23" s="40"/>
-      <c r="D23" s="47"/>
-      <c r="E23" s="47"/>
-      <c r="F23" s="47"/>
-      <c r="G23" s="55"/>
-      <c r="H23" s="55"/>
-      <c r="I23" s="52"/>
+      <c r="B23" s="55"/>
+      <c r="C23" s="56"/>
+      <c r="D23" s="57"/>
+      <c r="E23" s="57"/>
+      <c r="F23" s="57"/>
+      <c r="G23" s="58"/>
+      <c r="H23" s="58"/>
+      <c r="I23" s="59"/>
     </row>
     <row r="24" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="39"/>
-      <c r="C24" s="40"/>
-      <c r="D24" s="47"/>
-      <c r="E24" s="47"/>
-      <c r="F24" s="47"/>
-      <c r="G24" s="55"/>
-      <c r="H24" s="55"/>
-      <c r="I24" s="52"/>
+      <c r="B24" s="55"/>
+      <c r="C24" s="56"/>
+      <c r="D24" s="57"/>
+      <c r="E24" s="57"/>
+      <c r="F24" s="57"/>
+      <c r="G24" s="58"/>
+      <c r="H24" s="58"/>
+      <c r="I24" s="59"/>
     </row>
     <row r="25" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="39"/>
-      <c r="C25" s="40"/>
-      <c r="D25" s="47"/>
-      <c r="E25" s="47"/>
-      <c r="F25" s="47"/>
-      <c r="G25" s="55"/>
-      <c r="H25" s="55"/>
-      <c r="I25" s="52"/>
+      <c r="B25" s="55"/>
+      <c r="C25" s="56"/>
+      <c r="D25" s="57"/>
+      <c r="E25" s="57"/>
+      <c r="F25" s="57"/>
+      <c r="G25" s="58"/>
+      <c r="H25" s="58"/>
+      <c r="I25" s="59"/>
     </row>
     <row r="26" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="39"/>
-      <c r="C26" s="40"/>
-      <c r="D26" s="47"/>
-      <c r="E26" s="47"/>
-      <c r="F26" s="47"/>
-      <c r="G26" s="55"/>
-      <c r="H26" s="55"/>
-      <c r="I26" s="52"/>
+      <c r="B26" s="55"/>
+      <c r="C26" s="56"/>
+      <c r="D26" s="57"/>
+      <c r="E26" s="57"/>
+      <c r="F26" s="57"/>
+      <c r="G26" s="58"/>
+      <c r="H26" s="58"/>
+      <c r="I26" s="59"/>
     </row>
     <row r="27" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="39"/>
-      <c r="C27" s="40"/>
-      <c r="D27" s="47"/>
-      <c r="E27" s="47"/>
-      <c r="F27" s="47"/>
-      <c r="G27" s="55"/>
-      <c r="H27" s="55"/>
-      <c r="I27" s="52"/>
+      <c r="B27" s="55"/>
+      <c r="C27" s="56"/>
+      <c r="D27" s="57"/>
+      <c r="E27" s="57"/>
+      <c r="F27" s="57"/>
+      <c r="G27" s="58"/>
+      <c r="H27" s="58"/>
+      <c r="I27" s="59"/>
     </row>
     <row r="28" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="39"/>
-      <c r="C28" s="40"/>
-      <c r="D28" s="47"/>
-      <c r="E28" s="47"/>
-      <c r="F28" s="47"/>
-      <c r="G28" s="55"/>
-      <c r="H28" s="55"/>
-      <c r="I28" s="52"/>
+      <c r="B28" s="55"/>
+      <c r="C28" s="56"/>
+      <c r="D28" s="57"/>
+      <c r="E28" s="57"/>
+      <c r="F28" s="57"/>
+      <c r="G28" s="58"/>
+      <c r="H28" s="58"/>
+      <c r="I28" s="59"/>
     </row>
     <row r="29" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="39"/>
-      <c r="C29" s="40"/>
-      <c r="D29" s="47"/>
-      <c r="E29" s="47"/>
-      <c r="F29" s="47"/>
-      <c r="G29" s="55"/>
-      <c r="H29" s="55"/>
-      <c r="I29" s="52"/>
+      <c r="B29" s="55"/>
+      <c r="C29" s="56"/>
+      <c r="D29" s="57"/>
+      <c r="E29" s="57"/>
+      <c r="F29" s="57"/>
+      <c r="G29" s="58"/>
+      <c r="H29" s="58"/>
+      <c r="I29" s="59"/>
     </row>
     <row r="30" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="39"/>
-      <c r="C30" s="40"/>
-      <c r="D30" s="47"/>
-      <c r="E30" s="47"/>
-      <c r="F30" s="47"/>
-      <c r="G30" s="55"/>
-      <c r="H30" s="55"/>
-      <c r="I30" s="52"/>
+      <c r="B30" s="55"/>
+      <c r="C30" s="56"/>
+      <c r="D30" s="57"/>
+      <c r="E30" s="57"/>
+      <c r="F30" s="57"/>
+      <c r="G30" s="58"/>
+      <c r="H30" s="58"/>
+      <c r="I30" s="59"/>
     </row>
     <row r="31" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="39"/>
-      <c r="C31" s="40"/>
-      <c r="D31" s="47"/>
-      <c r="E31" s="47"/>
-      <c r="F31" s="47"/>
-      <c r="G31" s="55"/>
-      <c r="H31" s="55"/>
-      <c r="I31" s="52"/>
+      <c r="B31" s="55"/>
+      <c r="C31" s="56"/>
+      <c r="D31" s="57"/>
+      <c r="E31" s="57"/>
+      <c r="F31" s="57"/>
+      <c r="G31" s="58"/>
+      <c r="H31" s="58"/>
+      <c r="I31" s="59"/>
     </row>
     <row r="32" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="39"/>
-      <c r="C32" s="40"/>
-      <c r="D32" s="47"/>
-      <c r="E32" s="47"/>
-      <c r="F32" s="47"/>
-      <c r="G32" s="55"/>
-      <c r="H32" s="55"/>
-      <c r="I32" s="52"/>
+      <c r="B32" s="55"/>
+      <c r="C32" s="56"/>
+      <c r="D32" s="57"/>
+      <c r="E32" s="57"/>
+      <c r="F32" s="57"/>
+      <c r="G32" s="58"/>
+      <c r="H32" s="58"/>
+      <c r="I32" s="59"/>
     </row>
     <row r="33" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="39"/>
-      <c r="C33" s="40"/>
-      <c r="D33" s="47"/>
-      <c r="E33" s="47"/>
-      <c r="F33" s="47"/>
-      <c r="G33" s="55"/>
-      <c r="H33" s="55"/>
-      <c r="I33" s="52"/>
+      <c r="B33" s="55"/>
+      <c r="C33" s="56"/>
+      <c r="D33" s="57"/>
+      <c r="E33" s="57"/>
+      <c r="F33" s="57"/>
+      <c r="G33" s="58"/>
+      <c r="H33" s="58"/>
+      <c r="I33" s="59"/>
     </row>
     <row r="34" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="39"/>
-      <c r="C34" s="40"/>
-      <c r="D34" s="47"/>
-      <c r="E34" s="47"/>
-      <c r="F34" s="47"/>
-      <c r="G34" s="55"/>
-      <c r="H34" s="55"/>
-      <c r="I34" s="52"/>
+      <c r="B34" s="55"/>
+      <c r="C34" s="56"/>
+      <c r="D34" s="57"/>
+      <c r="E34" s="57"/>
+      <c r="F34" s="57"/>
+      <c r="G34" s="58"/>
+      <c r="H34" s="58"/>
+      <c r="I34" s="59"/>
     </row>
     <row r="35" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="39"/>
-      <c r="C35" s="40"/>
-      <c r="D35" s="47"/>
-      <c r="E35" s="47"/>
-      <c r="F35" s="47"/>
-      <c r="G35" s="55"/>
-      <c r="H35" s="55"/>
-      <c r="I35" s="52"/>
+      <c r="B35" s="55"/>
+      <c r="C35" s="56"/>
+      <c r="D35" s="57"/>
+      <c r="E35" s="57"/>
+      <c r="F35" s="57"/>
+      <c r="G35" s="58"/>
+      <c r="H35" s="58"/>
+      <c r="I35" s="59"/>
     </row>
     <row r="36" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="39"/>
-      <c r="C36" s="40"/>
-      <c r="D36" s="47"/>
-      <c r="E36" s="47"/>
-      <c r="F36" s="47"/>
-      <c r="G36" s="55"/>
-      <c r="H36" s="55"/>
-      <c r="I36" s="52"/>
+      <c r="B36" s="55"/>
+      <c r="C36" s="56"/>
+      <c r="D36" s="57"/>
+      <c r="E36" s="57"/>
+      <c r="F36" s="57"/>
+      <c r="G36" s="58"/>
+      <c r="H36" s="58"/>
+      <c r="I36" s="59"/>
     </row>
     <row r="37" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="39"/>
-      <c r="C37" s="40"/>
-      <c r="D37" s="47"/>
-      <c r="E37" s="47"/>
-      <c r="F37" s="47"/>
-      <c r="G37" s="55"/>
-      <c r="H37" s="55"/>
-      <c r="I37" s="52"/>
+      <c r="B37" s="55"/>
+      <c r="C37" s="56"/>
+      <c r="D37" s="57"/>
+      <c r="E37" s="57"/>
+      <c r="F37" s="57"/>
+      <c r="G37" s="58"/>
+      <c r="H37" s="58"/>
+      <c r="I37" s="59"/>
     </row>
     <row r="38" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="39"/>
-      <c r="C38" s="40"/>
-      <c r="D38" s="47"/>
-      <c r="E38" s="47"/>
-      <c r="F38" s="47"/>
-      <c r="G38" s="55"/>
-      <c r="H38" s="55"/>
-      <c r="I38" s="52"/>
+      <c r="B38" s="55"/>
+      <c r="C38" s="56"/>
+      <c r="D38" s="57"/>
+      <c r="E38" s="57"/>
+      <c r="F38" s="57"/>
+      <c r="G38" s="58"/>
+      <c r="H38" s="58"/>
+      <c r="I38" s="59"/>
     </row>
     <row r="39" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="39"/>
-      <c r="C39" s="40"/>
-      <c r="D39" s="47"/>
-      <c r="E39" s="47"/>
-      <c r="F39" s="47"/>
-      <c r="G39" s="55"/>
-      <c r="H39" s="55"/>
-      <c r="I39" s="52"/>
+      <c r="B39" s="55"/>
+      <c r="C39" s="56"/>
+      <c r="D39" s="57"/>
+      <c r="E39" s="57"/>
+      <c r="F39" s="57"/>
+      <c r="G39" s="58"/>
+      <c r="H39" s="58"/>
+      <c r="I39" s="59"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -37886,7 +37883,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="5152" r:id="rId24" name="$H$15">
+            <control shapeId="5152" r:id="rId24" name="Check Box 32">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -37908,7 +37905,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="5153" r:id="rId25" name="$H$16">
+            <control shapeId="5153" r:id="rId25" name="Check Box 33">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -37930,7 +37927,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="5154" r:id="rId26" name="$H$17">
+            <control shapeId="5154" r:id="rId26" name="Check Box 34">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -37952,7 +37949,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="5155" r:id="rId27" name="$H$18">
+            <control shapeId="5155" r:id="rId27" name="Check Box 35">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -37974,7 +37971,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="5156" r:id="rId28" name="$H$19">
+            <control shapeId="5156" r:id="rId28" name="Check Box 36">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -37996,7 +37993,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="5157" r:id="rId29" name="$H$20">
+            <control shapeId="5157" r:id="rId29" name="Check Box 37">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -38018,7 +38015,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="5158" r:id="rId30" name="$H$21">
+            <control shapeId="5158" r:id="rId30" name="Check Box 38">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -38040,7 +38037,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="5159" r:id="rId31" name="$H$22">
+            <control shapeId="5159" r:id="rId31" name="Check Box 39">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -38062,7 +38059,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="5160" r:id="rId32" name="$H$23">
+            <control shapeId="5160" r:id="rId32" name="Check Box 40">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -38084,7 +38081,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="5161" r:id="rId33" name="$H$24">
+            <control shapeId="5161" r:id="rId33" name="Check Box 41">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -38106,7 +38103,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="5162" r:id="rId34" name="$H$25">
+            <control shapeId="5162" r:id="rId34" name="Check Box 42">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>

</xml_diff>

<commit_message>
Updated DB Change Scripts
</commit_message>
<xml_diff>
--- a/Stores IT System v0.xlsx
+++ b/Stores IT System v0.xlsx
@@ -26198,8 +26198,33 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2052" r:id="rId5" name="CommandButton1">
+        <control shapeId="2049" r:id="rId5" name="BtnDBConnect">
           <controlPr defaultSize="0" autoLine="0" r:id="rId6">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>24</xdr:row>
+                <xdr:rowOff>180975</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>26</xdr:row>
+                <xdr:rowOff>76200</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2049" r:id="rId5" name="BtnDBConnect"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2052" r:id="rId7" name="CommandButton1">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId8">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
@@ -26218,32 +26243,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2052" r:id="rId5" name="CommandButton1"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2049" r:id="rId7" name="BtnDBConnect">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId8">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>24</xdr:row>
-                <xdr:rowOff>180975</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>26</xdr:row>
-                <xdr:rowOff>76200</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2049" r:id="rId7" name="BtnDBConnect"/>
+        <control shapeId="2052" r:id="rId7" name="CommandButton1"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">

</xml_diff>

<commit_message>
Added Find Order Button
</commit_message>
<xml_diff>
--- a/Stores IT System v0.xlsx
+++ b/Stores IT System v0.xlsx
@@ -11553,6 +11553,44 @@
         <a:xfrm>
           <a:off x="21957926" y="3867150"/>
           <a:ext cx="258680" cy="252000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>153426</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>144000</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="925" name="TEMPLATE - FindOrder"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="23441026" y="3238500"/>
+          <a:ext cx="153425" cy="144000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -20595,7 +20633,7 @@
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
@@ -20991,8 +21029,33 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2052" r:id="rId5" name="CommandButton1">
+        <control shapeId="2049" r:id="rId5" name="BtnDBConnect">
           <controlPr defaultSize="0" autoLine="0" r:id="rId6">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>24</xdr:row>
+                <xdr:rowOff>180975</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>26</xdr:row>
+                <xdr:rowOff>76200</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2049" r:id="rId5" name="BtnDBConnect"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2052" r:id="rId7" name="CommandButton1">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId8">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
@@ -21011,32 +21074,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2052" r:id="rId5" name="CommandButton1"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2049" r:id="rId7" name="BtnDBConnect">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId8">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>24</xdr:row>
-                <xdr:rowOff>180975</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>26</xdr:row>
-                <xdr:rowOff>76200</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2049" r:id="rId7" name="BtnDBConnect"/>
+        <control shapeId="2052" r:id="rId7" name="CommandButton1"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">

</xml_diff>

<commit_message>
User Profile Building dropdown lists
</commit_message>
<xml_diff>
--- a/Stores IT System v0.xlsx
+++ b/Stores IT System v0.xlsx
@@ -2,6 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileSharing readOnlyRecommended="1" userName="Julian Turner" reservationPassword="CEBA"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="21075" windowHeight="9975"/>
@@ -12,10 +13,11 @@
     <sheet name="Version Control" sheetId="6" r:id="rId3"/>
     <sheet name="Lists" sheetId="7" r:id="rId4"/>
     <sheet name="Order List" sheetId="8" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="9" r:id="rId6"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId6"/>
     <externalReference r:id="rId7"/>
+    <externalReference r:id="rId8"/>
   </externalReferences>
   <definedNames>
     <definedName name="ACAExtCovCol">'[1]Station Detail'!$AB$13</definedName>
@@ -9266,7 +9268,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0000"/>
-    <numFmt numFmtId="166" formatCode="dd\ mmm\ yy"/>
+    <numFmt numFmtId="165" formatCode="dd\ mmm\ yy"/>
   </numFmts>
   <fonts count="13" x14ac:knownFonts="1">
     <font>
@@ -9812,21 +9814,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -9848,7 +9835,22 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -11596,6 +11598,44 @@
         <a:xfrm>
           <a:off x="22583775" y="3914775"/>
           <a:ext cx="238500" cy="216000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>152401</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>316806</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>73125</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1436" name="TEMPLATE - DropDown"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="23593426" y="2143125"/>
+          <a:ext cx="164405" cy="216000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14573,6 +14613,130 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>19049</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>209325</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>85724</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Rectangle 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3286125" y="1162049"/>
+          <a:ext cx="1800000" cy="2352675"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>501140</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>68668</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>555549</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>8120</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Right Triangle 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="18900000">
+          <a:off x="3549140" y="1973668"/>
+          <a:ext cx="1273609" cy="1272952"/>
+        </a:xfrm>
+        <a:prstGeom prst="rtTriangle">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent5"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
@@ -20603,7 +20767,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="ShtMain"/>
-  <dimension ref="B4:P28"/>
+  <dimension ref="C4:P28"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
@@ -20620,7 +20784,7 @@
     <col min="11" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
@@ -20628,7 +20792,7 @@
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -20636,58 +20800,53 @@
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B9" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C15" s="3"/>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C16" s="3"/>
     </row>
     <row r="23" spans="12:16" x14ac:dyDescent="0.25">
-      <c r="L23" s="51"/>
-      <c r="M23" s="51"/>
-      <c r="N23" s="51"/>
-      <c r="O23" s="51"/>
-      <c r="P23" s="51"/>
+      <c r="L23" s="59"/>
+      <c r="M23" s="59"/>
+      <c r="N23" s="59"/>
+      <c r="O23" s="59"/>
+      <c r="P23" s="59"/>
     </row>
     <row r="24" spans="12:16" x14ac:dyDescent="0.25">
-      <c r="L24" s="51"/>
-      <c r="M24" s="51"/>
-      <c r="N24" s="51"/>
-      <c r="O24" s="51"/>
-      <c r="P24" s="51"/>
+      <c r="L24" s="59"/>
+      <c r="M24" s="59"/>
+      <c r="N24" s="59"/>
+      <c r="O24" s="59"/>
+      <c r="P24" s="59"/>
     </row>
     <row r="25" spans="12:16" x14ac:dyDescent="0.25">
-      <c r="L25" s="51"/>
-      <c r="M25" s="51"/>
-      <c r="N25" s="51"/>
-      <c r="O25" s="51"/>
-      <c r="P25" s="51"/>
+      <c r="L25" s="59"/>
+      <c r="M25" s="59"/>
+      <c r="N25" s="59"/>
+      <c r="O25" s="59"/>
+      <c r="P25" s="59"/>
     </row>
     <row r="26" spans="12:16" x14ac:dyDescent="0.25">
-      <c r="L26" s="51"/>
-      <c r="M26" s="51"/>
-      <c r="N26" s="51"/>
-      <c r="O26" s="51"/>
-      <c r="P26" s="51"/>
+      <c r="L26" s="59"/>
+      <c r="M26" s="59"/>
+      <c r="N26" s="59"/>
+      <c r="O26" s="59"/>
+      <c r="P26" s="59"/>
     </row>
     <row r="27" spans="12:16" x14ac:dyDescent="0.25">
-      <c r="L27" s="51"/>
-      <c r="M27" s="51"/>
-      <c r="N27" s="51"/>
-      <c r="O27" s="51"/>
-      <c r="P27" s="51"/>
+      <c r="L27" s="59"/>
+      <c r="M27" s="59"/>
+      <c r="N27" s="59"/>
+      <c r="O27" s="59"/>
+      <c r="P27" s="59"/>
     </row>
     <row r="28" spans="12:16" x14ac:dyDescent="0.25">
-      <c r="L28" s="51"/>
-      <c r="M28" s="51"/>
-      <c r="N28" s="51"/>
-      <c r="O28" s="51"/>
-      <c r="P28" s="51"/>
+      <c r="L28" s="59"/>
+      <c r="M28" s="59"/>
+      <c r="N28" s="59"/>
+      <c r="O28" s="59"/>
+      <c r="P28" s="59"/>
     </row>
   </sheetData>
   <dataConsolidate/>
@@ -21034,8 +21193,33 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2052" r:id="rId5" name="CommandButton1">
+        <control shapeId="2049" r:id="rId5" name="BtnDBConnect">
           <controlPr defaultSize="0" autoLine="0" r:id="rId6">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>24</xdr:row>
+                <xdr:rowOff>180975</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>26</xdr:row>
+                <xdr:rowOff>76200</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2049" r:id="rId5" name="BtnDBConnect"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2052" r:id="rId7" name="CommandButton1">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId8">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
@@ -21054,32 +21238,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2052" r:id="rId5" name="CommandButton1"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2049" r:id="rId7" name="BtnDBConnect">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId8">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>24</xdr:row>
-                <xdr:rowOff>180975</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>26</xdr:row>
-                <xdr:rowOff>76200</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2049" r:id="rId7" name="BtnDBConnect"/>
+        <control shapeId="2052" r:id="rId7" name="CommandButton1"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -34993,53 +35152,53 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="52" t="s">
+      <c r="B1" s="60" t="s">
         <v>1919</v>
       </c>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
-      <c r="I1" s="52"/>
-      <c r="J1" s="52"/>
-    </row>
-    <row r="3" spans="2:11" s="60" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="61" t="s">
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="60"/>
+      <c r="H1" s="60"/>
+      <c r="I1" s="60"/>
+      <c r="J1" s="60"/>
+    </row>
+    <row r="3" spans="2:11" s="55" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="56" t="s">
         <v>1913</v>
       </c>
-      <c r="C3" s="58">
+      <c r="C3" s="53">
         <v>443</v>
       </c>
-      <c r="D3" s="61" t="s">
+      <c r="D3" s="56" t="s">
         <v>3059</v>
       </c>
-      <c r="E3" s="63">
+      <c r="E3" s="58">
         <v>42898</v>
       </c>
-      <c r="F3" s="58"/>
-      <c r="G3" s="61" t="s">
+      <c r="F3" s="53"/>
+      <c r="G3" s="56" t="s">
         <v>1931</v>
       </c>
-      <c r="H3" s="58" t="s">
+      <c r="H3" s="53" t="s">
         <v>121</v>
       </c>
-      <c r="I3" s="59" t="s">
+      <c r="I3" s="54" t="s">
         <v>1914</v>
       </c>
-      <c r="J3" s="62" t="s">
+      <c r="J3" s="57" t="s">
         <v>3060</v>
       </c>
     </row>
     <row r="4" spans="2:11" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="2:11" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="53" t="s">
+      <c r="B5" s="61" t="s">
         <v>1915</v>
       </c>
-      <c r="C5" s="55"/>
-      <c r="D5" s="55"/>
-      <c r="E5" s="54"/>
+      <c r="C5" s="62"/>
+      <c r="D5" s="62"/>
+      <c r="E5" s="63"/>
       <c r="F5" s="37" t="s">
         <v>1916</v>
       </c>
@@ -35063,8 +35222,8 @@
       <c r="B6" s="41" t="s">
         <v>303</v>
       </c>
-      <c r="C6" s="56"/>
-      <c r="D6" s="56"/>
+      <c r="C6" s="51"/>
+      <c r="D6" s="51"/>
       <c r="E6" s="42"/>
       <c r="F6" s="43">
         <v>1</v>
@@ -35085,8 +35244,8 @@
       <c r="B7" s="46" t="s">
         <v>371</v>
       </c>
-      <c r="C7" s="57"/>
-      <c r="D7" s="57"/>
+      <c r="C7" s="52"/>
+      <c r="D7" s="52"/>
       <c r="E7" s="47"/>
       <c r="F7" s="48">
         <v>1</v>
@@ -35103,8 +35262,8 @@
     </row>
     <row r="8" spans="2:11" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="46"/>
-      <c r="C8" s="57"/>
-      <c r="D8" s="57"/>
+      <c r="C8" s="52"/>
+      <c r="D8" s="52"/>
       <c r="E8" s="47"/>
       <c r="F8" s="48"/>
       <c r="G8" s="48"/>
@@ -35115,8 +35274,8 @@
     </row>
     <row r="9" spans="2:11" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="46"/>
-      <c r="C9" s="57"/>
-      <c r="D9" s="57"/>
+      <c r="C9" s="52"/>
+      <c r="D9" s="52"/>
       <c r="E9" s="47"/>
       <c r="F9" s="48"/>
       <c r="G9" s="48"/>
@@ -35127,8 +35286,8 @@
     </row>
     <row r="10" spans="2:11" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="46"/>
-      <c r="C10" s="57"/>
-      <c r="D10" s="57"/>
+      <c r="C10" s="52"/>
+      <c r="D10" s="52"/>
       <c r="E10" s="47"/>
       <c r="F10" s="48"/>
       <c r="G10" s="48"/>
@@ -35139,8 +35298,8 @@
     </row>
     <row r="11" spans="2:11" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="46"/>
-      <c r="C11" s="57"/>
-      <c r="D11" s="57"/>
+      <c r="C11" s="52"/>
+      <c r="D11" s="52"/>
       <c r="E11" s="47"/>
       <c r="F11" s="48"/>
       <c r="G11" s="48"/>
@@ -35151,8 +35310,8 @@
     </row>
     <row r="12" spans="2:11" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="46"/>
-      <c r="C12" s="57"/>
-      <c r="D12" s="57"/>
+      <c r="C12" s="52"/>
+      <c r="D12" s="52"/>
       <c r="E12" s="47"/>
       <c r="F12" s="48"/>
       <c r="G12" s="48"/>
@@ -35163,8 +35322,8 @@
     </row>
     <row r="13" spans="2:11" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="46"/>
-      <c r="C13" s="57"/>
-      <c r="D13" s="57"/>
+      <c r="C13" s="52"/>
+      <c r="D13" s="52"/>
       <c r="E13" s="47"/>
       <c r="F13" s="48"/>
       <c r="G13" s="48"/>
@@ -35175,8 +35334,8 @@
     </row>
     <row r="14" spans="2:11" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="46"/>
-      <c r="C14" s="57"/>
-      <c r="D14" s="57"/>
+      <c r="C14" s="52"/>
+      <c r="D14" s="52"/>
       <c r="E14" s="47"/>
       <c r="F14" s="48"/>
       <c r="G14" s="48"/>
@@ -35187,8 +35346,8 @@
     </row>
     <row r="15" spans="2:11" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="46"/>
-      <c r="C15" s="57"/>
-      <c r="D15" s="57"/>
+      <c r="C15" s="52"/>
+      <c r="D15" s="52"/>
       <c r="E15" s="47"/>
       <c r="F15" s="48"/>
       <c r="G15" s="48"/>
@@ -35199,8 +35358,8 @@
     </row>
     <row r="16" spans="2:11" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="46"/>
-      <c r="C16" s="57"/>
-      <c r="D16" s="57"/>
+      <c r="C16" s="52"/>
+      <c r="D16" s="52"/>
       <c r="E16" s="47"/>
       <c r="F16" s="48"/>
       <c r="G16" s="48"/>
@@ -35211,8 +35370,8 @@
     </row>
     <row r="17" spans="2:11" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="46"/>
-      <c r="C17" s="57"/>
-      <c r="D17" s="57"/>
+      <c r="C17" s="52"/>
+      <c r="D17" s="52"/>
       <c r="E17" s="47"/>
       <c r="F17" s="48"/>
       <c r="G17" s="48"/>
@@ -35223,8 +35382,8 @@
     </row>
     <row r="18" spans="2:11" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="46"/>
-      <c r="C18" s="57"/>
-      <c r="D18" s="57"/>
+      <c r="C18" s="52"/>
+      <c r="D18" s="52"/>
       <c r="E18" s="47"/>
       <c r="F18" s="48"/>
       <c r="G18" s="48"/>
@@ -35235,8 +35394,8 @@
     </row>
     <row r="19" spans="2:11" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="46"/>
-      <c r="C19" s="57"/>
-      <c r="D19" s="57"/>
+      <c r="C19" s="52"/>
+      <c r="D19" s="52"/>
       <c r="E19" s="47"/>
       <c r="F19" s="48"/>
       <c r="G19" s="48"/>
@@ -35247,8 +35406,8 @@
     </row>
     <row r="20" spans="2:11" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="46"/>
-      <c r="C20" s="57"/>
-      <c r="D20" s="57"/>
+      <c r="C20" s="52"/>
+      <c r="D20" s="52"/>
       <c r="E20" s="47"/>
       <c r="F20" s="48"/>
       <c r="G20" s="48"/>
@@ -35259,8 +35418,8 @@
     </row>
     <row r="21" spans="2:11" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="46"/>
-      <c r="C21" s="57"/>
-      <c r="D21" s="57"/>
+      <c r="C21" s="52"/>
+      <c r="D21" s="52"/>
       <c r="E21" s="47"/>
       <c r="F21" s="48"/>
       <c r="G21" s="48"/>
@@ -35271,8 +35430,8 @@
     </row>
     <row r="22" spans="2:11" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="46"/>
-      <c r="C22" s="57"/>
-      <c r="D22" s="57"/>
+      <c r="C22" s="52"/>
+      <c r="D22" s="52"/>
       <c r="E22" s="47"/>
       <c r="F22" s="48"/>
       <c r="G22" s="48"/>
@@ -35283,8 +35442,8 @@
     </row>
     <row r="23" spans="2:11" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="46"/>
-      <c r="C23" s="57"/>
-      <c r="D23" s="57"/>
+      <c r="C23" s="52"/>
+      <c r="D23" s="52"/>
       <c r="E23" s="47"/>
       <c r="F23" s="48"/>
       <c r="G23" s="48"/>
@@ -35295,8 +35454,8 @@
     </row>
     <row r="24" spans="2:11" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="46"/>
-      <c r="C24" s="57"/>
-      <c r="D24" s="57"/>
+      <c r="C24" s="52"/>
+      <c r="D24" s="52"/>
       <c r="E24" s="47"/>
       <c r="F24" s="48"/>
       <c r="G24" s="48"/>
@@ -35307,8 +35466,8 @@
     </row>
     <row r="25" spans="2:11" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="46"/>
-      <c r="C25" s="57"/>
-      <c r="D25" s="57"/>
+      <c r="C25" s="52"/>
+      <c r="D25" s="52"/>
       <c r="E25" s="47"/>
       <c r="F25" s="48"/>
       <c r="G25" s="48"/>
@@ -35319,8 +35478,8 @@
     </row>
     <row r="26" spans="2:11" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="46"/>
-      <c r="C26" s="57"/>
-      <c r="D26" s="57"/>
+      <c r="C26" s="52"/>
+      <c r="D26" s="52"/>
       <c r="E26" s="47"/>
       <c r="F26" s="48"/>
       <c r="G26" s="48"/>
@@ -35331,8 +35490,8 @@
     </row>
     <row r="27" spans="2:11" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="46"/>
-      <c r="C27" s="57"/>
-      <c r="D27" s="57"/>
+      <c r="C27" s="52"/>
+      <c r="D27" s="52"/>
       <c r="E27" s="47"/>
       <c r="F27" s="48"/>
       <c r="G27" s="48"/>
@@ -35343,8 +35502,8 @@
     </row>
     <row r="28" spans="2:11" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="46"/>
-      <c r="C28" s="57"/>
-      <c r="D28" s="57"/>
+      <c r="C28" s="52"/>
+      <c r="D28" s="52"/>
       <c r="E28" s="47"/>
       <c r="F28" s="48"/>
       <c r="G28" s="48"/>
@@ -35355,8 +35514,8 @@
     </row>
     <row r="29" spans="2:11" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="46"/>
-      <c r="C29" s="57"/>
-      <c r="D29" s="57"/>
+      <c r="C29" s="52"/>
+      <c r="D29" s="52"/>
       <c r="E29" s="47"/>
       <c r="F29" s="48"/>
       <c r="G29" s="48"/>
@@ -35367,8 +35526,8 @@
     </row>
     <row r="30" spans="2:11" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="46"/>
-      <c r="C30" s="57"/>
-      <c r="D30" s="57"/>
+      <c r="C30" s="52"/>
+      <c r="D30" s="52"/>
       <c r="E30" s="47"/>
       <c r="F30" s="48"/>
       <c r="G30" s="48"/>
@@ -35379,8 +35538,8 @@
     </row>
     <row r="31" spans="2:11" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="46"/>
-      <c r="C31" s="57"/>
-      <c r="D31" s="57"/>
+      <c r="C31" s="52"/>
+      <c r="D31" s="52"/>
       <c r="E31" s="47"/>
       <c r="F31" s="48"/>
       <c r="G31" s="48"/>
@@ -35391,8 +35550,8 @@
     </row>
     <row r="32" spans="2:11" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="46"/>
-      <c r="C32" s="57"/>
-      <c r="D32" s="57"/>
+      <c r="C32" s="52"/>
+      <c r="D32" s="52"/>
       <c r="E32" s="47"/>
       <c r="F32" s="48"/>
       <c r="G32" s="48"/>
@@ -35403,8 +35562,8 @@
     </row>
     <row r="33" spans="2:11" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="46"/>
-      <c r="C33" s="57"/>
-      <c r="D33" s="57"/>
+      <c r="C33" s="52"/>
+      <c r="D33" s="52"/>
       <c r="E33" s="47"/>
       <c r="F33" s="48"/>
       <c r="G33" s="48"/>
@@ -35415,8 +35574,8 @@
     </row>
     <row r="34" spans="2:11" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="46"/>
-      <c r="C34" s="57"/>
-      <c r="D34" s="57"/>
+      <c r="C34" s="52"/>
+      <c r="D34" s="52"/>
       <c r="E34" s="47"/>
       <c r="F34" s="48"/>
       <c r="G34" s="48"/>
@@ -35427,8 +35586,8 @@
     </row>
     <row r="35" spans="2:11" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="46"/>
-      <c r="C35" s="57"/>
-      <c r="D35" s="57"/>
+      <c r="C35" s="52"/>
+      <c r="D35" s="52"/>
       <c r="E35" s="47"/>
       <c r="F35" s="48"/>
       <c r="G35" s="48"/>
@@ -35439,8 +35598,8 @@
     </row>
     <row r="36" spans="2:11" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="46"/>
-      <c r="C36" s="57"/>
-      <c r="D36" s="57"/>
+      <c r="C36" s="52"/>
+      <c r="D36" s="52"/>
       <c r="E36" s="47"/>
       <c r="F36" s="48"/>
       <c r="G36" s="48"/>
@@ -35451,8 +35610,8 @@
     </row>
     <row r="37" spans="2:11" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="46"/>
-      <c r="C37" s="57"/>
-      <c r="D37" s="57"/>
+      <c r="C37" s="52"/>
+      <c r="D37" s="52"/>
       <c r="E37" s="47"/>
       <c r="F37" s="48"/>
       <c r="G37" s="48"/>
@@ -35463,8 +35622,8 @@
     </row>
     <row r="38" spans="2:11" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="46"/>
-      <c r="C38" s="57"/>
-      <c r="D38" s="57"/>
+      <c r="C38" s="52"/>
+      <c r="D38" s="52"/>
       <c r="E38" s="47"/>
       <c r="F38" s="48"/>
       <c r="G38" s="48"/>
@@ -35475,8 +35634,8 @@
     </row>
     <row r="39" spans="2:11" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="46"/>
-      <c r="C39" s="57"/>
-      <c r="D39" s="57"/>
+      <c r="C39" s="52"/>
+      <c r="D39" s="52"/>
       <c r="E39" s="47"/>
       <c r="F39" s="48"/>
       <c r="G39" s="48"/>
@@ -36449,4 +36608,20 @@
     </mc:Choice>
   </mc:AlternateContent>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
User Profile Display icon build dropdown class
</commit_message>
<xml_diff>
--- a/Stores IT System v0.xlsx
+++ b/Stores IT System v0.xlsx
@@ -13,10 +13,11 @@
     <sheet name="Version Control" sheetId="6" r:id="rId3"/>
     <sheet name="Lists" sheetId="7" r:id="rId4"/>
     <sheet name="Order List" sheetId="8" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="9" r:id="rId6"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId6"/>
     <externalReference r:id="rId7"/>
+    <externalReference r:id="rId8"/>
   </externalReferences>
   <definedNames>
     <definedName name="ACAExtCovCol">'[1]Station Detail'!$AB$13</definedName>
@@ -9709,7 +9710,7 @@
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -9836,6 +9837,9 @@
     </xf>
     <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -10109,98 +10113,6 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>127000</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>66675</xdr:colOff>
-      <xdr:row>54</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="Main Screen"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="127000" y="127000"/>
-          <a:ext cx="13017500" cy="10160000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:gradFill flip="none" rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:srgbClr val="154E54"/>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:srgbClr val="154E54"/>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="1"/>
-          <a:tileRect/>
-        </a:gradFill>
-        <a:ln w="0" cap="flat" cmpd="sng" algn="ctr">
-          <a:noFill/>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst>
-          <a:outerShdw blurRad="63500" dist="37357" dir="2700000" rotWithShape="0">
-            <a:prstClr val="black">
-              <a:alpha val="40000"/>
-            </a:prstClr>
-          </a:outerShdw>
-        </a:effectLst>
-        <a:extLst>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:prstDash val="solid"/>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="en-GB" sz="1100" b="0">
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:latin typeface=""/>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>25</xdr:col>
@@ -11697,2620 +11609,234 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>28576</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>685800</xdr:colOff>
-      <xdr:row>54</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="MenuBar"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="127000"/>
-          <a:ext cx="1905000" cy="10160000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:gradFill flip="none" rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:srgbClr val="322924"/>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:srgbClr val="322924"/>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="1"/>
-          <a:tileRect/>
-        </a:gradFill>
-        <a:ln w="0" cap="flat" cmpd="sng" algn="ctr">
-          <a:noFill/>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst>
-          <a:outerShdw blurRad="63500" dist="37357" dir="2700000" rotWithShape="0">
-            <a:prstClr val="black">
-              <a:alpha val="40000"/>
-            </a:prstClr>
-          </a:outerShdw>
-        </a:effectLst>
-        <a:extLst>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:prstDash val="solid"/>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="en-GB" sz="1100" b="0">
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:latin typeface=""/>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>127000</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="Rectangle 2" hidden="1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="127000" cy="127000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="en-GB" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>685800</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>139700</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="'ModUIMenu.ProcessBtnPress(1)'" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="MenuItem - My Station"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="2413000"/>
-          <a:ext cx="1905000" cy="393700"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:gradFill flip="none" rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:srgbClr val="705C50"/>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:srgbClr val="322924"/>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="1"/>
-          <a:tileRect/>
-        </a:gradFill>
-        <a:ln w="0" cap="flat" cmpd="sng" algn="ctr">
-          <a:noFill/>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst/>
-        <a:extLst>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:prstDash val="solid"/>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1200" b="0">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-              <a:latin typeface="Eras Medium ITC"/>
-            </a:rPr>
-            <a:t>My Station</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>63500</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>263640</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>25500</xdr:rowOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>229725</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>76095</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="24" name="Icon - My Station"/>
+        <xdr:cNvPr id="1318" name="TEMPLATE - DropDown"/>
         <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12">
-          <a:clrChange>
-            <a:clrFrom>
-              <a:srgbClr val="FFFFFF"/>
-            </a:clrFrom>
-            <a:clrTo>
-              <a:srgbClr val="FFFFFF">
-                <a:alpha val="0"/>
-              </a:srgbClr>
-            </a:clrTo>
-          </a:clrChange>
-        </a:blip>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="63500" y="2476500"/>
-          <a:ext cx="200140" cy="216000"/>
+          <a:off x="21697950" y="2886076"/>
+          <a:ext cx="144000" cy="238019"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent4">
+              <a:lumMod val="50000"/>
+              <a:lumOff val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>180976</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>685800</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>139700</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="'ModUIMenu.ProcessBtnPress(2)'" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="10" name="MenuItem - Stores"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="2794000"/>
-          <a:ext cx="1905000" cy="393700"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:gradFill flip="none" rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:srgbClr val="705C50"/>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:srgbClr val="322924"/>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="1"/>
-          <a:tileRect/>
-        </a:gradFill>
-        <a:ln w="0" cap="flat" cmpd="sng" algn="ctr">
-          <a:noFill/>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst/>
-        <a:extLst>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:prstDash val="solid"/>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1200" b="0">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-              <a:latin typeface="Eras Medium ITC"/>
-            </a:rPr>
-            <a:t>Stores</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>63500</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>280206</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>25500</xdr:rowOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>382125</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>37995</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="26" name="Icon - Stores"/>
+        <xdr:cNvPr id="1213" name="TEMPLATE - DropDown"/>
         <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13">
-          <a:clrChange>
-            <a:clrFrom>
-              <a:srgbClr val="FFFFFF"/>
-            </a:clrFrom>
-            <a:clrTo>
-              <a:srgbClr val="FFFFFF">
-                <a:alpha val="0"/>
-              </a:srgbClr>
-            </a:clrTo>
-          </a:clrChange>
-        </a:blip>
-        <a:srcRect t="1291"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="63500" y="2857500"/>
-          <a:ext cx="216706" cy="216000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>685800</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>139700</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="'ModUIMenu.ProcessBtnPress(3)'" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="13" name="MenuItem - Reports"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="3175000"/>
-          <a:ext cx="1905000" cy="393700"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:gradFill flip="none" rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:srgbClr val="705C50"/>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:srgbClr val="322924"/>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="1"/>
-          <a:tileRect/>
-        </a:gradFill>
-        <a:ln w="0" cap="flat" cmpd="sng" algn="ctr">
-          <a:noFill/>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst/>
-        <a:extLst>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:prstDash val="solid"/>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1200" b="0">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-              <a:latin typeface="Eras Medium ITC"/>
-            </a:rPr>
-            <a:t>Reports</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>63500</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>223500</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>25500</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="28" name="Icon - Reports"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14">
-          <a:clrChange>
-            <a:clrFrom>
-              <a:srgbClr val="F8FFF4"/>
-            </a:clrFrom>
-            <a:clrTo>
-              <a:srgbClr val="F8FFF4">
-                <a:alpha val="0"/>
-              </a:srgbClr>
-            </a:clrTo>
-          </a:clrChange>
-        </a:blip>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="63500" y="3238500"/>
-          <a:ext cx="160000" cy="216000"/>
+          <a:off x="21850350" y="3038476"/>
+          <a:ext cx="144000" cy="238019"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent4">
+              <a:lumMod val="50000"/>
+              <a:lumOff val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>180976</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>685800</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>139700</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="'ModUIMenu.ProcessBtnPress(4)'" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="14" name="MenuItem - My Profile"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="3556000"/>
-          <a:ext cx="1905000" cy="393700"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:gradFill flip="none" rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:srgbClr val="20A39E"/>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:srgbClr val="20A39E"/>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="1"/>
-          <a:tileRect/>
-        </a:gradFill>
-        <a:ln w="0" cap="flat" cmpd="sng" algn="ctr">
-          <a:noFill/>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst/>
-        <a:extLst>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:prstDash val="solid"/>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1200" b="0">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-              <a:latin typeface="Eras Medium ITC"/>
-            </a:rPr>
-            <a:t>My Profile</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>63500</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>270634</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>25500</xdr:rowOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>382125</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>37995</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="30" name="Icon - My Profile"/>
+        <xdr:cNvPr id="1222" name="TEMPLATE - DropDown"/>
         <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15">
-          <a:clrChange>
-            <a:clrFrom>
-              <a:srgbClr val="FFFFFF"/>
-            </a:clrFrom>
-            <a:clrTo>
-              <a:srgbClr val="FFFFFF">
-                <a:alpha val="0"/>
-              </a:srgbClr>
-            </a:clrTo>
-          </a:clrChange>
-        </a:blip>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="63500" y="3619500"/>
-          <a:ext cx="207134" cy="216000"/>
+          <a:off x="21850350" y="3038476"/>
+          <a:ext cx="144000" cy="238019"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent4">
+              <a:lumMod val="50000"/>
+              <a:lumOff val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>180976</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>685800</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>139700</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="'ModUIMenu.ProcessBtnPress(5)'" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="15" name="MenuItem - Support"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="3937000"/>
-          <a:ext cx="1905000" cy="393700"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:gradFill flip="none" rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:srgbClr val="705C50"/>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:srgbClr val="322924"/>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="1"/>
-          <a:tileRect/>
-        </a:gradFill>
-        <a:ln w="0" cap="flat" cmpd="sng" algn="ctr">
-          <a:noFill/>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst/>
-        <a:extLst>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:prstDash val="solid"/>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1200" b="0">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-              <a:latin typeface="Eras Medium ITC"/>
-            </a:rPr>
-            <a:t>Support</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>63500</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>277622</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>25500</xdr:rowOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>382125</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>37995</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="32" name="Icon - Support"/>
+        <xdr:cNvPr id="1345" name="TEMPLATE - DropDown"/>
         <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16">
-          <a:clrChange>
-            <a:clrFrom>
-              <a:srgbClr val="F8FFF4"/>
-            </a:clrFrom>
-            <a:clrTo>
-              <a:srgbClr val="F8FFF4">
-                <a:alpha val="0"/>
-              </a:srgbClr>
-            </a:clrTo>
-          </a:clrChange>
-        </a:blip>
-        <a:srcRect l="2786" t="3867" r="1938" b="817"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="63500" y="4000500"/>
-          <a:ext cx="214122" cy="216000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>685800</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>139700</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="'ModUIMenu.ProcessBtnPress(6)'" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="16" name="MenuItem - Exit"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="4318000"/>
-          <a:ext cx="1905000" cy="393700"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:gradFill flip="none" rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:srgbClr val="705C50"/>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:srgbClr val="322924"/>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="1"/>
-          <a:tileRect/>
-        </a:gradFill>
-        <a:ln w="0" cap="flat" cmpd="sng" algn="ctr">
-          <a:noFill/>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst/>
-        <a:extLst>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:prstDash val="solid"/>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1200" b="0">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-              <a:latin typeface="Eras Medium ITC"/>
-            </a:rPr>
-            <a:t>Exit</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>63500</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>302000</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>25500</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="34" name="Icon - Exit"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17">
-          <a:clrChange>
-            <a:clrFrom>
-              <a:srgbClr val="F8FFF4"/>
-            </a:clrFrom>
-            <a:clrTo>
-              <a:srgbClr val="F8FFF4">
-                <a:alpha val="0"/>
-              </a:srgbClr>
-            </a:clrTo>
-          </a:clrChange>
-        </a:blip>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="63500" y="4381500"/>
-          <a:ext cx="238500" cy="216000"/>
+          <a:off x="21850350" y="3038476"/>
+          <a:ext cx="144000" cy="238019"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent4">
+              <a:lumMod val="50000"/>
+              <a:lumOff val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>180976</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>127000</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="901" name="Rectangle 900"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="127000" cy="127000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="en-GB" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>29</xdr:col>
-      <xdr:colOff>38098</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>29</xdr:col>
-      <xdr:colOff>186871</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>20175</xdr:rowOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>382125</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>37995</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="111" name="TEMPLATE - DropDown"/>
+        <xdr:cNvPr id="1357" name="TEMPLATE - DropDown"/>
         <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="22869523" y="2543175"/>
-          <a:ext cx="148773" cy="144000"/>
+          <a:off x="21850350" y="3038476"/>
+          <a:ext cx="144000" cy="238019"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>1003300</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>1943100</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="1598" name="My Profile Frame 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2222500" y="254000"/>
-          <a:ext cx="5588000" cy="3111500"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:gradFill flip="none" rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:srgbClr val="FFFFFF"/>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:srgbClr val="FFFFFF"/>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="1"/>
-          <a:tileRect/>
-        </a:gradFill>
-        <a:ln w="0" cap="flat" cmpd="sng" algn="ctr">
-          <a:noFill/>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst>
-          <a:outerShdw blurRad="63500" dist="37357" dir="2700000" rotWithShape="0">
-            <a:prstClr val="black">
-              <a:alpha val="40000"/>
-            </a:prstClr>
-          </a:outerShdw>
-        </a:effectLst>
-        <a:extLst>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:prstDash val="solid"/>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="en-GB" sz="1100" b="0">
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:latin typeface=""/>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>1003300</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>1943100</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="1597" name="My Profile 1 Header"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2222500" y="254000"/>
-          <a:ext cx="5588000" cy="317500"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:gradFill flip="none" rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:srgbClr val="20A39E"/>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:srgbClr val="20A39E"/>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="1"/>
-          <a:tileRect/>
-        </a:gradFill>
-        <a:ln w="0" cap="flat" cmpd="sng" algn="ctr">
-          <a:noFill/>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst/>
-        <a:extLst>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:prstDash val="solid"/>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1200" b="1">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-              <a:latin typeface="Calibri"/>
-            </a:rPr>
-            <a:t>My Profile</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>1672466</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>1879600</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>152500</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="98" name="My Profile Frame 1 Icon"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15">
-          <a:clrChange>
-            <a:clrFrom>
-              <a:srgbClr val="FFFFFF"/>
-            </a:clrFrom>
-            <a:clrTo>
-              <a:srgbClr val="FFFFFF">
-                <a:alpha val="0"/>
-              </a:srgbClr>
-            </a:clrTo>
-          </a:clrChange>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7539866" y="317500"/>
-          <a:ext cx="207134" cy="216000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>1130300</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>701675</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="" fLocksText="0">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="913" name="TextBox 912"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2349500" y="762000"/>
-          <a:ext cx="952500" cy="254000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:gradFill flip="none" rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:srgbClr val="FFFFFF"/>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:srgbClr val="FFFFFF"/>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="1"/>
-          <a:tileRect/>
-        </a:gradFill>
-        <a:ln w="0" cmpd="sng">
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-        <a:extLst>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1000" b="0">
-              <a:solidFill>
-                <a:srgbClr val="154E54"/>
-              </a:solidFill>
-              <a:latin typeface="Eras Medium ITC"/>
-            </a:rPr>
-            <a:t>Crew No</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>701675</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>454025</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="" fLocksText="0">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="914" name="TextBox 913"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3302000" y="762000"/>
-          <a:ext cx="1524000" cy="254000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
+        <a:ln>
           <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:shade val="50000"/>
+            <a:schemeClr val="accent4">
+              <a:lumMod val="50000"/>
+              <a:lumOff val="50000"/>
             </a:schemeClr>
           </a:solidFill>
         </a:ln>
       </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100"/>
-            <a:t>5398</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>1130300</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>701675</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="" fLocksText="0">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="915" name="TextBox 914"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2349500" y="1270000"/>
-          <a:ext cx="952500" cy="254000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:gradFill flip="none" rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:srgbClr val="FFFFFF"/>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:srgbClr val="FFFFFF"/>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="1"/>
-          <a:tileRect/>
-        </a:gradFill>
-        <a:ln w="0" cmpd="sng">
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-        <a:extLst>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1000" b="0">
-              <a:solidFill>
-                <a:srgbClr val="154E54"/>
-              </a:solidFill>
-              <a:latin typeface="Eras Medium ITC"/>
-            </a:rPr>
-            <a:t>Forename</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>701675</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>454025</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="" fLocksText="0">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="916" name="TextBox 915"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3302000" y="1270000"/>
-          <a:ext cx="1524000" cy="254000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100"/>
-            <a:t>Julian</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>708025</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>165100</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="" fLocksText="0">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="917" name="TextBox 916"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5080000" y="1270000"/>
-          <a:ext cx="952500" cy="254000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:gradFill flip="none" rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:srgbClr val="FFFFFF"/>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:srgbClr val="FFFFFF"/>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="1"/>
-          <a:tileRect/>
-        </a:gradFill>
-        <a:ln w="0" cmpd="sng">
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-        <a:extLst>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1000" b="0">
-              <a:solidFill>
-                <a:srgbClr val="154E54"/>
-              </a:solidFill>
-              <a:latin typeface="Eras Medium ITC"/>
-            </a:rPr>
-            <a:t>Surname</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>165100</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>1689100</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="" fLocksText="0">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="918" name="TextBox 917"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6032500" y="1270000"/>
-          <a:ext cx="1524000" cy="254000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100"/>
-            <a:t>Turner</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>1130300</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>701675</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="" fLocksText="0">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="919" name="TextBox 918"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2349500" y="1778000"/>
-          <a:ext cx="952500" cy="254000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:gradFill flip="none" rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:srgbClr val="FFFFFF"/>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:srgbClr val="FFFFFF"/>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="1"/>
-          <a:tileRect/>
-        </a:gradFill>
-        <a:ln w="0" cmpd="sng">
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-        <a:extLst>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1000" b="0">
-              <a:solidFill>
-                <a:srgbClr val="154E54"/>
-              </a:solidFill>
-              <a:latin typeface="Eras Medium ITC"/>
-            </a:rPr>
-            <a:t>Role</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>701675</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>454025</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="" fLocksText="0">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="920" name="TextBox 919"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3302000" y="1778000"/>
-          <a:ext cx="1524000" cy="254000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100"/>
-            <a:t>Crew Manager Competent (Operator)</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>708025</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>165100</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="" fLocksText="0">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="921" name="TextBox 920"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5080000" y="762000"/>
-          <a:ext cx="952500" cy="254000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:gradFill flip="none" rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:srgbClr val="FFFFFF"/>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:srgbClr val="FFFFFF"/>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="1"/>
-          <a:tileRect/>
-        </a:gradFill>
-        <a:ln w="0" cmpd="sng">
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-        <a:extLst>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1000" b="0">
-              <a:solidFill>
-                <a:srgbClr val="154E54"/>
-              </a:solidFill>
-              <a:latin typeface="Eras Medium ITC"/>
-            </a:rPr>
-            <a:t>Rank / Grade</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>165100</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>1689100</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="" fLocksText="0">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="922" name="TextBox 921"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6032500" y="762000"/>
-          <a:ext cx="1524000" cy="254000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100"/>
-            <a:t>Crew Manager</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>1130300</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>701675</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="" fLocksText="0">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="923" name="TextBox 922"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2349500" y="2286000"/>
-          <a:ext cx="952500" cy="254000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:gradFill flip="none" rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:srgbClr val="FFFFFF"/>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:srgbClr val="FFFFFF"/>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="1"/>
-          <a:tileRect/>
-        </a:gradFill>
-        <a:ln w="0" cmpd="sng">
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-        <a:extLst>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1000" b="0">
-              <a:solidFill>
-                <a:srgbClr val="154E54"/>
-              </a:solidFill>
-              <a:latin typeface="Eras Medium ITC"/>
-            </a:rPr>
-            <a:t>Location</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>708025</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>165100</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="" fLocksText="0">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="926" name="TextBox 925"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5080000" y="2286000"/>
-          <a:ext cx="952500" cy="254000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:gradFill flip="none" rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:srgbClr val="FFFFFF"/>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:srgbClr val="FFFFFF"/>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="1"/>
-          <a:tileRect/>
-        </a:gradFill>
-        <a:ln w="0" cmpd="sng">
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-        <a:extLst>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1000" b="0">
-              <a:solidFill>
-                <a:srgbClr val="154E54"/>
-              </a:solidFill>
-              <a:latin typeface="Eras Medium ITC"/>
-            </a:rPr>
-            <a:t>Watch</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>165100</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>1689100</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="" fLocksText="0">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="927" name="TextBox 926"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6032500" y="2286000"/>
-          <a:ext cx="1524000" cy="254000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:endParaRPr lang="en-GB" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>708025</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>165100</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="" fLocksText="0">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="33" name="TextBox 32"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5080000" y="1778000"/>
-          <a:ext cx="952500" cy="254000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:gradFill flip="none" rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:srgbClr val="FFFFFF"/>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:srgbClr val="FFFFFF"/>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="1"/>
-          <a:tileRect/>
-        </a:gradFill>
-        <a:ln w="0" cmpd="sng">
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-        <a:extLst>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1000" b="0">
-              <a:solidFill>
-                <a:srgbClr val="154E54"/>
-              </a:solidFill>
-              <a:latin typeface="Eras Medium ITC"/>
-            </a:rPr>
-            <a:t>Access Level</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>165100</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>1689100</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="" fLocksText="0">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="35" name="TextBox 34"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6032500" y="1778000"/>
-          <a:ext cx="1524000" cy="254000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100"/>
-            <a:t>4</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>701675</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>454025</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="924" name="TextBox 923"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3302000" y="2286000"/>
-          <a:ext cx="1524000" cy="254000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100"/>
-            <a:t>Brant Broughton</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>828675</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>91623</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>67800</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="112" name="DropDown"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3429000" y="2400300"/>
-          <a:ext cx="148773" cy="144000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
     </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>1689100</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="'ModUISupportScreen.ProcessBtnPress(8)'" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="912" name="BtnUpdate"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6286500" y="2794000"/>
-          <a:ext cx="1270000" cy="317500"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:gradFill flip="none" rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:srgbClr val="FFCC00"/>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:srgbClr val="FFA634"/>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="1"/>
-          <a:tileRect/>
-        </a:gradFill>
-        <a:ln w="0" cap="flat" cmpd="sng" algn="ctr">
-          <a:noFill/>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst>
-          <a:outerShdw blurRad="63500" dist="37357" dir="2700000" rotWithShape="0">
-            <a:prstClr val="black">
-              <a:alpha val="40000"/>
-            </a:prstClr>
-          </a:outerShdw>
-        </a:effectLst>
-        <a:extLst>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:prstDash val="solid"/>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1200" b="0">
-              <a:solidFill>
-                <a:srgbClr val="322924"/>
-              </a:solidFill>
-              <a:latin typeface="Eras Medium ITC"/>
-            </a:rPr>
-            <a:t>Update</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -17282,6 +14808,130 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Rectangle 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3924300" y="809625"/>
+          <a:ext cx="2781300" cy="2428875"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Isosceles Triangle 2"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000">
+          <a:off x="3924300" y="2028825"/>
+          <a:ext cx="1962150" cy="1219200"/>
+        </a:xfrm>
+        <a:prstGeom prst="triangle">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
@@ -23312,11 +20962,9 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="ShtMain"/>
-  <dimension ref="B4:P28"/>
+  <dimension ref="C4:P28"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q11" sqref="Q11"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -23331,7 +20979,7 @@
     <col min="11" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
@@ -23339,7 +20987,7 @@
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -23347,61 +20995,55 @@
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B9" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C15" s="3"/>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C16" s="3"/>
     </row>
     <row r="23" spans="12:16" x14ac:dyDescent="0.25">
-      <c r="L23" s="59"/>
-      <c r="M23" s="59"/>
-      <c r="N23" s="59"/>
-      <c r="O23" s="59"/>
-      <c r="P23" s="59"/>
+      <c r="L23" s="60"/>
+      <c r="M23" s="60"/>
+      <c r="N23" s="60"/>
+      <c r="O23" s="60"/>
+      <c r="P23" s="60"/>
     </row>
     <row r="24" spans="12:16" x14ac:dyDescent="0.25">
-      <c r="L24" s="59"/>
-      <c r="M24" s="59"/>
-      <c r="N24" s="59"/>
-      <c r="O24" s="59"/>
-      <c r="P24" s="59"/>
+      <c r="L24" s="60"/>
+      <c r="M24" s="60"/>
+      <c r="N24" s="60"/>
+      <c r="O24" s="60"/>
+      <c r="P24" s="60"/>
     </row>
     <row r="25" spans="12:16" x14ac:dyDescent="0.25">
-      <c r="L25" s="59"/>
-      <c r="M25" s="59"/>
-      <c r="N25" s="59"/>
-      <c r="O25" s="59"/>
-      <c r="P25" s="59"/>
+      <c r="L25" s="60"/>
+      <c r="M25" s="60"/>
+      <c r="N25" s="60"/>
+      <c r="O25" s="60"/>
+      <c r="P25" s="60"/>
     </row>
     <row r="26" spans="12:16" x14ac:dyDescent="0.25">
-      <c r="L26" s="59"/>
-      <c r="M26" s="59"/>
-      <c r="N26" s="59"/>
-      <c r="O26" s="59"/>
-      <c r="P26" s="59"/>
+      <c r="L26" s="60"/>
+      <c r="M26" s="60"/>
+      <c r="N26" s="60"/>
+      <c r="O26" s="60"/>
+      <c r="P26" s="60"/>
     </row>
     <row r="27" spans="12:16" x14ac:dyDescent="0.25">
-      <c r="L27" s="59"/>
-      <c r="M27" s="59"/>
-      <c r="N27" s="59"/>
-      <c r="O27" s="59"/>
-      <c r="P27" s="59"/>
+      <c r="L27" s="60"/>
+      <c r="M27" s="60"/>
+      <c r="N27" s="60"/>
+      <c r="O27" s="60"/>
+      <c r="P27" s="60"/>
     </row>
     <row r="28" spans="12:16" x14ac:dyDescent="0.25">
-      <c r="L28" s="59"/>
-      <c r="M28" s="59"/>
-      <c r="N28" s="59"/>
-      <c r="O28" s="59"/>
-      <c r="P28" s="59"/>
+      <c r="L28" s="60"/>
+      <c r="M28" s="60"/>
+      <c r="N28" s="60"/>
+      <c r="O28" s="60"/>
+      <c r="P28" s="60"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <dataConsolidate/>
   <mergeCells count="1">
     <mergeCell ref="L23:P28"/>
@@ -23420,10 +21062,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="ShtSettings"/>
-  <dimension ref="B2:L28"/>
+  <dimension ref="B1:L28"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23437,7 +21079,11 @@
     <col min="12" max="12" width="9.140625" style="6"/>
   </cols>
   <sheetData>
+    <row r="1" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C1" s="59"/>
+    </row>
     <row r="2" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C2" s="59"/>
       <c r="D2" s="4"/>
       <c r="E2" t="s">
         <v>0</v>
@@ -37705,17 +35351,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="60" t="s">
+      <c r="B1" s="61" t="s">
         <v>1919</v>
       </c>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
-      <c r="F1" s="60"/>
-      <c r="G1" s="60"/>
-      <c r="H1" s="60"/>
-      <c r="I1" s="60"/>
-      <c r="J1" s="60"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="61"/>
+      <c r="G1" s="61"/>
+      <c r="H1" s="61"/>
+      <c r="I1" s="61"/>
+      <c r="J1" s="61"/>
     </row>
     <row r="3" spans="2:11" s="55" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="56" t="s">
@@ -37746,12 +35392,12 @@
     </row>
     <row r="4" spans="2:11" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="2:11" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="61" t="s">
+      <c r="B5" s="62" t="s">
         <v>1915</v>
       </c>
-      <c r="C5" s="62"/>
-      <c r="D5" s="62"/>
-      <c r="E5" s="63"/>
+      <c r="C5" s="63"/>
+      <c r="D5" s="63"/>
+      <c r="E5" s="64"/>
       <c r="F5" s="37" t="s">
         <v>1916</v>
       </c>
@@ -38829,7 +36475,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="5152" r:id="rId24" name="Check Box 32">
+            <control shapeId="5152" r:id="rId24" name="$H$15">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -38851,7 +36497,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="5153" r:id="rId25" name="Check Box 33">
+            <control shapeId="5153" r:id="rId25" name="$H$16">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -38873,7 +36519,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="5154" r:id="rId26" name="Check Box 34">
+            <control shapeId="5154" r:id="rId26" name="$H$17">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -38895,7 +36541,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="5155" r:id="rId27" name="Check Box 35">
+            <control shapeId="5155" r:id="rId27" name="$H$18">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -38917,7 +36563,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="5156" r:id="rId28" name="Check Box 36">
+            <control shapeId="5156" r:id="rId28" name="$H$19">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -38939,7 +36585,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="5157" r:id="rId29" name="Check Box 37">
+            <control shapeId="5157" r:id="rId29" name="$H$20">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -38961,7 +36607,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="5158" r:id="rId30" name="Check Box 38">
+            <control shapeId="5158" r:id="rId30" name="$H$21">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -38983,7 +36629,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="5159" r:id="rId31" name="Check Box 39">
+            <control shapeId="5159" r:id="rId31" name="$H$22">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -39005,7 +36651,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="5160" r:id="rId32" name="Check Box 40">
+            <control shapeId="5160" r:id="rId32" name="$H$23">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -39027,7 +36673,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="5161" r:id="rId33" name="Check Box 41">
+            <control shapeId="5161" r:id="rId33" name="$H$24">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -39049,7 +36695,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="5162" r:id="rId34" name="Check Box 42">
+            <control shapeId="5162" r:id="rId34" name="$H$25">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -39161,4 +36807,20 @@
     </mc:Choice>
   </mc:AlternateContent>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O22" sqref="O22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added Release Notes Tweaked message Added date changed frame size
</commit_message>
<xml_diff>
--- a/Stores IT System v0.xlsx
+++ b/Stores IT System v0.xlsx
@@ -9171,9 +9171,6 @@
     <t>Date</t>
   </si>
   <si>
-    <t>\\lincsfire.lincolnshire.gov.uk\folderredir$\Documents\julian.turner\Documents\RDS Project\Stores IT Project\Database\Stores IT System Dev DB v0,38.accdb</t>
-  </si>
-  <si>
     <t>Return Req'd</t>
   </si>
   <si>
@@ -9187,6 +9184,9 @@
   </si>
   <si>
     <t>Leverton (BV57GNK)</t>
+  </si>
+  <si>
+    <t>\\lincsfire.lincolnshire.gov.uk\folderredir$\Documents\julian.turner\Documents\RDS Project\Stores IT Project\Database\Stores IT System Dev DB v0,391.accdb</t>
   </si>
 </sst>
 </file>
@@ -20896,7 +20896,7 @@
         <v>45</v>
       </c>
       <c r="J28" t="s">
-        <v>3033</v>
+        <v>3038</v>
       </c>
     </row>
   </sheetData>
@@ -20915,8 +20915,33 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2049" r:id="rId5" name="BtnDBConnect">
+        <control shapeId="2052" r:id="rId5" name="CommandButton1">
           <controlPr defaultSize="0" autoLine="0" r:id="rId6">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>904875</xdr:colOff>
+                <xdr:row>18</xdr:row>
+                <xdr:rowOff>76200</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>19</xdr:row>
+                <xdr:rowOff>152400</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2052" r:id="rId5" name="CommandButton1"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2049" r:id="rId7" name="BtnDBConnect">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId8">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>6</xdr:col>
@@ -20935,32 +20960,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2049" r:id="rId5" name="BtnDBConnect"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2052" r:id="rId7" name="CommandButton1">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId8">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>904875</xdr:colOff>
-                <xdr:row>18</xdr:row>
-                <xdr:rowOff>76200</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>19</xdr:row>
-                <xdr:rowOff>152400</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2052" r:id="rId7" name="CommandButton1"/>
+        <control shapeId="2049" r:id="rId7" name="BtnDBConnect"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -34385,7 +34385,7 @@
         <v>1894</v>
       </c>
       <c r="J3" s="49" t="s">
-        <v>3036</v>
+        <v>3035</v>
       </c>
       <c r="K3" s="49"/>
     </row>
@@ -34413,7 +34413,7 @@
         <v>1904</v>
       </c>
       <c r="K5" s="42" t="s">
-        <v>3034</v>
+        <v>3033</v>
       </c>
       <c r="L5" s="30" t="b">
         <v>1</v>
@@ -34433,7 +34433,7 @@
       <c r="H6" s="33"/>
       <c r="I6" s="34"/>
       <c r="J6" s="34" t="s">
-        <v>3037</v>
+        <v>3036</v>
       </c>
       <c r="K6" s="34"/>
       <c r="L6" s="35" t="b">
@@ -34454,10 +34454,10 @@
       <c r="H7" s="38"/>
       <c r="I7" s="39"/>
       <c r="J7" s="39" t="s">
-        <v>3038</v>
+        <v>3037</v>
       </c>
       <c r="K7" s="39" t="s">
-        <v>3035</v>
+        <v>3034</v>
       </c>
       <c r="L7" s="40"/>
     </row>

</xml_diff>

<commit_message>
Return Flag Fix changed Clear Range to include all columns
</commit_message>
<xml_diff>
--- a/Stores IT System v0.xlsx
+++ b/Stores IT System v0.xlsx
@@ -56,7 +56,7 @@
     <definedName name="NoWeeks">#REF!</definedName>
     <definedName name="PencilGraphData">[1]Test!#REF!</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="3">'Order List'!$B$1:$L$39</definedName>
-    <definedName name="RngClear">'Order List'!$C$3,'Order List'!$H$3,'Order List'!$J$3,'Order List'!$B$6:$J$39</definedName>
+    <definedName name="RngClear">'Order List'!$C$3,'Order List'!$H$3,'Order List'!$J$3,'Order List'!$B$6:$K$39</definedName>
     <definedName name="Role">#REF!</definedName>
     <definedName name="StationLookUp">[1]Lists!$A$1:$C$38</definedName>
     <definedName name="StationName">'[1]Station Detail'!$AG$4</definedName>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3206" uniqueCount="3039">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3205" uniqueCount="3039">
   <si>
     <t>Colour 1</t>
   </si>
@@ -9177,16 +9177,16 @@
     <t>Yes</t>
   </si>
   <si>
-    <t>Leverton</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ()</t>
-  </si>
-  <si>
-    <t>Leverton (BV57GNK)</t>
-  </si>
-  <si>
     <t>\\lincsfire.lincolnshire.gov.uk\folderredir$\Documents\julian.turner\Documents\RDS Project\Stores IT Project\Database\Stores IT System Dev DB v0,391.accdb</t>
+  </si>
+  <si>
+    <t>Louth</t>
+  </si>
+  <si>
+    <t>Large</t>
+  </si>
+  <si>
+    <t>Louth (Paul Gale)</t>
   </si>
 </sst>
 </file>
@@ -20896,7 +20896,7 @@
         <v>45</v>
       </c>
       <c r="J28" t="s">
-        <v>3038</v>
+        <v>3035</v>
       </c>
     </row>
   </sheetData>
@@ -20915,8 +20915,33 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2052" r:id="rId5" name="CommandButton1">
+        <control shapeId="2049" r:id="rId5" name="BtnDBConnect">
           <controlPr defaultSize="0" autoLine="0" r:id="rId6">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>24</xdr:row>
+                <xdr:rowOff>180975</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>26</xdr:row>
+                <xdr:rowOff>76200</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2049" r:id="rId5" name="BtnDBConnect"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2052" r:id="rId7" name="CommandButton1">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId8">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
@@ -20935,32 +20960,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2052" r:id="rId5" name="CommandButton1"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2049" r:id="rId7" name="BtnDBConnect">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId8">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>24</xdr:row>
-                <xdr:rowOff>180975</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>26</xdr:row>
-                <xdr:rowOff>76200</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2049" r:id="rId7" name="BtnDBConnect"/>
+        <control shapeId="2052" r:id="rId7" name="CommandButton1"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -34328,7 +34328,7 @@
   <dimension ref="B1:L39"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="26.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -34366,26 +34366,26 @@
         <v>1893</v>
       </c>
       <c r="C3" s="45">
-        <v>481</v>
+        <v>1645</v>
       </c>
       <c r="D3" s="48" t="s">
         <v>3032</v>
       </c>
       <c r="E3" s="50">
-        <v>42902</v>
+        <v>43045</v>
       </c>
       <c r="F3" s="45"/>
       <c r="G3" s="48" t="s">
         <v>1906</v>
       </c>
       <c r="H3" s="45" t="s">
-        <v>1614</v>
+        <v>1539</v>
       </c>
       <c r="I3" s="46" t="s">
         <v>1894</v>
       </c>
       <c r="J3" s="49" t="s">
-        <v>3035</v>
+        <v>3036</v>
       </c>
       <c r="K3" s="49"/>
     </row>
@@ -34421,7 +34421,7 @@
     </row>
     <row r="6" spans="2:12" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="31" t="s">
-        <v>2349</v>
+        <v>1910</v>
       </c>
       <c r="C6" s="43"/>
       <c r="D6" s="43"/>
@@ -34429,36 +34429,32 @@
       <c r="F6" s="33">
         <v>1</v>
       </c>
-      <c r="G6" s="33"/>
+      <c r="G6" s="33" t="s">
+        <v>3037</v>
+      </c>
       <c r="H6" s="33"/>
       <c r="I6" s="34"/>
       <c r="J6" s="34" t="s">
-        <v>3036</v>
-      </c>
-      <c r="K6" s="34"/>
+        <v>3038</v>
+      </c>
+      <c r="K6" s="34" t="s">
+        <v>3034</v>
+      </c>
       <c r="L6" s="35" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="2:12" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="36" t="s">
-        <v>525</v>
-      </c>
+      <c r="B7" s="36"/>
       <c r="C7" s="44"/>
       <c r="D7" s="44"/>
       <c r="E7" s="37"/>
-      <c r="F7" s="38">
-        <v>1</v>
-      </c>
+      <c r="F7" s="38"/>
       <c r="G7" s="38"/>
       <c r="H7" s="38"/>
       <c r="I7" s="39"/>
-      <c r="J7" s="39" t="s">
-        <v>3037</v>
-      </c>
-      <c r="K7" s="39" t="s">
-        <v>3034</v>
-      </c>
+      <c r="J7" s="39"/>
+      <c r="K7" s="39"/>
       <c r="L7" s="40"/>
     </row>
     <row r="8" spans="2:12" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added Purchase Unit to Print Order Form
</commit_message>
<xml_diff>
--- a/Stores IT System v0.xlsx
+++ b/Stores IT System v0.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Julian\Documents\StoresOrderingSystem\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="21075" windowHeight="9975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="21075" windowHeight="9975"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="4" r:id="rId1"/>
@@ -74,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3227" uniqueCount="3056">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3241" uniqueCount="3067">
   <si>
     <t>Colour 1</t>
   </si>
@@ -9121,21 +9116,6 @@
     <t>Return Req'd</t>
   </si>
   <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>Louth</t>
-  </si>
-  <si>
-    <t>Large</t>
-  </si>
-  <si>
-    <t>Louth (Paul Gale)</t>
-  </si>
-  <si>
-    <t>C:\Users\Julian\OneDrive\RDS Project\Stores IT Project\Database\Stores IT System Dev DB v0,393.accdb</t>
-  </si>
-  <si>
     <t>Pete Green</t>
   </si>
   <si>
@@ -9242,12 +9222,60 @@
   </si>
   <si>
     <t>Julian</t>
+  </si>
+  <si>
+    <t>\\lincsfire.lincolnshire.gov.uk\folderredir$\Documents\julian.turner\Documents\RDS Project\Stores IT Project\Database\Stores IT System Dev DB v0,396.accdb</t>
+  </si>
+  <si>
+    <t>Horncastle</t>
+  </si>
+  <si>
+    <t>Patient Report Form (Each)</t>
+  </si>
+  <si>
+    <t>F17</t>
+  </si>
+  <si>
+    <t>Horncastle (Michael Baumber)</t>
+  </si>
+  <si>
+    <t>Hot Pack Food (Box)</t>
+  </si>
+  <si>
+    <t>Box</t>
+  </si>
+  <si>
+    <t>E01</t>
+  </si>
+  <si>
+    <t>Horncastle (WX14ZKE)</t>
+  </si>
+  <si>
+    <t>Water bottled (Case of 24)</t>
+  </si>
+  <si>
+    <t>A00</t>
+  </si>
+  <si>
+    <t>Sugar - Sachets (Pack of 100)</t>
+  </si>
+  <si>
+    <t>Pack of 100</t>
+  </si>
+  <si>
+    <t>E03</t>
+  </si>
+  <si>
+    <t>Tea - Tube (24 pack) (24 Pack)</t>
+  </si>
+  <si>
+    <t>24 pack</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0000"/>
     <numFmt numFmtId="165" formatCode="dd\ mmm\ yy"/>
@@ -9803,8 +9831,8 @@
   <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="Percent 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Percent 2" xfId="2"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -10080,7 +10108,7 @@
         <xdr:cNvPr id="5" name="TEMPLATE - Icon_Alocations">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10840,7 +10868,7 @@
         <xdr:cNvPr id="7" name="TEMPLATE - Icon_Left_Frame">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10884,7 +10912,7 @@
         <xdr:cNvPr id="8" name="TEMPLATE - Icon_Right_Frame">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10928,7 +10956,7 @@
         <xdr:cNvPr id="9" name="TEMPLATE - Icon_New_Order">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000009000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10983,7 +11011,7 @@
         <xdr:cNvPr id="11" name="TEMPLATE - Message">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000B000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11032,7 +11060,7 @@
         <xdr:cNvPr id="12" name="TEMPLATE - Orders">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000C000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11081,7 +11109,7 @@
         <xdr:cNvPr id="120" name="TEMPLATE - Delivery">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000078000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000078000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11125,7 +11153,7 @@
         <xdr:cNvPr id="121" name="TEMPLATE - Phone">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000079000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000079000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11169,7 +11197,7 @@
         <xdr:cNvPr id="122" name="TEMPLATE - Closed Orders">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00007A000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00007A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11213,7 +11241,7 @@
         <xdr:cNvPr id="123" name="TEMPLATE - User">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00007B000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00007B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11257,7 +11285,7 @@
         <xdr:cNvPr id="124" name="TEMPLATE - DataManage">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00007C000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00007C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11312,7 +11340,7 @@
         <xdr:cNvPr id="925" name="TEMPLATE - FindOrder">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00009D030000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00009D030000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11356,7 +11384,7 @@
         <xdr:cNvPr id="38" name="TEMPLATE - Icon_Station">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000026000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000026000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11411,7 +11439,7 @@
         <xdr:cNvPr id="202" name="TEMPLATE - Icon_Stores">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-0000CA000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-0000CA000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11465,7 +11493,7 @@
         <xdr:cNvPr id="1335" name="TEMPLATE - Icon_Document">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000037050000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000037050000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11520,7 +11548,7 @@
         <xdr:cNvPr id="1424" name="TEMPLATE - Icon_Head">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000090050000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000090050000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11575,7 +11603,7 @@
         <xdr:cNvPr id="1510" name="TEMPLATE - Icon_Support">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-0000E6050000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-0000E6050000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11629,7 +11657,7 @@
         <xdr:cNvPr id="1596" name="TEMPLATE - Exit">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003C060000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00003C060000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11684,7 +11712,7 @@
         <xdr:cNvPr id="1409" name="TEMPLATE - Settings">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000081050000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000081050000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11734,7 +11762,7 @@
         <xdr:cNvPr id="88" name="TEMPLATE - Graph">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000058000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000058000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11793,14 +11821,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s2049"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000001080000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -11808,20 +11833,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:noFill/>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -11851,14 +11862,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s2050"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002080000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -11866,29 +11874,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
             <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
@@ -11938,14 +11923,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s2051"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003080000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -11953,29 +11935,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
             <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
@@ -12025,14 +11984,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s2052"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000004080000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -12040,20 +11996,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:noFill/>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -12083,14 +12025,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s2053"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000005080000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -12098,29 +12037,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="1">
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -12150,14 +12066,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s2054"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000006080000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -12165,29 +12078,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="1">
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -12217,14 +12107,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s2055"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000007080000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -12232,29 +12119,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="1">
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -12284,14 +12148,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s2056"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000008080000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -12299,29 +12160,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="1">
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -12351,14 +12189,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s2057"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000009080000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -12366,29 +12201,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="1">
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -12418,14 +12230,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s2058"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000A080000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -12433,29 +12242,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="1">
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -12485,14 +12271,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s2059"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000B080000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -12500,29 +12283,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="1">
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -12552,14 +12312,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s2060"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000C080000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -12567,29 +12324,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="1">
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -12619,14 +12353,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s2061"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000D080000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -12634,29 +12365,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="1">
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -12686,14 +12394,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s2062"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000E080000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -12701,29 +12406,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="1">
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -12753,14 +12435,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s2063"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000F080000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -12768,29 +12447,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="1">
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -12820,14 +12476,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s2064"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000010080000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -12835,29 +12488,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="1">
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -12887,14 +12517,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s2065"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000011080000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -12902,29 +12529,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="1">
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -12954,14 +12558,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s2066"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000012080000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -12969,29 +12570,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="1">
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -13021,14 +12599,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s2067"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000013080000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -13036,29 +12611,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="1">
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -13084,7 +12636,7 @@
         <xdr:cNvPr id="21" name="Rectangle 20">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000015000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000015000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -13144,7 +12696,7 @@
         <xdr:cNvPr id="22" name="Rectangle 21">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000016000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000016000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -13204,7 +12756,7 @@
         <xdr:cNvPr id="23" name="Rectangle 22">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000017000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000017000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -13264,7 +12816,7 @@
         <xdr:cNvPr id="24" name="Rectangle 23">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000018000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000018000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -13324,7 +12876,7 @@
         <xdr:cNvPr id="25" name="Rectangle 24">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000019000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000019000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -13384,7 +12936,7 @@
         <xdr:cNvPr id="26" name="Rectangle 25">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00001A000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00001A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -13444,7 +12996,7 @@
         <xdr:cNvPr id="27" name="Rectangle 26">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00001B000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00001B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -13504,7 +13056,7 @@
         <xdr:cNvPr id="28" name="Rectangle 27">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00001C000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00001C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -13564,7 +13116,7 @@
         <xdr:cNvPr id="29" name="Rectangle 28">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00001D000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00001D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -13624,7 +13176,7 @@
         <xdr:cNvPr id="30" name="Rectangle 29">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00001E000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00001E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -13684,7 +13236,7 @@
         <xdr:cNvPr id="31" name="Rectangle 30">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00001F000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00001F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -13744,7 +13296,7 @@
         <xdr:cNvPr id="32" name="Rectangle 31" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000020000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000020000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -13804,7 +13356,7 @@
         <xdr:cNvPr id="33" name="Rectangle 32">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000021000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000021000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -13873,14 +13425,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s5121"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000001140000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -13888,29 +13437,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="1">
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -13940,14 +13466,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s5122"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002140000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -13955,29 +13478,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="1">
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -14007,14 +13507,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s5123"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003140000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -14022,29 +13519,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="1">
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -14074,14 +13548,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s5124"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000004140000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -14089,29 +13560,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="1">
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -14141,14 +13589,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s5125"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000005140000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -14156,29 +13601,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="1">
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -14208,14 +13630,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s5126"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000006140000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -14223,29 +13642,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="1">
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -14275,14 +13671,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s5127"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000007140000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -14290,29 +13683,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="1">
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -14342,14 +13712,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s5128"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000008140000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -14357,29 +13724,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="1">
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -14409,14 +13753,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s5129"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000009140000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -14424,29 +13765,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="1">
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -14476,14 +13794,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s5130"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000A140000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -14491,29 +13806,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="1">
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -14543,14 +13835,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s5131"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000B140000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -14558,29 +13847,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="1">
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -14610,14 +13876,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s5132"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000C140000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -14625,29 +13888,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="1">
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -14677,14 +13917,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s5133"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000D140000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -14692,29 +13929,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="1">
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -14744,14 +13958,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s5134"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000E140000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -14759,29 +13970,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="1">
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -14811,14 +13999,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s5135"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000F140000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -14826,29 +14011,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="1">
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -14878,14 +14040,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s5136"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000010140000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -14893,29 +14052,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="1">
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -14945,14 +14081,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s5137"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000011140000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -14960,29 +14093,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="1">
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -15012,14 +14122,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s5138"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000012140000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -15027,29 +14134,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="1">
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -15079,14 +14163,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s5139"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000013140000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -15094,29 +14175,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="1">
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -15146,14 +14204,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s5140"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000014140000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -15161,29 +14216,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="1">
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -15213,14 +14245,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s5152"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000020140000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -15228,29 +14257,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="1">
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -15280,14 +14286,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s5153"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000021140000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -15295,29 +14298,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="1">
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -15347,14 +14327,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s5154"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000022140000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -15362,29 +14339,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="1">
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -15414,14 +14368,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s5155"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000023140000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -15429,29 +14380,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="1">
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -15481,14 +14409,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s5156"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000024140000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -15496,29 +14421,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="1">
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -15548,14 +14450,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s5157"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000025140000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -15563,29 +14462,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="1">
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -15615,14 +14491,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s5158"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000026140000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -15630,29 +14503,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="1">
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -15682,14 +14532,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s5159"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000027140000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -15697,29 +14544,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="1">
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -15749,14 +14573,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s5160"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000028140000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -15764,29 +14585,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="1">
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -15816,14 +14614,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s5161"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000029140000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -15831,29 +14626,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="1">
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -15883,14 +14655,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s5162"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00002A140000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -15898,29 +14667,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="1">
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -15950,14 +14696,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s5163"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00002B140000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -15965,29 +14708,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="1">
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -16017,14 +14737,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s5164"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00002C140000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -16032,29 +14749,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="1">
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -16084,14 +14778,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s5165"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00002D140000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -16099,29 +14790,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="1">
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -16151,14 +14819,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s5166"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00002E140000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -16166,29 +14831,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="1">
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -16475,7 +15117,7 @@
             <v>8.25</v>
           </cell>
           <cell r="AC4">
-            <v>158.48336791992188</v>
+            <v>158.48336791992187</v>
           </cell>
           <cell r="AD4">
             <v>0</v>
@@ -16514,7 +15156,7 @@
             <v>17.016651153564453</v>
           </cell>
           <cell r="AR4">
-            <v>502.45004272460938</v>
+            <v>502.45004272460937</v>
           </cell>
           <cell r="AS4">
             <v>39.899993896484375</v>
@@ -16707,7 +15349,7 @@
             <v>16.566673278808594</v>
           </cell>
           <cell r="M6">
-            <v>37.133316040039063</v>
+            <v>37.133316040039062</v>
           </cell>
           <cell r="N6">
             <v>28.633323669433594</v>
@@ -16755,7 +15397,7 @@
             <v>14.299995422363281</v>
           </cell>
           <cell r="AE6">
-            <v>36.083328247070313</v>
+            <v>36.083328247070312</v>
           </cell>
           <cell r="AF6">
             <v>4863.58349609375</v>
@@ -16931,13 +15573,13 @@
             <v>3.5</v>
           </cell>
           <cell r="AT7">
-            <v>24.766708374023438</v>
+            <v>24.766708374023437</v>
           </cell>
           <cell r="AU7">
             <v>0</v>
           </cell>
           <cell r="AV7">
-            <v>2.6999740600585938</v>
+            <v>2.6999740600585937</v>
           </cell>
           <cell r="AW7">
             <v>3833.18310546875</v>
@@ -16975,10 +15617,10 @@
             <v>538.416748046875</v>
           </cell>
           <cell r="K8">
-            <v>39.666610717773438</v>
+            <v>39.666610717773437</v>
           </cell>
           <cell r="L8">
-            <v>177.83328247070313</v>
+            <v>177.83328247070312</v>
           </cell>
           <cell r="M8">
             <v>3.75</v>
@@ -17243,13 +15885,13 @@
             <v>6</v>
           </cell>
           <cell r="I10">
-            <v>210.38339233398438</v>
+            <v>210.38339233398437</v>
           </cell>
           <cell r="J10">
             <v>492.18341064453125</v>
           </cell>
           <cell r="K10">
-            <v>20.616683959960938</v>
+            <v>20.616683959960937</v>
           </cell>
           <cell r="L10">
             <v>190.29994201660156</v>
@@ -17297,7 +15939,7 @@
             <v>4.1666717529296875</v>
           </cell>
           <cell r="AC10">
-            <v>119.08328247070313</v>
+            <v>119.08328247070312</v>
           </cell>
           <cell r="AD10">
             <v>0</v>
@@ -17339,7 +15981,7 @@
             <v>564.9500732421875</v>
           </cell>
           <cell r="AS10">
-            <v>10.433334350585938</v>
+            <v>10.433334350585937</v>
           </cell>
           <cell r="AT10">
             <v>179.04991149902344</v>
@@ -17937,7 +16579,7 @@
             <v>22.683364868164063</v>
           </cell>
           <cell r="L15">
-            <v>41.599990844726563</v>
+            <v>41.599990844726562</v>
           </cell>
           <cell r="M15">
             <v>0</v>
@@ -18485,7 +17127,7 @@
             <v>5.13336181640625</v>
           </cell>
           <cell r="L19">
-            <v>199.20004272460938</v>
+            <v>199.20004272460937</v>
           </cell>
           <cell r="M19">
             <v>0</v>
@@ -18530,10 +17172,10 @@
             <v>29.550079345703125</v>
           </cell>
           <cell r="AC19">
-            <v>148.91665649414063</v>
+            <v>148.91665649414062</v>
           </cell>
           <cell r="AD19">
-            <v>6.5833358764648438</v>
+            <v>6.5833358764648437</v>
           </cell>
           <cell r="AE19">
             <v>34.283424377441406</v>
@@ -18673,7 +17315,7 @@
             <v>0</v>
           </cell>
           <cell r="AE20">
-            <v>18.166641235351563</v>
+            <v>18.166641235351562</v>
           </cell>
           <cell r="AF20">
             <v>4593.93310546875</v>
@@ -18899,7 +17541,7 @@
             <v>77.116676330566406</v>
           </cell>
           <cell r="M22">
-            <v>4.5833206176757813</v>
+            <v>4.5833206176757812</v>
           </cell>
           <cell r="N22">
             <v>26.5</v>
@@ -19123,7 +17765,7 @@
             <v>3.98333740234375</v>
           </cell>
           <cell r="AT23">
-            <v>23.466690063476563</v>
+            <v>23.466690063476562</v>
           </cell>
           <cell r="AU23">
             <v>29.766647338867188</v>
@@ -19170,7 +17812,7 @@
             <v>6.6650390625E-2</v>
           </cell>
           <cell r="L24">
-            <v>29.383377075195313</v>
+            <v>29.383377075195312</v>
           </cell>
           <cell r="M24">
             <v>0</v>
@@ -19251,7 +17893,7 @@
             <v>12</v>
           </cell>
           <cell r="AQ24">
-            <v>39.433303833007813</v>
+            <v>39.433303833007812</v>
           </cell>
           <cell r="AR24">
             <v>741.24993896484375</v>
@@ -19531,10 +18173,10 @@
             <v>734.13330078125</v>
           </cell>
           <cell r="AS26">
-            <v>9.5999832153320313</v>
+            <v>9.5999832153320312</v>
           </cell>
           <cell r="AT26">
-            <v>9.8667068481445313</v>
+            <v>9.8667068481445312</v>
           </cell>
           <cell r="AU26">
             <v>0</v>
@@ -19632,7 +18274,7 @@
             <v>1.25</v>
           </cell>
           <cell r="AE27">
-            <v>7.9999771118164063</v>
+            <v>7.9999771118164062</v>
           </cell>
           <cell r="AF27">
             <v>4070.650146484375</v>
@@ -19718,7 +18360,7 @@
             <v>0</v>
           </cell>
           <cell r="L28">
-            <v>34.666702270507813</v>
+            <v>34.666702270507812</v>
           </cell>
           <cell r="M28">
             <v>0.75</v>
@@ -20263,7 +18905,7 @@
             <v>555.4666748046875</v>
           </cell>
           <cell r="K32">
-            <v>19.033340454101563</v>
+            <v>19.033340454101562</v>
           </cell>
           <cell r="L32">
             <v>118.48329162597656</v>
@@ -20493,7 +19135,7 @@
             <v>16.683296203613281</v>
           </cell>
           <cell r="AT33">
-            <v>126.23330688476563</v>
+            <v>126.23330688476562</v>
           </cell>
           <cell r="AU33">
             <v>6.25</v>
@@ -20945,7 +19587,7 @@
             <v>142.99998474121094</v>
           </cell>
           <cell r="J37">
-            <v>431.84994506835938</v>
+            <v>431.84994506835937</v>
           </cell>
           <cell r="K37">
             <v>4.91668701171875</v>
@@ -20987,7 +19629,7 @@
             <v>6</v>
           </cell>
           <cell r="Z37">
-            <v>158.86666870117188</v>
+            <v>158.86666870117187</v>
           </cell>
           <cell r="AA37">
             <v>387.23333740234375</v>
@@ -21133,7 +19775,7 @@
             <v>16</v>
           </cell>
           <cell r="AC38">
-            <v>149.33328247070313</v>
+            <v>149.33328247070312</v>
           </cell>
           <cell r="AD38">
             <v>0</v>
@@ -21225,7 +19867,7 @@
             <v>0</v>
           </cell>
           <cell r="L39">
-            <v>5.0333328247070313</v>
+            <v>5.0333328247070312</v>
           </cell>
           <cell r="M39">
             <v>0</v>
@@ -21362,7 +20004,7 @@
             <v>48.450004577636719</v>
           </cell>
           <cell r="L40">
-            <v>240.21670532226563</v>
+            <v>240.21670532226562</v>
           </cell>
           <cell r="M40">
             <v>23.75</v>
@@ -21452,7 +20094,7 @@
             <v>132.03326416015625</v>
           </cell>
           <cell r="AT40">
-            <v>354.18325805664063</v>
+            <v>354.18325805664062</v>
           </cell>
           <cell r="AU40">
             <v>26.166671752929688</v>
@@ -22227,7 +20869,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="ShtMain"/>
   <dimension ref="C4:P28"/>
   <sheetViews>
@@ -22327,7 +20969,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="ShtSettings"/>
   <dimension ref="B2:L28"/>
   <sheetViews>
@@ -22355,7 +20997,7 @@
         <v>5525013</v>
       </c>
       <c r="H2" t="s">
-        <v>3044</v>
+        <v>3039</v>
       </c>
       <c r="K2" s="5" t="s">
         <v>1</v>
@@ -22370,7 +21012,7 @@
         <v>2369842</v>
       </c>
       <c r="H3" t="s">
-        <v>3043</v>
+        <v>3038</v>
       </c>
       <c r="K3" t="s">
         <v>3</v>
@@ -22436,7 +21078,7 @@
         <v>3450623</v>
       </c>
       <c r="H7" t="s">
-        <v>3042</v>
+        <v>3037</v>
       </c>
       <c r="K7" t="s">
         <v>13</v>
@@ -22529,7 +21171,7 @@
         <v>52479</v>
       </c>
       <c r="H12" t="s">
-        <v>3041</v>
+        <v>3036</v>
       </c>
       <c r="K12" t="s">
         <v>28</v>
@@ -22648,7 +21290,7 @@
         <v>45</v>
       </c>
       <c r="J28" t="s">
-        <v>3019</v>
+        <v>3051</v>
       </c>
     </row>
   </sheetData>
@@ -22658,7 +21300,7 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="J25" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="J25" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -22667,8 +21309,33 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2052" r:id="rId5" name="CommandButton1">
+        <control shapeId="2049" r:id="rId5" name="BtnDBConnect">
           <controlPr defaultSize="0" autoLine="0" r:id="rId6">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>24</xdr:row>
+                <xdr:rowOff>180975</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>26</xdr:row>
+                <xdr:rowOff>76200</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2049" r:id="rId5" name="BtnDBConnect"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2052" r:id="rId7" name="CommandButton1">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId8">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
@@ -22687,32 +21354,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2052" r:id="rId5" name="CommandButton1"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2049" r:id="rId7" name="BtnDBConnect">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId8">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>24</xdr:row>
-                <xdr:rowOff>180975</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>26</xdr:row>
-                <xdr:rowOff>76200</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2049" r:id="rId7" name="BtnDBConnect"/>
+        <control shapeId="2052" r:id="rId7" name="CommandButton1"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -23094,7 +21736,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="ShtLists"/>
   <dimension ref="A1:V1115"/>
   <sheetViews>
@@ -23125,7 +21767,7 @@
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
-        <v>3045</v>
+        <v>3040</v>
       </c>
       <c r="B2" t="s">
         <v>2784</v>
@@ -23269,7 +21911,7 @@
         <v>66</v>
       </c>
       <c r="D11" t="s">
-        <v>3020</v>
+        <v>3015</v>
       </c>
       <c r="V11" s="22"/>
     </row>
@@ -24040,7 +22682,7 @@
         <v>134</v>
       </c>
       <c r="D63" t="s">
-        <v>3021</v>
+        <v>3016</v>
       </c>
       <c r="V63" s="22"/>
     </row>
@@ -25543,7 +24185,7 @@
     </row>
     <row r="165" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A165" s="20" t="s">
-        <v>3046</v>
+        <v>3041</v>
       </c>
       <c r="B165" t="s">
         <v>2220</v>
@@ -25747,7 +24389,7 @@
         <v>453</v>
       </c>
       <c r="D178" t="s">
-        <v>3022</v>
+        <v>3017</v>
       </c>
       <c r="V178" s="22"/>
     </row>
@@ -25909,7 +24551,7 @@
         <v>484</v>
       </c>
       <c r="D189" t="s">
-        <v>3023</v>
+        <v>3018</v>
       </c>
       <c r="V189" s="22"/>
     </row>
@@ -25966,7 +24608,7 @@
         <v>494</v>
       </c>
       <c r="D193" t="s">
-        <v>3024</v>
+        <v>3019</v>
       </c>
       <c r="V193" s="22"/>
     </row>
@@ -26791,7 +25433,7 @@
         <v>650</v>
       </c>
       <c r="D249" t="s">
-        <v>3025</v>
+        <v>3020</v>
       </c>
       <c r="V249" s="22"/>
     </row>
@@ -27358,7 +26000,7 @@
         <v>756</v>
       </c>
       <c r="D287" t="s">
-        <v>3026</v>
+        <v>3021</v>
       </c>
       <c r="V287" s="22"/>
     </row>
@@ -28057,7 +26699,7 @@
         <v>753</v>
       </c>
       <c r="B334" t="s">
-        <v>3047</v>
+        <v>3042</v>
       </c>
       <c r="C334" s="21" t="s">
         <v>883</v>
@@ -28285,7 +26927,7 @@
         <v>2371</v>
       </c>
       <c r="C349" s="21" t="s">
-        <v>3027</v>
+        <v>3022</v>
       </c>
       <c r="D349" t="s">
         <v>1983</v>
@@ -28318,7 +26960,7 @@
         <v>929</v>
       </c>
       <c r="D351" t="s">
-        <v>3028</v>
+        <v>3023</v>
       </c>
       <c r="V351" s="22"/>
     </row>
@@ -28429,7 +27071,7 @@
         <v>952</v>
       </c>
       <c r="D359" t="s">
-        <v>3029</v>
+        <v>3024</v>
       </c>
       <c r="V359" s="22"/>
     </row>
@@ -28534,7 +27176,7 @@
         <v>969</v>
       </c>
       <c r="D366" t="s">
-        <v>3030</v>
+        <v>3025</v>
       </c>
       <c r="V366" s="22"/>
     </row>
@@ -28654,7 +27296,7 @@
         <v>993</v>
       </c>
       <c r="D374" t="s">
-        <v>3031</v>
+        <v>3026</v>
       </c>
       <c r="V374" s="22"/>
     </row>
@@ -29059,7 +27701,7 @@
         <v>2433</v>
       </c>
       <c r="B402" t="s">
-        <v>3048</v>
+        <v>3043</v>
       </c>
       <c r="C402" s="21" t="s">
         <v>1073</v>
@@ -30121,7 +28763,7 @@
         <v>1268</v>
       </c>
       <c r="D474" t="s">
-        <v>3032</v>
+        <v>3027</v>
       </c>
       <c r="V474" s="22"/>
     </row>
@@ -30358,7 +29000,7 @@
         <v>1312</v>
       </c>
       <c r="D490" t="s">
-        <v>3033</v>
+        <v>3028</v>
       </c>
       <c r="V490" s="22"/>
     </row>
@@ -31426,7 +30068,7 @@
         <v>1506</v>
       </c>
       <c r="D563" t="s">
-        <v>3034</v>
+        <v>3029</v>
       </c>
       <c r="V563" s="22"/>
     </row>
@@ -32980,10 +31622,10 @@
         <v>2734</v>
       </c>
       <c r="C668" s="21" t="s">
-        <v>3035</v>
+        <v>3030</v>
       </c>
       <c r="D668" t="s">
-        <v>3036</v>
+        <v>3031</v>
       </c>
       <c r="V668" s="22"/>
     </row>
@@ -32995,10 +31637,10 @@
         <v>2734</v>
       </c>
       <c r="C669" s="21" t="s">
-        <v>3037</v>
+        <v>3032</v>
       </c>
       <c r="D669" t="s">
-        <v>3038</v>
+        <v>3033</v>
       </c>
       <c r="V669" s="22"/>
     </row>
@@ -33292,7 +31934,7 @@
         <v>1843</v>
       </c>
       <c r="D689" t="s">
-        <v>3039</v>
+        <v>3034</v>
       </c>
       <c r="V689" s="22"/>
     </row>
@@ -33319,7 +31961,7 @@
         <v>2758</v>
       </c>
       <c r="C691" s="21" t="s">
-        <v>3054</v>
+        <v>3049</v>
       </c>
       <c r="D691" t="s">
         <v>1888</v>
@@ -33334,10 +31976,10 @@
         <v>2759</v>
       </c>
       <c r="C692" s="21" t="s">
-        <v>3040</v>
+        <v>3035</v>
       </c>
       <c r="D692" t="s">
-        <v>3055</v>
+        <v>3050</v>
       </c>
       <c r="V692" s="22"/>
     </row>
@@ -33517,25 +32159,25 @@
     </row>
     <row r="713" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A713" s="20" t="s">
-        <v>3049</v>
+        <v>3044</v>
       </c>
       <c r="B713" t="s">
-        <v>3050</v>
+        <v>3045</v>
       </c>
       <c r="V713" s="22"/>
     </row>
     <row r="714" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A714" s="20" t="s">
-        <v>3051</v>
+        <v>3046</v>
       </c>
       <c r="B714" t="s">
-        <v>3050</v>
+        <v>3045</v>
       </c>
       <c r="V714" s="22"/>
     </row>
     <row r="715" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A715" s="20" t="s">
-        <v>3052</v>
+        <v>3047</v>
       </c>
       <c r="B715" t="s">
         <v>2918</v>
@@ -34543,7 +33185,7 @@
     </row>
     <row r="828" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A828" s="20" t="s">
-        <v>3053</v>
+        <v>3048</v>
       </c>
       <c r="B828" t="s">
         <v>2918</v>
@@ -36123,14 +34765,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="ShtOrderList">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="B1:L39"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="26.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -36168,26 +34810,26 @@
         <v>1878</v>
       </c>
       <c r="C3" s="44">
-        <v>1645</v>
+        <v>4277</v>
       </c>
       <c r="D3" s="47" t="s">
         <v>3013</v>
       </c>
       <c r="E3" s="49">
-        <v>43045</v>
+        <v>43377</v>
       </c>
       <c r="F3" s="44"/>
       <c r="G3" s="47" t="s">
         <v>1891</v>
       </c>
       <c r="H3" s="44" t="s">
-        <v>1525</v>
+        <v>1166</v>
       </c>
       <c r="I3" s="45" t="s">
         <v>1879</v>
       </c>
       <c r="J3" s="48" t="s">
-        <v>3016</v>
+        <v>3052</v>
       </c>
       <c r="K3" s="48"/>
     </row>
@@ -36223,7 +34865,7 @@
     </row>
     <row r="6" spans="2:12" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="30" t="s">
-        <v>1895</v>
+        <v>3060</v>
       </c>
       <c r="C6" s="42"/>
       <c r="D6" s="42"/>
@@ -36231,70 +34873,106 @@
       <c r="F6" s="32">
         <v>1</v>
       </c>
-      <c r="G6" s="32" t="s">
-        <v>3017</v>
-      </c>
+      <c r="G6" s="32"/>
       <c r="H6" s="32"/>
-      <c r="I6" s="33"/>
+      <c r="I6" s="33" t="s">
+        <v>3061</v>
+      </c>
       <c r="J6" s="33" t="s">
-        <v>3018</v>
-      </c>
-      <c r="K6" s="33" t="s">
-        <v>3015</v>
-      </c>
+        <v>3052</v>
+      </c>
+      <c r="K6" s="33"/>
       <c r="L6" s="34" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="2:12" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="35"/>
+      <c r="B7" s="35" t="s">
+        <v>3056</v>
+      </c>
       <c r="C7" s="43"/>
       <c r="D7" s="43"/>
       <c r="E7" s="36"/>
-      <c r="F7" s="37"/>
-      <c r="G7" s="37"/>
+      <c r="F7" s="37">
+        <v>12</v>
+      </c>
+      <c r="G7" s="37" t="s">
+        <v>3057</v>
+      </c>
       <c r="H7" s="37"/>
-      <c r="I7" s="38"/>
-      <c r="J7" s="38"/>
+      <c r="I7" s="38" t="s">
+        <v>3058</v>
+      </c>
+      <c r="J7" s="38" t="s">
+        <v>3059</v>
+      </c>
       <c r="K7" s="38"/>
       <c r="L7" s="39"/>
     </row>
     <row r="8" spans="2:12" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="35"/>
+      <c r="B8" s="35" t="s">
+        <v>3062</v>
+      </c>
       <c r="C8" s="43"/>
       <c r="D8" s="43"/>
       <c r="E8" s="36"/>
-      <c r="F8" s="37"/>
-      <c r="G8" s="37"/>
+      <c r="F8" s="37">
+        <v>1</v>
+      </c>
+      <c r="G8" s="37" t="s">
+        <v>3063</v>
+      </c>
       <c r="H8" s="37"/>
-      <c r="I8" s="38"/>
-      <c r="J8" s="38"/>
+      <c r="I8" s="38" t="s">
+        <v>3064</v>
+      </c>
+      <c r="J8" s="38" t="s">
+        <v>3059</v>
+      </c>
       <c r="K8" s="38"/>
       <c r="L8" s="39"/>
     </row>
     <row r="9" spans="2:12" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="35"/>
+      <c r="B9" s="35" t="s">
+        <v>3065</v>
+      </c>
       <c r="C9" s="43"/>
       <c r="D9" s="43"/>
       <c r="E9" s="36"/>
-      <c r="F9" s="37"/>
-      <c r="G9" s="37"/>
+      <c r="F9" s="37">
+        <v>2</v>
+      </c>
+      <c r="G9" s="37" t="s">
+        <v>3066</v>
+      </c>
       <c r="H9" s="37"/>
-      <c r="I9" s="38"/>
-      <c r="J9" s="38"/>
+      <c r="I9" s="38" t="s">
+        <v>3064</v>
+      </c>
+      <c r="J9" s="38" t="s">
+        <v>3059</v>
+      </c>
       <c r="K9" s="38"/>
       <c r="L9" s="39"/>
     </row>
     <row r="10" spans="2:12" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="35"/>
+      <c r="B10" s="35" t="s">
+        <v>3053</v>
+      </c>
       <c r="C10" s="43"/>
       <c r="D10" s="43"/>
       <c r="E10" s="36"/>
-      <c r="F10" s="37"/>
+      <c r="F10" s="37">
+        <v>2</v>
+      </c>
       <c r="G10" s="37"/>
       <c r="H10" s="37"/>
-      <c r="I10" s="38"/>
-      <c r="J10" s="38"/>
+      <c r="I10" s="38" t="s">
+        <v>3054</v>
+      </c>
+      <c r="J10" s="38" t="s">
+        <v>3055</v>
+      </c>
       <c r="K10" s="38"/>
       <c r="L10" s="39"/>
     </row>
@@ -36676,7 +35354,7 @@
       <c r="L39" s="39"/>
     </row>
   </sheetData>
-  <sortState ref="B6:J39">
+  <sortState ref="B6:K39">
     <sortCondition ref="I6"/>
   </sortState>
   <mergeCells count="2">
@@ -37307,7 +35985,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="5152" r:id="rId24" name="$H$15">
+            <control shapeId="5152" r:id="rId24" name="Check Box 32">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -37329,7 +36007,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="5153" r:id="rId25" name="$H$16">
+            <control shapeId="5153" r:id="rId25" name="Check Box 33">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -37351,7 +36029,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="5154" r:id="rId26" name="$H$17">
+            <control shapeId="5154" r:id="rId26" name="Check Box 34">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -37373,7 +36051,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="5155" r:id="rId27" name="$H$18">
+            <control shapeId="5155" r:id="rId27" name="Check Box 35">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -37395,7 +36073,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="5156" r:id="rId28" name="$H$19">
+            <control shapeId="5156" r:id="rId28" name="Check Box 36">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -37417,7 +36095,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="5157" r:id="rId29" name="$H$20">
+            <control shapeId="5157" r:id="rId29" name="Check Box 37">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -37439,7 +36117,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="5158" r:id="rId30" name="$H$21">
+            <control shapeId="5158" r:id="rId30" name="Check Box 38">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -37461,7 +36139,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="5159" r:id="rId31" name="$H$22">
+            <control shapeId="5159" r:id="rId31" name="Check Box 39">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -37483,7 +36161,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="5160" r:id="rId32" name="$H$23">
+            <control shapeId="5160" r:id="rId32" name="Check Box 40">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -37505,7 +36183,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="5161" r:id="rId33" name="$H$24">
+            <control shapeId="5161" r:id="rId33" name="Check Box 41">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -37527,7 +36205,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="5162" r:id="rId34" name="$H$25">
+            <control shapeId="5162" r:id="rId34" name="Check Box 42">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>

</xml_diff>